<commit_message>
almost done!! need to check work
</commit_message>
<xml_diff>
--- a/Food_SR_Organization.xlsx
+++ b/Food_SR_Organization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="4440" windowWidth="28660" windowHeight="14760" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-40" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Food Need" sheetId="3" r:id="rId1"/>
@@ -178,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="299">
   <si>
     <t>ALL LOCAL</t>
   </si>
@@ -1020,9 +1020,6 @@
     <t>livestock</t>
   </si>
   <si>
-    <t>Match Crops to Commodities</t>
-  </si>
-  <si>
     <t>Need</t>
   </si>
   <si>
@@ -1054,6 +1051,30 @@
   </si>
   <si>
     <t>Peas</t>
+  </si>
+  <si>
+    <t>Done! But no difference between</t>
+  </si>
+  <si>
+    <t>Likeley an error somewhere</t>
+  </si>
+  <si>
+    <t>Imports and No Imports</t>
+  </si>
+  <si>
+    <t>TO DO:</t>
+  </si>
+  <si>
+    <t>1. Check SWBC production results</t>
+  </si>
+  <si>
+    <t>2. Organize Diet and Seasonality Constraint</t>
+  </si>
+  <si>
+    <t>3. Calculate Food Need</t>
+  </si>
+  <si>
+    <t>4. Calculate Error</t>
   </si>
 </sst>
 </file>
@@ -1119,7 +1140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1231,6 +1252,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1548,7 +1575,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1597,23 +1624,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -1635,6 +1650,17 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="179">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2146,8 +2172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A115"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5793,8 +5819,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1"/>
+    <sheetView topLeftCell="K107" workbookViewId="0">
+      <selection activeCell="M114" sqref="M114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5837,10 +5863,10 @@
         <v>108</v>
       </c>
       <c r="R1" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="T1" s="29" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="V1" s="29">
         <v>0</v>
@@ -5867,13 +5893,13 @@
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
       <c r="K2" s="37"/>
-      <c r="O2" s="60"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="52" t="s">
+      <c r="O2" s="56"/>
+      <c r="P2" s="47"/>
+      <c r="Q2" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="S2" s="49"/>
-      <c r="U2" s="49"/>
+      <c r="S2" s="45"/>
+      <c r="U2" s="45"/>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="29" t="s">
@@ -5906,13 +5932,13 @@
       <c r="K3" s="34" t="s">
         <v>64</v>
       </c>
-      <c r="O3" s="60"/>
-      <c r="P3" s="51"/>
-      <c r="Q3" s="52" t="s">
+      <c r="O3" s="56"/>
+      <c r="P3" s="47"/>
+      <c r="Q3" s="48" t="s">
         <v>115</v>
       </c>
-      <c r="S3" s="49"/>
-      <c r="U3" s="49"/>
+      <c r="S3" s="45"/>
+      <c r="U3" s="45"/>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="29" t="s">
@@ -5935,13 +5961,13 @@
       <c r="I4" s="40"/>
       <c r="J4" s="40"/>
       <c r="K4" s="41"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="51"/>
-      <c r="Q4" s="52" t="s">
+      <c r="O4" s="56"/>
+      <c r="P4" s="47"/>
+      <c r="Q4" s="48" t="s">
         <v>117</v>
       </c>
-      <c r="S4" s="49"/>
-      <c r="U4" s="49"/>
+      <c r="S4" s="45"/>
+      <c r="U4" s="45"/>
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="29" t="s">
@@ -5959,19 +5985,19 @@
       <c r="E5">
         <v>875.89090909090896</v>
       </c>
-      <c r="O5" s="60"/>
-      <c r="P5" s="51"/>
-      <c r="Q5" s="52" t="s">
+      <c r="O5" s="56"/>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="48" t="s">
         <v>118</v>
       </c>
       <c r="R5" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="S5" s="66"/>
+      <c r="S5" s="62"/>
       <c r="T5" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="U5" s="66"/>
+      <c r="U5" s="62"/>
       <c r="V5" t="s">
         <v>68</v>
       </c>
@@ -5992,19 +6018,19 @@
       <c r="E6">
         <v>2205.4574468085102</v>
       </c>
-      <c r="O6" s="60"/>
-      <c r="P6" s="51"/>
-      <c r="Q6" s="52" t="s">
+      <c r="O6" s="56"/>
+      <c r="P6" s="47"/>
+      <c r="Q6" s="48" t="s">
         <v>120</v>
       </c>
       <c r="R6" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="S6" s="66"/>
+      <c r="S6" s="62"/>
       <c r="T6" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="U6" s="66"/>
+      <c r="U6" s="62"/>
       <c r="V6" t="s">
         <v>68</v>
       </c>
@@ -6025,21 +6051,21 @@
       <c r="E7">
         <v>755.91131812060496</v>
       </c>
-      <c r="O7" s="60"/>
-      <c r="P7" s="52" t="s">
+      <c r="O7" s="56"/>
+      <c r="P7" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="Q7" s="52" t="s">
+      <c r="Q7" s="48" t="s">
         <v>122</v>
       </c>
       <c r="R7" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="S7" s="66"/>
+      <c r="S7" s="62"/>
       <c r="T7" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="U7" s="66"/>
+      <c r="U7" s="62"/>
       <c r="V7" t="s">
         <v>68</v>
       </c>
@@ -6057,22 +6083,22 @@
       <c r="D8">
         <v>1</v>
       </c>
-      <c r="E8" s="62">
+      <c r="E8" s="58">
         <v>2.65384907534246</v>
       </c>
-      <c r="O8" s="60"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="52" t="s">
+      <c r="O8" s="56"/>
+      <c r="P8" s="47"/>
+      <c r="Q8" s="48" t="s">
         <v>124</v>
       </c>
       <c r="R8" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="S8" s="66"/>
+      <c r="S8" s="62"/>
       <c r="T8" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="U8" s="66"/>
+      <c r="U8" s="62"/>
       <c r="V8" t="s">
         <v>68</v>
       </c>
@@ -6093,19 +6119,19 @@
       <c r="E9">
         <v>19306.6766385589</v>
       </c>
-      <c r="O9" s="60"/>
-      <c r="P9" s="53"/>
-      <c r="Q9" s="54" t="s">
+      <c r="O9" s="56"/>
+      <c r="P9" s="49"/>
+      <c r="Q9" s="50" t="s">
         <v>125</v>
       </c>
       <c r="R9" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="S9" s="66"/>
+      <c r="S9" s="62"/>
       <c r="T9" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="U9" s="66"/>
+      <c r="U9" s="62"/>
       <c r="V9" t="s">
         <v>69</v>
       </c>
@@ -6126,21 +6152,21 @@
       <c r="E10">
         <v>67.958693255813898</v>
       </c>
-      <c r="O10" s="60"/>
-      <c r="P10" s="54" t="s">
+      <c r="O10" s="56"/>
+      <c r="P10" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="Q10" s="54" t="s">
+      <c r="Q10" s="50" t="s">
         <v>127</v>
       </c>
       <c r="R10" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="S10" s="66"/>
+      <c r="S10" s="62"/>
       <c r="T10" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="U10" s="66"/>
+      <c r="U10" s="62"/>
       <c r="V10" t="s">
         <v>69</v>
       </c>
@@ -6161,19 +6187,19 @@
       <c r="E11">
         <v>12705.9235555553</v>
       </c>
-      <c r="O11" s="60"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="52" t="s">
+      <c r="O11" s="56"/>
+      <c r="P11" s="47"/>
+      <c r="Q11" s="48" t="s">
         <v>129</v>
       </c>
       <c r="R11" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="S11" s="66"/>
+      <c r="S11" s="62"/>
       <c r="T11" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="U11" s="66"/>
+      <c r="U11" s="62"/>
       <c r="V11" t="s">
         <v>79</v>
       </c>
@@ -6194,21 +6220,21 @@
       <c r="E12">
         <v>221.37858600800499</v>
       </c>
-      <c r="O12" s="60"/>
-      <c r="P12" s="52" t="s">
+      <c r="O12" s="56"/>
+      <c r="P12" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="Q12" s="52" t="s">
+      <c r="Q12" s="48" t="s">
         <v>131</v>
       </c>
       <c r="R12" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="S12" s="66"/>
+      <c r="S12" s="62"/>
       <c r="T12" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="U12" s="66"/>
+      <c r="U12" s="62"/>
       <c r="V12" t="s">
         <v>79</v>
       </c>
@@ -6249,7 +6275,7 @@
       <c r="E14" s="13">
         <v>234.88788304347801</v>
       </c>
-      <c r="Q14" s="59" t="s">
+      <c r="Q14" s="55" t="s">
         <v>134</v>
       </c>
     </row>
@@ -6289,17 +6315,17 @@
       <c r="E16">
         <v>81.618866521739093</v>
       </c>
-      <c r="Q16" s="59" t="s">
+      <c r="Q16" s="55" t="s">
         <v>139</v>
       </c>
       <c r="R16" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="S16" s="66"/>
+      <c r="S16" s="62"/>
       <c r="T16" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="U16" s="66"/>
+      <c r="U16" s="62"/>
       <c r="V16" t="s">
         <v>80</v>
       </c>
@@ -6320,17 +6346,17 @@
       <c r="E17">
         <v>3475.59762118649</v>
       </c>
-      <c r="Q17" s="59" t="s">
+      <c r="Q17" s="55" t="s">
         <v>140</v>
       </c>
       <c r="R17" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="S17" s="66"/>
+      <c r="S17" s="62"/>
       <c r="T17" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="U17" s="66"/>
+      <c r="U17" s="62"/>
       <c r="V17" t="s">
         <v>80</v>
       </c>
@@ -6351,17 +6377,17 @@
       <c r="E18">
         <v>404.5597952</v>
       </c>
-      <c r="Q18" s="59" t="s">
+      <c r="Q18" s="55" t="s">
         <v>141</v>
       </c>
       <c r="R18" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="S18" s="66"/>
+      <c r="S18" s="62"/>
       <c r="T18" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="U18" s="66"/>
+      <c r="U18" s="62"/>
       <c r="V18" t="s">
         <v>80</v>
       </c>
@@ -6382,7 +6408,13 @@
       <c r="E19">
         <v>185.76237623762299</v>
       </c>
-      <c r="Q19" s="58" t="s">
+      <c r="M19" s="54" t="s">
+        <v>46</v>
+      </c>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="54" t="s">
         <v>142</v>
       </c>
     </row>
@@ -6402,19 +6434,19 @@
       <c r="E20">
         <v>5171</v>
       </c>
-      <c r="O20" s="60"/>
-      <c r="P20" s="51"/>
-      <c r="Q20" s="52" t="s">
+      <c r="O20" s="56"/>
+      <c r="P20" s="47"/>
+      <c r="Q20" s="48" t="s">
         <v>144</v>
       </c>
       <c r="R20" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="S20" s="66"/>
+      <c r="S20" s="62"/>
       <c r="T20" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="U20" s="66"/>
+      <c r="U20" s="62"/>
       <c r="V20" t="s">
         <v>81</v>
       </c>
@@ -6435,21 +6467,21 @@
       <c r="E21">
         <v>3377.0704225352101</v>
       </c>
-      <c r="O21" s="60"/>
-      <c r="P21" s="52" t="s">
+      <c r="O21" s="56"/>
+      <c r="P21" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="Q21" s="52" t="s">
+      <c r="Q21" s="48" t="s">
         <v>145</v>
       </c>
       <c r="R21" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="S21" s="66"/>
+      <c r="S21" s="62"/>
       <c r="T21" s="29" t="s">
         <v>81</v>
       </c>
-      <c r="U21" s="66"/>
+      <c r="U21" s="62"/>
       <c r="V21" t="s">
         <v>81</v>
       </c>
@@ -6470,19 +6502,19 @@
       <c r="E22">
         <v>1688.0866425992699</v>
       </c>
-      <c r="O22" s="60"/>
-      <c r="P22" s="53"/>
-      <c r="Q22" s="54" t="s">
+      <c r="O22" s="56"/>
+      <c r="P22" s="49"/>
+      <c r="Q22" s="50" t="s">
         <v>146</v>
       </c>
       <c r="R22" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="S22" s="66"/>
+      <c r="S22" s="62"/>
       <c r="T22" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="U22" s="66"/>
+      <c r="U22" s="62"/>
       <c r="V22" t="s">
         <v>70</v>
       </c>
@@ -6503,21 +6535,21 @@
       <c r="E23">
         <v>3697.5744680850999</v>
       </c>
-      <c r="O23" s="60"/>
-      <c r="P23" s="54" t="s">
+      <c r="O23" s="56"/>
+      <c r="P23" s="50" t="s">
         <v>70</v>
       </c>
-      <c r="Q23" s="54" t="s">
+      <c r="Q23" s="50" t="s">
         <v>147</v>
       </c>
       <c r="R23" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="S23" s="66"/>
+      <c r="S23" s="62"/>
       <c r="T23" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="U23" s="66"/>
+      <c r="U23" s="62"/>
       <c r="V23" t="s">
         <v>70</v>
       </c>
@@ -6538,19 +6570,19 @@
       <c r="E24">
         <v>4929.9014492753604</v>
       </c>
-      <c r="O24" s="60"/>
-      <c r="P24" s="53"/>
-      <c r="Q24" s="54" t="s">
+      <c r="O24" s="56"/>
+      <c r="P24" s="49"/>
+      <c r="Q24" s="50" t="s">
         <v>148</v>
       </c>
       <c r="R24" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="S24" s="66"/>
+      <c r="S24" s="62"/>
       <c r="T24" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="U24" s="66"/>
+      <c r="U24" s="62"/>
       <c r="V24" t="s">
         <v>70</v>
       </c>
@@ -6571,18 +6603,18 @@
       <c r="E25">
         <v>622.95652173913004</v>
       </c>
-      <c r="P25" s="51"/>
-      <c r="Q25" s="52" t="s">
+      <c r="P25" s="47"/>
+      <c r="Q25" s="48" t="s">
         <v>149</v>
       </c>
       <c r="R25" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="S25" s="66"/>
+      <c r="S25" s="62"/>
       <c r="T25" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="U25" s="66"/>
+      <c r="U25" s="62"/>
       <c r="V25" t="s">
         <v>82</v>
       </c>
@@ -6603,21 +6635,21 @@
       <c r="E26">
         <v>80</v>
       </c>
-      <c r="O26" s="60"/>
-      <c r="P26" s="52" t="s">
+      <c r="O26" s="56"/>
+      <c r="P26" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="Q26" s="52" t="s">
+      <c r="Q26" s="48" t="s">
         <v>150</v>
       </c>
       <c r="R26" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="S26" s="66"/>
+      <c r="S26" s="62"/>
       <c r="T26" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="U26" s="66"/>
+      <c r="U26" s="62"/>
       <c r="V26" t="s">
         <v>82</v>
       </c>
@@ -6638,21 +6670,21 @@
       <c r="E27">
         <v>10036.285714285699</v>
       </c>
-      <c r="O27" s="60"/>
-      <c r="P27" s="55" t="s">
+      <c r="O27" s="56"/>
+      <c r="P27" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="Q27" s="55" t="s">
+      <c r="Q27" s="51" t="s">
         <v>152</v>
       </c>
       <c r="R27" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="S27" s="66"/>
+      <c r="S27" s="62"/>
       <c r="T27" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="U27" s="66"/>
+      <c r="U27" s="62"/>
       <c r="V27" t="s">
         <v>83</v>
       </c>
@@ -6673,19 +6705,19 @@
       <c r="E28">
         <v>1793.5737704917999</v>
       </c>
-      <c r="O28" s="60"/>
-      <c r="P28" s="56"/>
-      <c r="Q28" s="55" t="s">
+      <c r="O28" s="56"/>
+      <c r="P28" s="52"/>
+      <c r="Q28" s="51" t="s">
         <v>154</v>
       </c>
       <c r="R28" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="S28" s="66"/>
+      <c r="S28" s="62"/>
       <c r="T28" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="U28" s="66"/>
+      <c r="U28" s="62"/>
       <c r="V28" t="s">
         <v>83</v>
       </c>
@@ -6706,7 +6738,7 @@
       <c r="E29">
         <v>5761.7028112449798</v>
       </c>
-      <c r="Q29" s="58" t="s">
+      <c r="Q29" s="54" t="s">
         <v>155</v>
       </c>
     </row>
@@ -6726,7 +6758,7 @@
       <c r="E30">
         <v>1626.3364485981299</v>
       </c>
-      <c r="Q30" s="58" t="s">
+      <c r="Q30" s="54" t="s">
         <v>158</v>
       </c>
     </row>
@@ -6806,21 +6838,21 @@
       <c r="E34">
         <v>5912.79233226837</v>
       </c>
-      <c r="O34" s="60"/>
-      <c r="P34" s="55" t="s">
+      <c r="O34" s="56"/>
+      <c r="P34" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="Q34" s="55" t="s">
+      <c r="Q34" s="51" t="s">
         <v>165</v>
       </c>
       <c r="R34" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="S34" s="66"/>
+      <c r="S34" s="62"/>
       <c r="T34" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="U34" s="66"/>
+      <c r="U34" s="62"/>
       <c r="V34" t="s">
         <v>85</v>
       </c>
@@ -6838,24 +6870,24 @@
       <c r="D35">
         <v>135</v>
       </c>
-      <c r="E35" s="61">
+      <c r="E35" s="57">
         <v>2568.4322033898302</v>
       </c>
-      <c r="O35" s="60"/>
-      <c r="P35" s="52" t="s">
+      <c r="O35" s="56"/>
+      <c r="P35" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="Q35" s="52" t="s">
+      <c r="Q35" s="48" t="s">
         <v>167</v>
       </c>
       <c r="R35" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="S35" s="66"/>
+      <c r="S35" s="62"/>
       <c r="T35" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="U35" s="66"/>
+      <c r="U35" s="62"/>
       <c r="V35" t="s">
         <v>86</v>
       </c>
@@ -6876,7 +6908,7 @@
       <c r="E36">
         <v>2907.5887850467202</v>
       </c>
-      <c r="Q36" s="58" t="s">
+      <c r="Q36" s="54" t="s">
         <v>169</v>
       </c>
     </row>
@@ -6896,23 +6928,23 @@
       <c r="E37">
         <v>733.86666666666599</v>
       </c>
-      <c r="M37" s="69" t="s">
-        <v>285</v>
-      </c>
-      <c r="O37" s="60"/>
-      <c r="P37" s="52" t="s">
+      <c r="M37" s="65" t="s">
+        <v>284</v>
+      </c>
+      <c r="O37" s="56"/>
+      <c r="P37" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="Q37" s="52" t="s">
+      <c r="Q37" s="48" t="s">
         <v>171</v>
       </c>
-      <c r="S37" s="49"/>
+      <c r="S37" s="45"/>
       <c r="T37" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="U37" s="66"/>
+        <v>284</v>
+      </c>
+      <c r="U37" s="62"/>
       <c r="V37" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="38" spans="1:22">
@@ -6931,18 +6963,18 @@
       <c r="E38">
         <v>4316805699832.7402</v>
       </c>
-      <c r="O38" s="60"/>
-      <c r="P38" s="51"/>
-      <c r="Q38" s="52" t="s">
+      <c r="O38" s="56"/>
+      <c r="P38" s="47"/>
+      <c r="Q38" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="S38" s="49"/>
+      <c r="S38" s="45"/>
       <c r="T38" s="29" t="s">
-        <v>285</v>
-      </c>
-      <c r="U38" s="66"/>
+        <v>284</v>
+      </c>
+      <c r="U38" s="62"/>
       <c r="V38" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="39" spans="1:22">
@@ -6978,10 +7010,10 @@
       <c r="D40">
         <v>8781620000</v>
       </c>
-      <c r="E40" s="61">
+      <c r="E40" s="57">
         <v>5133342539307.2002</v>
       </c>
-      <c r="Q40" s="58" t="s">
+      <c r="Q40" s="54" t="s">
         <v>176</v>
       </c>
     </row>
@@ -7001,7 +7033,7 @@
       <c r="E41">
         <v>5043143942925.4697</v>
       </c>
-      <c r="Q41" s="58" t="s">
+      <c r="Q41" s="54" t="s">
         <v>177</v>
       </c>
     </row>
@@ -7021,191 +7053,197 @@
       <c r="E42">
         <v>2231691215348.4902</v>
       </c>
-      <c r="O42" s="60"/>
-      <c r="P42" s="51"/>
-      <c r="Q42" s="52" t="s">
+      <c r="O42" s="56"/>
+      <c r="P42" s="47"/>
+      <c r="Q42" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="S42" s="49"/>
+      <c r="S42" s="45"/>
       <c r="T42" s="29" t="s">
-        <v>286</v>
-      </c>
-      <c r="U42" s="66"/>
+        <v>285</v>
+      </c>
+      <c r="U42" s="62"/>
       <c r="V42" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="43" spans="1:22">
-      <c r="P43" s="51"/>
-      <c r="Q43" s="52" t="s">
+      <c r="P43" s="47"/>
+      <c r="Q43" s="48" t="s">
         <v>179</v>
       </c>
-      <c r="S43" s="68"/>
+      <c r="S43" s="64"/>
       <c r="T43" s="29" t="s">
-        <v>286</v>
-      </c>
-      <c r="U43" s="67"/>
+        <v>285</v>
+      </c>
+      <c r="U43" s="62"/>
       <c r="V43" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="44" spans="1:22">
-      <c r="M44" s="69" t="s">
-        <v>286</v>
-      </c>
-      <c r="O44" s="60"/>
-      <c r="P44" s="52" t="s">
+      <c r="M44" s="65" t="s">
+        <v>285</v>
+      </c>
+      <c r="O44" s="56"/>
+      <c r="P44" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="Q44" s="52" t="s">
+      <c r="Q44" s="48" t="s">
         <v>181</v>
       </c>
-      <c r="S44" s="49"/>
+      <c r="S44" s="45"/>
       <c r="T44" s="29" t="s">
-        <v>286</v>
-      </c>
-      <c r="U44" s="66"/>
+        <v>285</v>
+      </c>
+      <c r="U44" s="62"/>
       <c r="V44" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="45" spans="1:22">
-      <c r="O45" s="60"/>
-      <c r="P45" s="51"/>
-      <c r="Q45" s="52" t="s">
+      <c r="O45" s="56"/>
+      <c r="P45" s="47"/>
+      <c r="Q45" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="S45" s="49"/>
+      <c r="S45" s="45"/>
       <c r="T45" s="29" t="s">
-        <v>286</v>
-      </c>
-      <c r="U45" s="66"/>
+        <v>285</v>
+      </c>
+      <c r="U45" s="62"/>
       <c r="V45" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="46" spans="1:22">
-      <c r="Q46" s="58" t="s">
+      <c r="Q46" s="54" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:22">
       <c r="D47" t="s">
+        <v>280</v>
+      </c>
+      <c r="E47" t="s">
         <v>281</v>
       </c>
-      <c r="E47" t="s">
+      <c r="F47" t="s">
         <v>282</v>
       </c>
-      <c r="F47" t="s">
-        <v>283</v>
-      </c>
-      <c r="O47" s="60"/>
-      <c r="P47" s="52" t="s">
+      <c r="O47" s="56"/>
+      <c r="P47" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="Q47" s="52" t="s">
+      <c r="Q47" s="48" t="s">
         <v>185</v>
       </c>
       <c r="R47" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="S47" s="66"/>
+      <c r="S47" s="62"/>
       <c r="T47" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="U47" s="66"/>
+      <c r="U47" s="62"/>
       <c r="V47" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:22">
-      <c r="D48" s="61">
+      <c r="D48" s="57">
         <v>1788.73395000286</v>
       </c>
-      <c r="E48" s="61">
+      <c r="E48" s="57">
         <f>SUM(E35,E40)</f>
         <v>5133342541875.6328</v>
       </c>
-      <c r="F48" s="61">
+      <c r="F48" s="57">
         <f>E48/D53</f>
         <v>90010483.617180794</v>
       </c>
-      <c r="G48" s="63">
+      <c r="G48" s="59">
         <v>1</v>
       </c>
-      <c r="N48" s="60"/>
-      <c r="O48" s="55" t="s">
+      <c r="N48" s="56"/>
+      <c r="O48" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="P48" s="55" t="s">
+      <c r="P48" s="51" t="s">
         <v>88</v>
       </c>
-      <c r="Q48" s="55" t="s">
+      <c r="Q48" s="51" t="s">
         <v>186</v>
       </c>
       <c r="R48" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="S48" s="66"/>
+      <c r="S48" s="62"/>
       <c r="T48" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="U48" s="66"/>
+      <c r="U48" s="62"/>
       <c r="V48" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="49" spans="4:22">
-      <c r="D49" s="61">
+      <c r="D49" s="57">
         <v>11562.729582981399</v>
       </c>
-      <c r="E49" s="61"/>
-      <c r="F49" s="61"/>
-      <c r="G49" s="61"/>
+      <c r="E49" s="57"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
       <c r="Q49" s="29" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="50" spans="4:22">
-      <c r="D50" s="61">
+      <c r="D50" s="57">
         <v>15112.2889690376</v>
       </c>
-      <c r="E50" s="61"/>
-      <c r="F50" s="61"/>
-      <c r="G50" s="61"/>
-      <c r="Q50" s="58" t="s">
+      <c r="E50" s="57"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+      <c r="M50" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="N50" s="69"/>
+      <c r="O50" s="69"/>
+      <c r="P50" s="69"/>
+      <c r="Q50" s="54" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="51" spans="4:22">
-      <c r="D51" s="61">
+      <c r="D51" s="57">
         <v>28566.743675601199</v>
       </c>
-      <c r="E51" s="61"/>
-      <c r="F51" s="61"/>
-      <c r="G51" s="61"/>
+      <c r="E51" s="57"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
       <c r="Q51" s="29" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="52" spans="4:22">
-      <c r="D52" s="61"/>
-      <c r="E52" s="61"/>
-      <c r="F52" s="61"/>
-      <c r="G52" s="61"/>
-      <c r="Q52" s="57" t="s">
+      <c r="D52" s="57"/>
+      <c r="E52" s="57"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+      <c r="Q52" s="53" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="53" spans="4:22">
-      <c r="D53" s="61">
+      <c r="D53" s="57">
         <f>SUM(D48:D51)</f>
         <v>57030.496177623063</v>
       </c>
-      <c r="E53" s="61"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="61"/>
-      <c r="Q53" s="57" t="s">
+      <c r="E53" s="57"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+      <c r="Q53" s="53" t="s">
         <v>193</v>
       </c>
     </row>
@@ -7215,36 +7253,36 @@
       </c>
     </row>
     <row r="55" spans="4:22">
-      <c r="P55" s="51"/>
-      <c r="Q55" s="52" t="s">
+      <c r="P55" s="47"/>
+      <c r="Q55" s="48" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="56" spans="4:22">
-      <c r="O56" s="60"/>
-      <c r="P56" s="52" t="s">
+      <c r="O56" s="56"/>
+      <c r="P56" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="Q56" s="52" t="s">
+      <c r="Q56" s="48" t="s">
         <v>196</v>
       </c>
       <c r="R56" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="S56" s="66"/>
+      <c r="S56" s="62"/>
       <c r="T56" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="U56" s="66"/>
+      <c r="U56" s="62"/>
       <c r="V56" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="57" spans="4:22">
-      <c r="D57" s="62">
+      <c r="D57" s="58">
         <v>49.687054166746101</v>
       </c>
-      <c r="E57" s="62">
+      <c r="E57" s="58">
         <v>2.65384907534246</v>
       </c>
       <c r="Q57" s="29" t="s">
@@ -7252,24 +7290,24 @@
       </c>
     </row>
     <row r="58" spans="4:22">
-      <c r="D58" s="62">
+      <c r="D58" s="58">
         <v>211.693502810045</v>
       </c>
-      <c r="O58" s="60"/>
-      <c r="P58" s="52" t="s">
+      <c r="O58" s="56"/>
+      <c r="P58" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="Q58" s="52" t="s">
+      <c r="Q58" s="48" t="s">
         <v>198</v>
       </c>
       <c r="R58" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="S58" s="66"/>
+      <c r="S58" s="62"/>
       <c r="T58" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="U58" s="66"/>
+      <c r="U58" s="62"/>
       <c r="V58" t="s">
         <v>89</v>
       </c>
@@ -7280,15 +7318,15 @@
       </c>
     </row>
     <row r="60" spans="4:22">
-      <c r="D60" s="62">
+      <c r="D60" s="58">
         <f xml:space="preserve"> SUM(D57+D58)</f>
         <v>261.38055697679113</v>
       </c>
-      <c r="F60" s="62">
+      <c r="F60" s="58">
         <f>(E57/D60)*100</f>
         <v>1.0153200016243382</v>
       </c>
-      <c r="G60" s="65">
+      <c r="G60" s="61">
         <v>1</v>
       </c>
       <c r="Q60" s="29" t="s">
@@ -7296,45 +7334,51 @@
       </c>
     </row>
     <row r="61" spans="4:22">
-      <c r="O61" s="60"/>
-      <c r="P61" s="51"/>
-      <c r="Q61" s="52" t="s">
+      <c r="O61" s="56"/>
+      <c r="P61" s="47"/>
+      <c r="Q61" s="48" t="s">
         <v>202</v>
       </c>
       <c r="R61" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="S61" s="66"/>
+      <c r="S61" s="62"/>
       <c r="T61" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="U61" s="66"/>
+      <c r="U61" s="62"/>
       <c r="V61" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="62" spans="4:22">
-      <c r="O62" s="60"/>
-      <c r="P62" s="52" t="s">
+      <c r="O62" s="56"/>
+      <c r="P62" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="Q62" s="52" t="s">
+      <c r="Q62" s="48" t="s">
         <v>204</v>
       </c>
       <c r="R62" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="S62" s="66"/>
+      <c r="S62" s="62"/>
       <c r="T62" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="U62" s="66"/>
+      <c r="U62" s="62"/>
       <c r="V62" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="63" spans="4:22">
-      <c r="Q63" s="58" t="s">
+      <c r="M63" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="N63" s="69"/>
+      <c r="O63" s="69"/>
+      <c r="P63" s="69"/>
+      <c r="Q63" s="54" t="s">
         <v>205</v>
       </c>
     </row>
@@ -7345,21 +7389,21 @@
       <c r="E64" s="13">
         <v>234.88788304347801</v>
       </c>
-      <c r="O64" s="60"/>
-      <c r="P64" s="55" t="s">
+      <c r="O64" s="56"/>
+      <c r="P64" s="51" t="s">
         <v>21</v>
       </c>
-      <c r="Q64" s="55" t="s">
+      <c r="Q64" s="51" t="s">
         <v>206</v>
       </c>
       <c r="R64" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="S64" s="66"/>
+      <c r="S64" s="62"/>
       <c r="T64" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="U64" s="66"/>
+      <c r="U64" s="62"/>
       <c r="V64" t="s">
         <v>21</v>
       </c>
@@ -7372,26 +7416,26 @@
         <f>(E64/D67) *100</f>
         <v>5.4623378078715961</v>
       </c>
-      <c r="G65" s="64">
+      <c r="G65" s="60">
         <v>0.05</v>
       </c>
-      <c r="M65" s="69" t="s">
-        <v>287</v>
-      </c>
-      <c r="O65" s="60"/>
-      <c r="P65" s="52" t="s">
+      <c r="M65" s="65" t="s">
+        <v>286</v>
+      </c>
+      <c r="O65" s="56"/>
+      <c r="P65" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="Q65" s="52" t="s">
+      <c r="Q65" s="48" t="s">
         <v>208</v>
       </c>
-      <c r="S65" s="49"/>
+      <c r="S65" s="45"/>
       <c r="T65" s="29" t="s">
-        <v>287</v>
-      </c>
-      <c r="U65" s="66"/>
+        <v>286</v>
+      </c>
+      <c r="U65" s="62"/>
       <c r="V65" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="66" spans="4:22">
@@ -7409,169 +7453,169 @@
       </c>
     </row>
     <row r="68" spans="4:22">
-      <c r="Q68" s="58" t="s">
+      <c r="Q68" s="54" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="69" spans="4:22">
-      <c r="Q69" s="58" t="s">
+      <c r="Q69" s="54" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="70" spans="4:22">
-      <c r="O70" s="60"/>
-      <c r="P70" s="51"/>
-      <c r="Q70" s="52" t="s">
+      <c r="O70" s="56"/>
+      <c r="P70" s="47"/>
+      <c r="Q70" s="48" t="s">
         <v>213</v>
       </c>
-      <c r="S70" s="49"/>
+      <c r="S70" s="45"/>
       <c r="T70" s="29" t="s">
-        <v>288</v>
-      </c>
-      <c r="U70" s="66"/>
+        <v>287</v>
+      </c>
+      <c r="U70" s="62"/>
       <c r="V70" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="71" spans="4:22">
-      <c r="M71" s="69" t="s">
-        <v>288</v>
-      </c>
-      <c r="O71" s="60"/>
-      <c r="P71" s="52" t="s">
+      <c r="M71" s="65" t="s">
+        <v>287</v>
+      </c>
+      <c r="O71" s="56"/>
+      <c r="P71" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="Q71" s="52" t="s">
+      <c r="Q71" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="S71" s="49"/>
+      <c r="S71" s="45"/>
       <c r="T71" s="29" t="s">
-        <v>288</v>
-      </c>
-      <c r="U71" s="66"/>
+        <v>287</v>
+      </c>
+      <c r="U71" s="62"/>
       <c r="V71" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="72" spans="4:22">
       <c r="Q72" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="S72" s="49"/>
-      <c r="U72" s="67"/>
+      <c r="S72" s="64"/>
+      <c r="U72" s="64"/>
     </row>
     <row r="73" spans="4:22">
-      <c r="O73" s="60"/>
-      <c r="P73" s="51"/>
-      <c r="Q73" s="52" t="s">
+      <c r="O73" s="56"/>
+      <c r="P73" s="47"/>
+      <c r="Q73" s="48" t="s">
         <v>216</v>
       </c>
       <c r="R73" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="S73" s="66"/>
+      <c r="S73" s="62"/>
       <c r="T73" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="U73" s="66"/>
+      <c r="U73" s="62"/>
       <c r="V73" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="74" spans="4:22">
-      <c r="O74" s="60"/>
-      <c r="P74" s="52" t="s">
+      <c r="O74" s="56"/>
+      <c r="P74" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="Q74" s="52" t="s">
+      <c r="Q74" s="48" t="s">
         <v>217</v>
       </c>
       <c r="R74" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="S74" s="66"/>
+      <c r="S74" s="62"/>
       <c r="T74" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="U74" s="66"/>
+      <c r="U74" s="62"/>
       <c r="V74" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="75" spans="4:22">
-      <c r="N75" s="60"/>
-      <c r="O75" s="56"/>
-      <c r="P75" s="56"/>
-      <c r="Q75" s="55" t="s">
+      <c r="N75" s="56"/>
+      <c r="O75" s="52"/>
+      <c r="P75" s="52"/>
+      <c r="Q75" s="51" t="s">
         <v>218</v>
       </c>
-      <c r="S75" s="49"/>
+      <c r="S75" s="45"/>
       <c r="T75" s="29" t="s">
-        <v>291</v>
-      </c>
-      <c r="U75" s="66"/>
+        <v>290</v>
+      </c>
+      <c r="U75" s="62"/>
       <c r="V75" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="76" spans="4:22">
-      <c r="M76" s="69" t="s">
-        <v>289</v>
-      </c>
-      <c r="N76" s="60"/>
-      <c r="O76" s="55" t="s">
+      <c r="M76" s="65" t="s">
+        <v>288</v>
+      </c>
+      <c r="N76" s="56"/>
+      <c r="O76" s="51" t="s">
         <v>80</v>
       </c>
-      <c r="P76" s="55" t="s">
+      <c r="P76" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="Q76" s="55" t="s">
+      <c r="Q76" s="51" t="s">
         <v>219</v>
       </c>
-      <c r="S76" s="49"/>
+      <c r="S76" s="45"/>
       <c r="T76" s="29" t="s">
-        <v>291</v>
-      </c>
-      <c r="U76" s="66"/>
+        <v>290</v>
+      </c>
+      <c r="U76" s="62"/>
       <c r="V76" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="77" spans="4:22">
-      <c r="N77" s="60"/>
-      <c r="O77" s="56"/>
-      <c r="P77" s="56"/>
-      <c r="Q77" s="55" t="s">
+      <c r="N77" s="56"/>
+      <c r="O77" s="52"/>
+      <c r="P77" s="52"/>
+      <c r="Q77" s="51" t="s">
         <v>220</v>
       </c>
-      <c r="S77" s="49"/>
+      <c r="S77" s="45"/>
       <c r="T77" s="29" t="s">
-        <v>291</v>
-      </c>
-      <c r="U77" s="66"/>
+        <v>290</v>
+      </c>
+      <c r="U77" s="62"/>
       <c r="V77" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="78" spans="4:22">
-      <c r="N78" s="60"/>
-      <c r="O78" s="52" t="s">
+      <c r="N78" s="56"/>
+      <c r="O78" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="P78" s="52" t="s">
+      <c r="P78" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="Q78" s="52" t="s">
+      <c r="Q78" s="48" t="s">
         <v>221</v>
       </c>
       <c r="R78" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="S78" s="66"/>
+      <c r="S78" s="62"/>
       <c r="T78" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="U78" s="66"/>
+      <c r="U78" s="62"/>
       <c r="V78" t="s">
         <v>96</v>
       </c>
@@ -7588,11 +7632,11 @@
       <c r="R80" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="S80" s="67"/>
+      <c r="S80" s="63"/>
       <c r="T80" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="U80" s="67"/>
+      <c r="U80" s="62"/>
       <c r="V80" t="s">
         <v>68</v>
       </c>
@@ -7604,198 +7648,204 @@
       <c r="R81" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="S81" s="67"/>
+      <c r="S81" s="63"/>
       <c r="T81" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="U81" s="67"/>
+      <c r="U81" s="62"/>
       <c r="V81" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="82" spans="13:22">
-      <c r="M82" s="69" t="s">
-        <v>290</v>
-      </c>
-      <c r="N82" s="60"/>
-      <c r="O82" s="55" t="s">
+      <c r="M82" s="65" t="s">
+        <v>289</v>
+      </c>
+      <c r="N82" s="56"/>
+      <c r="O82" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="P82" s="55" t="s">
+      <c r="P82" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="Q82" s="55" t="s">
+      <c r="Q82" s="51" t="s">
         <v>226</v>
       </c>
-      <c r="S82" s="49"/>
+      <c r="S82" s="45"/>
       <c r="T82" s="29" t="s">
-        <v>290</v>
-      </c>
-      <c r="U82" s="66"/>
+        <v>289</v>
+      </c>
+      <c r="U82" s="62"/>
       <c r="V82" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="83" spans="13:22">
-      <c r="Q83" s="58" t="s">
+      <c r="M83" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="N83" s="69"/>
+      <c r="O83" s="69"/>
+      <c r="P83" s="69"/>
+      <c r="Q83" s="54" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="84" spans="13:22">
-      <c r="O84" s="60"/>
-      <c r="P84" s="52" t="s">
+      <c r="O84" s="56"/>
+      <c r="P84" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="Q84" s="52" t="s">
+      <c r="Q84" s="48" t="s">
         <v>229</v>
       </c>
       <c r="R84" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="S84" s="66"/>
+      <c r="S84" s="62"/>
       <c r="T84" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="U84" s="66"/>
+      <c r="U84" s="62"/>
       <c r="V84" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="85" spans="13:22">
-      <c r="O85" s="60"/>
-      <c r="P85" s="56"/>
-      <c r="Q85" s="55" t="s">
+      <c r="O85" s="56"/>
+      <c r="P85" s="52"/>
+      <c r="Q85" s="51" t="s">
         <v>231</v>
       </c>
       <c r="R85" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="S85" s="66"/>
+      <c r="S85" s="62"/>
       <c r="T85" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="U85" s="66"/>
+      <c r="U85" s="62"/>
       <c r="V85" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="86" spans="13:22">
-      <c r="O86" s="60"/>
-      <c r="P86" s="56"/>
-      <c r="Q86" s="55" t="s">
+      <c r="O86" s="56"/>
+      <c r="P86" s="52"/>
+      <c r="Q86" s="51" t="s">
         <v>232</v>
       </c>
       <c r="R86" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="S86" s="66"/>
+      <c r="S86" s="62"/>
       <c r="T86" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="U86" s="66"/>
+      <c r="U86" s="62"/>
       <c r="V86" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="87" spans="13:22">
-      <c r="O87" s="60"/>
-      <c r="P87" s="55" t="s">
+      <c r="O87" s="56"/>
+      <c r="P87" s="51" t="s">
         <v>99</v>
       </c>
-      <c r="Q87" s="55" t="s">
+      <c r="Q87" s="51" t="s">
         <v>233</v>
       </c>
       <c r="R87" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="S87" s="66"/>
+      <c r="S87" s="62"/>
       <c r="T87" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="U87" s="66"/>
+      <c r="U87" s="62"/>
       <c r="V87" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="88" spans="13:22">
-      <c r="Q88" s="58" t="s">
+      <c r="Q88" s="54" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="89" spans="13:22">
-      <c r="Q89" s="58" t="s">
+      <c r="Q89" s="54" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="90" spans="13:22">
-      <c r="Q90" s="58" t="s">
+      <c r="Q90" s="54" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="91" spans="13:22">
-      <c r="Q91" s="57" t="s">
+      <c r="Q91" s="53" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="92" spans="13:22">
-      <c r="N92" s="60"/>
-      <c r="O92" s="55" t="s">
+      <c r="N92" s="56"/>
+      <c r="O92" s="51" t="s">
         <v>94</v>
       </c>
-      <c r="P92" s="55" t="s">
+      <c r="P92" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="Q92" s="55" t="s">
+      <c r="Q92" s="51" t="s">
         <v>239</v>
       </c>
       <c r="R92" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="S92" s="66"/>
+      <c r="S92" s="62"/>
       <c r="T92" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="U92" s="66"/>
+      <c r="U92" s="62"/>
       <c r="V92" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="93" spans="13:22">
-      <c r="O93" s="60"/>
-      <c r="P93" s="52" t="s">
+      <c r="O93" s="56"/>
+      <c r="P93" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="Q93" s="52" t="s">
+      <c r="Q93" s="48" t="s">
         <v>240</v>
       </c>
       <c r="R93" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="S93" s="66"/>
+      <c r="S93" s="62"/>
       <c r="T93" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="U93" s="66"/>
+      <c r="U93" s="62"/>
       <c r="V93" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="94" spans="13:22">
-      <c r="O94" s="60"/>
-      <c r="P94" s="55" t="s">
+      <c r="O94" s="56"/>
+      <c r="P94" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="Q94" s="55" t="s">
+      <c r="Q94" s="51" t="s">
         <v>241</v>
       </c>
       <c r="R94" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="S94" s="66"/>
+      <c r="S94" s="62"/>
       <c r="T94" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="U94" s="66"/>
+      <c r="U94" s="62"/>
       <c r="V94" t="s">
         <v>77</v>
       </c>
@@ -7810,229 +7860,241 @@
         <v>243</v>
       </c>
     </row>
-    <row r="97" spans="14:22">
+    <row r="97" spans="13:22">
       <c r="Q97" s="29" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="98" spans="14:22">
-      <c r="Q98" s="58" t="s">
+    <row r="98" spans="13:22">
+      <c r="Q98" s="54" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="99" spans="14:22">
-      <c r="P99" s="58" t="s">
+    <row r="99" spans="13:22">
+      <c r="P99" s="54" t="s">
         <v>65</v>
       </c>
-      <c r="Q99" s="58" t="s">
+      <c r="Q99" s="54" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="100" spans="14:22">
-      <c r="Q100" s="58" t="s">
+    <row r="100" spans="13:22">
+      <c r="Q100" s="54" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="101" spans="14:22">
-      <c r="Q101" s="58" t="s">
+    <row r="101" spans="13:22">
+      <c r="Q101" s="54" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="102" spans="14:22">
-      <c r="O102" s="60"/>
-      <c r="P102" s="55" t="s">
+    <row r="102" spans="13:22">
+      <c r="O102" s="56"/>
+      <c r="P102" s="51" t="s">
         <v>93</v>
       </c>
-      <c r="Q102" s="55" t="s">
+      <c r="Q102" s="51" t="s">
         <v>248</v>
       </c>
       <c r="R102" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="S102" s="66"/>
+      <c r="S102" s="62"/>
       <c r="T102" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="U102" s="66"/>
+      <c r="U102" s="62"/>
       <c r="V102" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="103" spans="14:22">
-      <c r="O103" s="60"/>
-      <c r="P103" s="56"/>
-      <c r="Q103" s="55" t="s">
+    <row r="103" spans="13:22">
+      <c r="O103" s="56"/>
+      <c r="P103" s="52"/>
+      <c r="Q103" s="51" t="s">
         <v>249</v>
       </c>
       <c r="R103" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="S103" s="66"/>
+      <c r="S103" s="62"/>
       <c r="T103" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="U103" s="66"/>
+      <c r="U103" s="62"/>
       <c r="V103" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="104" spans="14:22">
-      <c r="Q104" s="58" t="s">
+    <row r="104" spans="13:22">
+      <c r="M104" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="N104" s="69"/>
+      <c r="O104" s="69"/>
+      <c r="P104" s="69"/>
+      <c r="Q104" s="54" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="105" spans="14:22">
-      <c r="O105" s="60"/>
-      <c r="P105" s="56"/>
-      <c r="Q105" s="55" t="s">
+    <row r="105" spans="13:22">
+      <c r="O105" s="56"/>
+      <c r="P105" s="52"/>
+      <c r="Q105" s="51" t="s">
         <v>251</v>
       </c>
       <c r="R105" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="S105" s="66"/>
+      <c r="S105" s="62"/>
       <c r="T105" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="U105" s="66"/>
+      <c r="U105" s="62"/>
       <c r="V105" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="106" spans="14:22">
-      <c r="O106" s="60"/>
-      <c r="P106" s="55" t="s">
+    <row r="106" spans="13:22">
+      <c r="O106" s="56"/>
+      <c r="P106" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="Q106" s="55" t="s">
+      <c r="Q106" s="51" t="s">
         <v>252</v>
       </c>
       <c r="R106" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="S106" s="66"/>
+      <c r="S106" s="62"/>
       <c r="T106" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="U106" s="66"/>
+      <c r="U106" s="62"/>
       <c r="V106" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="107" spans="14:22">
-      <c r="O107" s="60"/>
-      <c r="P107" s="56"/>
-      <c r="Q107" s="55" t="s">
+    <row r="107" spans="13:22">
+      <c r="O107" s="56"/>
+      <c r="P107" s="52"/>
+      <c r="Q107" s="51" t="s">
         <v>253</v>
       </c>
       <c r="R107" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="S107" s="66"/>
+      <c r="S107" s="62"/>
       <c r="T107" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="U107" s="66"/>
+      <c r="U107" s="62"/>
       <c r="V107" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="108" spans="14:22">
-      <c r="O108" s="51"/>
-      <c r="P108" s="51"/>
-      <c r="Q108" s="52" t="s">
+    <row r="108" spans="13:22">
+      <c r="O108" s="47"/>
+      <c r="P108" s="47"/>
+      <c r="Q108" s="48" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="109" spans="14:22">
-      <c r="O109" s="51"/>
-      <c r="P109" s="51"/>
-      <c r="Q109" s="52" t="s">
+    <row r="109" spans="13:22">
+      <c r="O109" s="47"/>
+      <c r="P109" s="47"/>
+      <c r="Q109" s="48" t="s">
         <v>255</v>
       </c>
       <c r="R109" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="S109" s="66"/>
+      <c r="S109" s="62"/>
       <c r="T109" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="U109" s="66"/>
+      <c r="U109" s="62"/>
       <c r="V109" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="110" spans="14:22">
-      <c r="N110" s="60"/>
-      <c r="O110" s="52" t="s">
+    <row r="110" spans="13:22">
+      <c r="N110" s="56"/>
+      <c r="O110" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="P110" s="52" t="s">
+      <c r="P110" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="Q110" s="52" t="s">
+      <c r="Q110" s="48" t="s">
         <v>256</v>
       </c>
       <c r="R110" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="S110" s="66"/>
+      <c r="S110" s="62"/>
       <c r="T110" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="U110" s="66"/>
+      <c r="U110" s="62"/>
       <c r="V110" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="111" spans="14:22">
-      <c r="O111" s="51"/>
-      <c r="P111" s="51"/>
-      <c r="Q111" s="52" t="s">
+    <row r="111" spans="13:22">
+      <c r="O111" s="47"/>
+      <c r="P111" s="47"/>
+      <c r="Q111" s="48" t="s">
         <v>257</v>
       </c>
       <c r="R111" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="S111" s="66"/>
+      <c r="S111" s="62"/>
       <c r="T111" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="U111" s="66"/>
+      <c r="U111" s="62"/>
       <c r="V111" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="112" spans="14:22">
-      <c r="Q112" s="57" t="s">
+    <row r="112" spans="13:22">
+      <c r="Q112" s="53" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="113" spans="13:22">
-      <c r="Q113" s="58" t="s">
+      <c r="M113" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="N113" s="69"/>
+      <c r="O113" s="69"/>
+      <c r="P113" s="69"/>
+      <c r="Q113" s="54" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="114" spans="13:22">
-      <c r="Q114" s="58" t="s">
+      <c r="Q114" s="54" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="115" spans="13:22">
-      <c r="M115" s="69" t="s">
+      <c r="M115" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="P115" s="52" t="s">
+      <c r="P115" s="48" t="s">
         <v>67</v>
       </c>
-      <c r="Q115" s="52" t="s">
+      <c r="Q115" s="48" t="s">
         <v>261</v>
       </c>
-      <c r="S115" s="49"/>
+      <c r="S115" s="45"/>
       <c r="T115" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="U115" s="66"/>
+      <c r="U115" s="62"/>
       <c r="V115" t="s">
         <v>17</v>
       </c>
@@ -8654,7 +8716,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="42" t="s">
+      <c r="M14" s="66" t="s">
         <v>42</v>
       </c>
       <c r="N14" s="4"/>
@@ -8674,7 +8736,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="43"/>
+      <c r="M15" s="67"/>
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:26">
@@ -8692,7 +8754,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="43"/>
+      <c r="M16" s="67"/>
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14">
@@ -8710,7 +8772,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="22"/>
-      <c r="M17" s="43"/>
+      <c r="M17" s="67"/>
       <c r="N17" s="22"/>
     </row>
     <row r="18" spans="1:14">
@@ -8728,7 +8790,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="22"/>
-      <c r="M18" s="43"/>
+      <c r="M18" s="67"/>
       <c r="N18" s="22"/>
     </row>
     <row r="19" spans="1:14">
@@ -8746,7 +8808,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="22"/>
-      <c r="M19" s="43"/>
+      <c r="M19" s="67"/>
       <c r="N19" s="22"/>
     </row>
     <row r="20" spans="1:14">
@@ -8762,7 +8824,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="44"/>
+      <c r="M20" s="68"/>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:14">
@@ -9174,8 +9236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:P129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:A129"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9200,16 +9262,16 @@
       <c r="A3" s="29" t="s">
         <v>272</v>
       </c>
-      <c r="L3" s="45" t="s">
+      <c r="L3" s="42" t="s">
         <v>273</v>
       </c>
-      <c r="M3" s="49" t="s">
+      <c r="M3" s="42" t="s">
         <v>275</v>
       </c>
-      <c r="N3" s="49" t="s">
+      <c r="N3" s="45" t="s">
         <v>276</v>
       </c>
-      <c r="P3" s="29" t="s">
+      <c r="P3" s="45" t="s">
         <v>273</v>
       </c>
     </row>
@@ -9223,16 +9285,17 @@
       <c r="G4" s="36"/>
       <c r="H4" s="36"/>
       <c r="I4" s="37"/>
-      <c r="L4" s="46" t="s">
+      <c r="L4" s="43" t="s">
         <v>274</v>
       </c>
-      <c r="M4" s="47" t="s">
+      <c r="M4" s="44" t="s">
         <v>277</v>
       </c>
-      <c r="N4" s="50"/>
+      <c r="N4" s="46"/>
       <c r="O4" t="s">
         <v>18</v>
       </c>
+      <c r="P4" s="46"/>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="33" t="s">
@@ -9262,11 +9325,12 @@
       <c r="I5" s="34" t="s">
         <v>271</v>
       </c>
-      <c r="L5" s="47"/>
-      <c r="M5" s="46" t="s">
+      <c r="L5" s="44"/>
+      <c r="M5" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="N5" s="50"/>
+      <c r="N5" s="46"/>
+      <c r="P5" s="46"/>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="39"/>
@@ -9278,783 +9342,442 @@
       <c r="G6" s="40"/>
       <c r="H6" s="40"/>
       <c r="I6" s="41"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="46" t="s">
+      <c r="L6" s="44"/>
+      <c r="M6" s="43" t="s">
         <v>278</v>
       </c>
-      <c r="N6" s="50"/>
+      <c r="N6" s="46"/>
+      <c r="P6" s="46"/>
     </row>
     <row r="7" spans="1:16">
-      <c r="L7" s="47"/>
-      <c r="M7" s="46" t="s">
+      <c r="L7" s="44"/>
+      <c r="M7" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="50"/>
+      <c r="N7" s="46"/>
+      <c r="P7" s="46"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="L8" s="47"/>
-      <c r="M8" s="46" t="s">
+      <c r="I8" s="30" t="s">
+        <v>291</v>
+      </c>
+      <c r="L8" s="44"/>
+      <c r="M8" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="N8" s="50"/>
+      <c r="N8" s="46"/>
+      <c r="P8" s="46"/>
     </row>
     <row r="9" spans="1:16">
-      <c r="L9" s="47"/>
-      <c r="M9" s="48" t="s">
+      <c r="I9" s="30" t="s">
+        <v>293</v>
+      </c>
+      <c r="L9" s="44"/>
+      <c r="M9" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="50"/>
+      <c r="N9" s="46"/>
+      <c r="P9" s="46"/>
     </row>
     <row r="10" spans="1:16">
-      <c r="L10" s="47"/>
-      <c r="M10" s="48" t="s">
+      <c r="I10" s="30" t="s">
+        <v>292</v>
+      </c>
+      <c r="L10" s="44"/>
+      <c r="M10" s="43" t="s">
         <v>279</v>
       </c>
-      <c r="N10" s="50"/>
+      <c r="N10" s="46"/>
+      <c r="P10" s="46"/>
     </row>
     <row r="11" spans="1:16">
-      <c r="L11" s="47"/>
-      <c r="M11" s="48" t="s">
+      <c r="L11" s="44"/>
+      <c r="M11" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="N11" s="50"/>
+      <c r="N11" s="46"/>
+      <c r="P11" s="46"/>
     </row>
     <row r="12" spans="1:16">
-      <c r="L12" s="47"/>
-      <c r="M12" s="48" t="s">
+      <c r="L12" s="44"/>
+      <c r="M12" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="N12" s="50"/>
+      <c r="N12" s="46"/>
+      <c r="P12" s="46"/>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="29" t="s">
-        <v>280</v>
-      </c>
+      <c r="A13" s="29"/>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>108</v>
-      </c>
+      <c r="C15" s="29"/>
     </row>
     <row r="16" spans="1:16">
-      <c r="C16" s="29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="C17" s="29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="C18" s="29" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="29" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" s="29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="29" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>68</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="29" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25" s="29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="29" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="C27" s="29" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="C28" s="29" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="C29" s="29" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="29" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
-        <v>80</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="29" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="C33" s="29" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" s="29" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="29" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>70</v>
-      </c>
-      <c r="C37" s="29" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="29" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" t="s">
-        <v>82</v>
-      </c>
-      <c r="C39" s="29" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="29" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="29" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" t="s">
-        <v>83</v>
-      </c>
-      <c r="C42" s="29" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="C43" s="29" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="C44" s="29" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="C45" s="29" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="C46" s="29" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="C47" s="29" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" t="s">
-        <v>85</v>
-      </c>
-      <c r="C48" s="29" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" t="s">
-        <v>86</v>
-      </c>
-      <c r="C49" s="29" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="C50" s="29" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="C51" s="29" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="C52" s="29" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="C53" s="29" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="C54" s="29" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="C55" s="29" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="C56" s="29" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="C57" s="29" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="C58" s="29" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="C59" s="29" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="C60" s="29" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" t="s">
-        <v>72</v>
-      </c>
-      <c r="C61" s="29" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" s="29" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="C63" s="29" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="C64" s="29" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="C65" s="29" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="C66" s="29" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="C67" s="29" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="C68" s="29" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="C69" s="29" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" t="s">
-        <v>73</v>
-      </c>
-      <c r="C70" s="29" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="C71" s="29" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" t="s">
-        <v>89</v>
-      </c>
-      <c r="C72" s="29" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="C73" s="29" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="C74" s="29" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" t="s">
-        <v>98</v>
-      </c>
-      <c r="C75" s="29" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" t="s">
-        <v>98</v>
-      </c>
-      <c r="C76" s="29" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="C77" s="29" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" t="s">
-        <v>21</v>
-      </c>
-      <c r="C78" s="29" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="C79" s="29" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="C80" s="29" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="C81" s="29" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="C82" s="29" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="C83" s="29" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="C84" s="29" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="C85" s="29" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="C86" s="29" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" t="s">
-        <v>75</v>
-      </c>
-      <c r="C87" s="29" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" t="s">
-        <v>75</v>
-      </c>
-      <c r="C88" s="29" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="C89" s="29" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="C90" s="29" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="C91" s="29" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" t="s">
-        <v>96</v>
-      </c>
-      <c r="C92" s="29" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="C93" s="29" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" t="s">
-        <v>68</v>
-      </c>
-      <c r="C94" s="29" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" t="s">
-        <v>68</v>
-      </c>
-      <c r="C95" s="29" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="C96" s="29" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="C97" s="29" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" t="s">
-        <v>25</v>
-      </c>
-      <c r="C98" s="29" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" t="s">
-        <v>99</v>
-      </c>
-      <c r="C99" s="29" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" t="s">
-        <v>99</v>
-      </c>
-      <c r="C100" s="29" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" t="s">
-        <v>99</v>
-      </c>
-      <c r="C101" s="29" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="C102" s="29" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="C103" s="29" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="C104" s="29" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="C105" s="29" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" t="s">
-        <v>91</v>
-      </c>
-      <c r="C106" s="29" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" t="s">
-        <v>97</v>
-      </c>
-      <c r="C107" s="29" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" t="s">
-        <v>77</v>
-      </c>
-      <c r="C108" s="29" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="C109" s="29" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="C110" s="29" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="C111" s="29" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="C112" s="29" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="C113" s="29" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="C114" s="29" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="C115" s="29" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" t="s">
-        <v>93</v>
-      </c>
-      <c r="C116" s="29" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" t="s">
-        <v>93</v>
-      </c>
-      <c r="C117" s="29" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="C118" s="29" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" t="s">
-        <v>78</v>
-      </c>
-      <c r="C119" s="29" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" t="s">
-        <v>78</v>
-      </c>
-      <c r="C120" s="29" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" t="s">
-        <v>78</v>
-      </c>
-      <c r="C121" s="29" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="C122" s="29" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" t="s">
-        <v>95</v>
-      </c>
-      <c r="C123" s="29" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" t="s">
-        <v>95</v>
-      </c>
-      <c r="C124" s="29" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125" t="s">
-        <v>95</v>
-      </c>
-      <c r="C125" s="29" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="C126" s="29" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="C127" s="29" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="C128" s="29" t="s">
-        <v>260</v>
-      </c>
+      <c r="C16" s="29"/>
+    </row>
+    <row r="17" spans="3:14">
+      <c r="C17" s="29"/>
+      <c r="L17" s="70" t="s">
+        <v>294</v>
+      </c>
+      <c r="M17" s="70"/>
+      <c r="N17" s="70"/>
+    </row>
+    <row r="18" spans="3:14">
+      <c r="C18" s="29"/>
+      <c r="L18" s="70" t="s">
+        <v>295</v>
+      </c>
+      <c r="M18" s="70"/>
+      <c r="N18" s="70"/>
+    </row>
+    <row r="19" spans="3:14">
+      <c r="C19" s="29"/>
+      <c r="L19" s="70" t="s">
+        <v>296</v>
+      </c>
+      <c r="M19" s="70"/>
+      <c r="N19" s="70"/>
+    </row>
+    <row r="20" spans="3:14">
+      <c r="C20" s="29"/>
+      <c r="L20" s="70" t="s">
+        <v>297</v>
+      </c>
+      <c r="M20" s="70"/>
+      <c r="N20" s="70"/>
+    </row>
+    <row r="21" spans="3:14">
+      <c r="C21" s="29"/>
+      <c r="L21" s="70" t="s">
+        <v>298</v>
+      </c>
+      <c r="M21" s="70"/>
+      <c r="N21" s="70"/>
+    </row>
+    <row r="22" spans="3:14">
+      <c r="C22" s="29"/>
+    </row>
+    <row r="23" spans="3:14">
+      <c r="C23" s="29"/>
+    </row>
+    <row r="24" spans="3:14">
+      <c r="C24" s="29"/>
+    </row>
+    <row r="25" spans="3:14">
+      <c r="C25" s="29"/>
+    </row>
+    <row r="26" spans="3:14">
+      <c r="C26" s="29"/>
+    </row>
+    <row r="27" spans="3:14">
+      <c r="C27" s="29"/>
+    </row>
+    <row r="28" spans="3:14">
+      <c r="C28" s="29"/>
+    </row>
+    <row r="29" spans="3:14">
+      <c r="C29" s="29"/>
+    </row>
+    <row r="30" spans="3:14">
+      <c r="C30" s="29"/>
+    </row>
+    <row r="31" spans="3:14">
+      <c r="C31" s="29"/>
+    </row>
+    <row r="32" spans="3:14">
+      <c r="C32" s="29"/>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="29"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="29"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="29"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="29"/>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="29"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="29"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="29"/>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="29"/>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="29"/>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="29"/>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="29"/>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="29"/>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" s="29"/>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" s="29"/>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" s="29"/>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48" s="29"/>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" s="29"/>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" s="29"/>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" s="29"/>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52" s="29"/>
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53" s="29"/>
+    </row>
+    <row r="54" spans="3:3">
+      <c r="C54" s="29"/>
+    </row>
+    <row r="55" spans="3:3">
+      <c r="C55" s="29"/>
+    </row>
+    <row r="56" spans="3:3">
+      <c r="C56" s="29"/>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57" s="29"/>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" s="29"/>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" s="29"/>
+    </row>
+    <row r="60" spans="3:3">
+      <c r="C60" s="29"/>
+    </row>
+    <row r="61" spans="3:3">
+      <c r="C61" s="29"/>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62" s="29"/>
+    </row>
+    <row r="63" spans="3:3">
+      <c r="C63" s="29"/>
+    </row>
+    <row r="64" spans="3:3">
+      <c r="C64" s="29"/>
+    </row>
+    <row r="65" spans="3:3">
+      <c r="C65" s="29"/>
+    </row>
+    <row r="66" spans="3:3">
+      <c r="C66" s="29"/>
+    </row>
+    <row r="67" spans="3:3">
+      <c r="C67" s="29"/>
+    </row>
+    <row r="68" spans="3:3">
+      <c r="C68" s="29"/>
+    </row>
+    <row r="69" spans="3:3">
+      <c r="C69" s="29"/>
+    </row>
+    <row r="70" spans="3:3">
+      <c r="C70" s="29"/>
+    </row>
+    <row r="71" spans="3:3">
+      <c r="C71" s="29"/>
+    </row>
+    <row r="72" spans="3:3">
+      <c r="C72" s="29"/>
+    </row>
+    <row r="73" spans="3:3">
+      <c r="C73" s="29"/>
+    </row>
+    <row r="74" spans="3:3">
+      <c r="C74" s="29"/>
+    </row>
+    <row r="75" spans="3:3">
+      <c r="C75" s="29"/>
+    </row>
+    <row r="76" spans="3:3">
+      <c r="C76" s="29"/>
+    </row>
+    <row r="77" spans="3:3">
+      <c r="C77" s="29"/>
+    </row>
+    <row r="78" spans="3:3">
+      <c r="C78" s="29"/>
+    </row>
+    <row r="79" spans="3:3">
+      <c r="C79" s="29"/>
+    </row>
+    <row r="80" spans="3:3">
+      <c r="C80" s="29"/>
+    </row>
+    <row r="81" spans="3:3">
+      <c r="C81" s="29"/>
+    </row>
+    <row r="82" spans="3:3">
+      <c r="C82" s="29"/>
+    </row>
+    <row r="83" spans="3:3">
+      <c r="C83" s="29"/>
+    </row>
+    <row r="84" spans="3:3">
+      <c r="C84" s="29"/>
+    </row>
+    <row r="85" spans="3:3">
+      <c r="C85" s="29"/>
+    </row>
+    <row r="86" spans="3:3">
+      <c r="C86" s="29"/>
+    </row>
+    <row r="87" spans="3:3">
+      <c r="C87" s="29"/>
+    </row>
+    <row r="88" spans="3:3">
+      <c r="C88" s="29"/>
+    </row>
+    <row r="89" spans="3:3">
+      <c r="C89" s="29"/>
+    </row>
+    <row r="90" spans="3:3">
+      <c r="C90" s="29"/>
+    </row>
+    <row r="91" spans="3:3">
+      <c r="C91" s="29"/>
+    </row>
+    <row r="92" spans="3:3">
+      <c r="C92" s="29"/>
+    </row>
+    <row r="93" spans="3:3">
+      <c r="C93" s="29"/>
+    </row>
+    <row r="94" spans="3:3">
+      <c r="C94" s="29"/>
+    </row>
+    <row r="95" spans="3:3">
+      <c r="C95" s="29"/>
+    </row>
+    <row r="96" spans="3:3">
+      <c r="C96" s="29"/>
+    </row>
+    <row r="97" spans="3:3">
+      <c r="C97" s="29"/>
+    </row>
+    <row r="98" spans="3:3">
+      <c r="C98" s="29"/>
+    </row>
+    <row r="99" spans="3:3">
+      <c r="C99" s="29"/>
+    </row>
+    <row r="100" spans="3:3">
+      <c r="C100" s="29"/>
+    </row>
+    <row r="101" spans="3:3">
+      <c r="C101" s="29"/>
+    </row>
+    <row r="102" spans="3:3">
+      <c r="C102" s="29"/>
+    </row>
+    <row r="103" spans="3:3">
+      <c r="C103" s="29"/>
+    </row>
+    <row r="104" spans="3:3">
+      <c r="C104" s="29"/>
+    </row>
+    <row r="105" spans="3:3">
+      <c r="C105" s="29"/>
+    </row>
+    <row r="106" spans="3:3">
+      <c r="C106" s="29"/>
+    </row>
+    <row r="107" spans="3:3">
+      <c r="C107" s="29"/>
+    </row>
+    <row r="108" spans="3:3">
+      <c r="C108" s="29"/>
+    </row>
+    <row r="109" spans="3:3">
+      <c r="C109" s="29"/>
+    </row>
+    <row r="110" spans="3:3">
+      <c r="C110" s="29"/>
+    </row>
+    <row r="111" spans="3:3">
+      <c r="C111" s="29"/>
+    </row>
+    <row r="112" spans="3:3">
+      <c r="C112" s="29"/>
+    </row>
+    <row r="113" spans="3:3">
+      <c r="C113" s="29"/>
+    </row>
+    <row r="114" spans="3:3">
+      <c r="C114" s="29"/>
+    </row>
+    <row r="115" spans="3:3">
+      <c r="C115" s="29"/>
+    </row>
+    <row r="116" spans="3:3">
+      <c r="C116" s="29"/>
+    </row>
+    <row r="117" spans="3:3">
+      <c r="C117" s="29"/>
+    </row>
+    <row r="118" spans="3:3">
+      <c r="C118" s="29"/>
+    </row>
+    <row r="119" spans="3:3">
+      <c r="C119" s="29"/>
+    </row>
+    <row r="120" spans="3:3">
+      <c r="C120" s="29"/>
+    </row>
+    <row r="121" spans="3:3">
+      <c r="C121" s="29"/>
+    </row>
+    <row r="122" spans="3:3">
+      <c r="C122" s="29"/>
+    </row>
+    <row r="123" spans="3:3">
+      <c r="C123" s="29"/>
+    </row>
+    <row r="124" spans="3:3">
+      <c r="C124" s="29"/>
+    </row>
+    <row r="125" spans="3:3">
+      <c r="C125" s="29"/>
+    </row>
+    <row r="126" spans="3:3">
+      <c r="C126" s="29"/>
+    </row>
+    <row r="127" spans="3:3">
+      <c r="C127" s="29"/>
+    </row>
+    <row r="128" spans="3:3">
+      <c r="C128" s="29"/>
     </row>
     <row r="129" spans="3:3">
-      <c r="C129" s="29" t="s">
-        <v>261</v>
-      </c>
+      <c r="C129" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
more.... started changes to food need balancing
</commit_message>
<xml_diff>
--- a/Food_SR_Organization.xlsx
+++ b/Food_SR_Organization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="560" windowWidth="28760" windowHeight="17540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="-80" yWindow="7560" windowWidth="28820" windowHeight="10020" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="1.Food Need" sheetId="3" r:id="rId1"/>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="381">
   <si>
     <t>ALL LOCAL</t>
   </si>
@@ -1220,9 +1220,6 @@
     <t>Field Crops (wheat/oats/barley/graincorn/drypeas/silage)</t>
   </si>
   <si>
-    <t>Key</t>
-  </si>
-  <si>
     <t>head of livestock/hectare</t>
   </si>
   <si>
@@ -1293,6 +1290,39 @@
   </si>
   <si>
     <t>4: Food Self Reliance</t>
+  </si>
+  <si>
+    <t>Instead of taking the average I am going to do a more precise method…….</t>
+  </si>
+  <si>
+    <t>(#1yr olds/SWBC pop)(food group recommended servings) + (#2yr olds/SWBC pop)(food group recommended servings)………</t>
+  </si>
+  <si>
+    <t>or by age group (it makes no difference quantitatively because the recommendation is expressed by group</t>
+  </si>
+  <si>
+    <t>(# in group #1)(food group recommended servings)+(# in group #2)(food group recommended servings)…….</t>
+  </si>
+  <si>
+    <t>To Do:</t>
+  </si>
+  <si>
+    <t>1. Change food recommendation balancing methods</t>
+  </si>
+  <si>
+    <t>2. Check food need values against the ones from Caitlin's email</t>
+  </si>
+  <si>
+    <t>4. Check SWBC crop production values against the ones from the Excel model</t>
+  </si>
+  <si>
+    <t>3. Take 10yr average for field crops and use that instead of one yr value.</t>
+  </si>
+  <si>
+    <t>6. Wait for Caitlin's response about livestock method. Double check methods.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Change to 10 yr average for Canola Meal yield. </t>
   </si>
 </sst>
 </file>
@@ -1377,7 +1407,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="28">
+  <fills count="29">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1538,6 +1568,12 @@
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1856,7 +1892,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="373">
+  <cellStyleXfs count="393">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2230,8 +2266,28 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="193">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2308,116 +2364,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
@@ -2430,16 +2378,32 @@
     <xf numFmtId="0" fontId="3" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2447,47 +2411,79 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2502,41 +2498,83 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2554,6 +2592,27 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2574,26 +2633,42 @@
     <xf numFmtId="0" fontId="8" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="373">
+  <cellStyles count="393">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2780,6 +2855,16 @@
     <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2966,6 +3051,16 @@
     <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -9841,7 +9936,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="68" t="s">
+      <c r="M14" s="90" t="s">
         <v>42</v>
       </c>
       <c r="N14" s="4"/>
@@ -9861,7 +9956,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="69"/>
+      <c r="M15" s="91"/>
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:26">
@@ -9879,7 +9974,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="69"/>
+      <c r="M16" s="91"/>
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14">
@@ -9897,7 +9992,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="22"/>
-      <c r="M17" s="69"/>
+      <c r="M17" s="91"/>
       <c r="N17" s="22"/>
     </row>
     <row r="18" spans="1:14">
@@ -9915,7 +10010,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="22"/>
-      <c r="M18" s="69"/>
+      <c r="M18" s="91"/>
       <c r="N18" s="22"/>
     </row>
     <row r="19" spans="1:14">
@@ -9933,7 +10028,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="22"/>
-      <c r="M19" s="69"/>
+      <c r="M19" s="91"/>
       <c r="N19" s="22"/>
     </row>
     <row r="20" spans="1:14">
@@ -9949,7 +10044,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="70"/>
+      <c r="M20" s="92"/>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:14">
@@ -10558,11 +10653,11 @@
     </row>
     <row r="19" spans="3:14">
       <c r="C19" s="29"/>
-      <c r="L19" s="71" t="s">
+      <c r="L19" s="68" t="s">
         <v>296</v>
       </c>
-      <c r="M19" s="71"/>
-      <c r="N19" s="71"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="68"/>
     </row>
     <row r="20" spans="3:14">
       <c r="C20" s="29"/>
@@ -10917,10 +11012,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE75"/>
+  <dimension ref="A1:AF75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="Q59" sqref="Q59"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="Q74" sqref="Q74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10939,41 +11034,41 @@
     <col min="28" max="28" width="4.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31">
-      <c r="A1" s="104" t="s">
+    <row r="1" spans="1:29">
+      <c r="A1" s="141" t="s">
         <v>304</v>
       </c>
-      <c r="B1" s="105"/>
-      <c r="C1" s="105"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="106"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="106"/>
-      <c r="K1" s="106"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="106"/>
-      <c r="N1" s="106"/>
-      <c r="O1" s="106"/>
-      <c r="P1" s="106"/>
-      <c r="Q1" s="106"/>
-      <c r="R1" s="106"/>
-      <c r="S1" s="106"/>
-      <c r="T1" s="106"/>
-      <c r="U1" s="106"/>
-      <c r="V1" s="106"/>
-      <c r="W1" s="106"/>
-      <c r="X1" s="106"/>
-      <c r="Y1" s="106"/>
-      <c r="Z1" s="106"/>
-      <c r="AA1" s="106"/>
-      <c r="AB1" s="106"/>
-      <c r="AC1" s="107"/>
-    </row>
-    <row r="2" spans="1:31">
-      <c r="A2" s="108"/>
+      <c r="B1" s="142"/>
+      <c r="C1" s="142"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="70"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
+      <c r="Z1" s="70"/>
+      <c r="AA1" s="70"/>
+      <c r="AB1" s="70"/>
+      <c r="AC1" s="71"/>
+    </row>
+    <row r="2" spans="1:29">
+      <c r="A2" s="72"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -11001,95 +11096,92 @@
       <c r="Z2" s="4"/>
       <c r="AA2" s="4"/>
       <c r="AB2" s="4"/>
-      <c r="AC2" s="109"/>
-      <c r="AE2" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:31" ht="15" customHeight="1">
-      <c r="A3" s="108"/>
-      <c r="B3" s="72" t="s">
+      <c r="AC2" s="73"/>
+    </row>
+    <row r="3" spans="1:29" ht="15" customHeight="1">
+      <c r="A3" s="72"/>
+      <c r="B3" s="111" t="s">
         <v>299</v>
       </c>
-      <c r="C3" s="73"/>
+      <c r="C3" s="113"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="132" t="s">
         <v>300</v>
       </c>
-      <c r="F3" s="77"/>
+      <c r="F3" s="133"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="72" t="s">
+      <c r="H3" s="111" t="s">
         <v>305</v>
       </c>
-      <c r="I3" s="73"/>
+      <c r="I3" s="113"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="72" t="s">
+      <c r="K3" s="111" t="s">
         <v>306</v>
       </c>
-      <c r="L3" s="73"/>
+      <c r="L3" s="113"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="76" t="s">
+      <c r="N3" s="132" t="s">
         <v>307</v>
       </c>
-      <c r="O3" s="77"/>
+      <c r="O3" s="133"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="76" t="s">
+      <c r="Q3" s="132" t="s">
         <v>308</v>
       </c>
-      <c r="R3" s="77"/>
+      <c r="R3" s="133"/>
       <c r="S3" s="4"/>
-      <c r="T3" s="92" t="s">
+      <c r="T3" s="105" t="s">
         <v>310</v>
       </c>
-      <c r="U3" s="93"/>
-      <c r="V3" s="93"/>
+      <c r="U3" s="169"/>
+      <c r="V3" s="169"/>
       <c r="W3" s="4"/>
-      <c r="X3" s="149" t="s">
-        <v>362</v>
-      </c>
-      <c r="Y3" s="150"/>
+      <c r="X3" s="159" t="s">
+        <v>361</v>
+      </c>
+      <c r="Y3" s="160"/>
       <c r="Z3" s="4"/>
-      <c r="AA3" s="149" t="s">
+      <c r="AA3" s="159" t="s">
         <v>312</v>
       </c>
-      <c r="AB3" s="150"/>
-      <c r="AC3" s="109"/>
-    </row>
-    <row r="4" spans="1:31" ht="15" customHeight="1">
-      <c r="A4" s="110" t="s">
+      <c r="AB3" s="160"/>
+      <c r="AC3" s="73"/>
+    </row>
+    <row r="4" spans="1:29" ht="15" customHeight="1">
+      <c r="A4" s="74" t="s">
         <v>302</v>
       </c>
-      <c r="B4" s="74"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="74"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="74"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="94"/>
-      <c r="N4" s="78"/>
-      <c r="O4" s="79"/>
-      <c r="P4" s="94"/>
-      <c r="Q4" s="78"/>
-      <c r="R4" s="79"/>
-      <c r="S4" s="94"/>
-      <c r="T4" s="92"/>
-      <c r="U4" s="93"/>
-      <c r="V4" s="93"/>
-      <c r="W4" s="94"/>
-      <c r="X4" s="151"/>
-      <c r="Y4" s="152"/>
-      <c r="Z4" s="94"/>
-      <c r="AA4" s="151"/>
-      <c r="AB4" s="152"/>
-      <c r="AC4" s="109"/>
-    </row>
-    <row r="5" spans="1:31">
-      <c r="A5" s="108"/>
+      <c r="B4" s="114"/>
+      <c r="C4" s="116"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="136"/>
+      <c r="F4" s="137"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="116"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="136"/>
+      <c r="O4" s="137"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="136"/>
+      <c r="R4" s="137"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="105"/>
+      <c r="U4" s="169"/>
+      <c r="V4" s="169"/>
+      <c r="W4" s="69"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="162"/>
+      <c r="Z4" s="69"/>
+      <c r="AA4" s="161"/>
+      <c r="AB4" s="162"/>
+      <c r="AC4" s="73"/>
+    </row>
+    <row r="5" spans="1:29">
+      <c r="A5" s="72"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
@@ -11117,17 +11209,17 @@
       <c r="Z5" s="4"/>
       <c r="AA5" s="4"/>
       <c r="AB5" s="4"/>
-      <c r="AC5" s="109"/>
-    </row>
-    <row r="6" spans="1:31" ht="15" customHeight="1">
-      <c r="A6" s="108"/>
+      <c r="AC5" s="73"/>
+    </row>
+    <row r="6" spans="1:29" ht="15" customHeight="1">
+      <c r="A6" s="72"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="80" t="s">
+      <c r="E6" s="95" t="s">
         <v>301</v>
       </c>
-      <c r="F6" s="81"/>
+      <c r="F6" s="96"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -11138,59 +11230,59 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="80" t="s">
+      <c r="Q6" s="95" t="s">
         <v>309</v>
       </c>
-      <c r="R6" s="81"/>
+      <c r="R6" s="96"/>
       <c r="S6" s="4"/>
-      <c r="T6" s="89" t="s">
-        <v>361</v>
-      </c>
-      <c r="U6" s="89"/>
-      <c r="V6" s="89"/>
+      <c r="T6" s="125" t="s">
+        <v>360</v>
+      </c>
+      <c r="U6" s="125"/>
+      <c r="V6" s="125"/>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
       <c r="AA6" s="4"/>
       <c r="AB6" s="4"/>
-      <c r="AC6" s="109"/>
-    </row>
-    <row r="7" spans="1:31" ht="15" customHeight="1">
-      <c r="A7" s="110" t="s">
+      <c r="AC6" s="73"/>
+    </row>
+    <row r="7" spans="1:29" ht="15" customHeight="1">
+      <c r="A7" s="74" t="s">
         <v>303</v>
       </c>
-      <c r="B7" s="94"/>
-      <c r="C7" s="94"/>
-      <c r="D7" s="94"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="91"/>
-      <c r="S7" s="94"/>
-      <c r="T7" s="89"/>
-      <c r="U7" s="89"/>
-      <c r="V7" s="89"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="128"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="69"/>
+      <c r="N7" s="69"/>
+      <c r="O7" s="69"/>
+      <c r="P7" s="69"/>
+      <c r="Q7" s="97"/>
+      <c r="R7" s="98"/>
+      <c r="S7" s="69"/>
+      <c r="T7" s="125"/>
+      <c r="U7" s="125"/>
+      <c r="V7" s="125"/>
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
       <c r="Z7" s="4"/>
       <c r="AA7" s="4"/>
       <c r="AB7" s="4"/>
-      <c r="AC7" s="109"/>
-    </row>
-    <row r="8" spans="1:31">
-      <c r="A8" s="108"/>
+      <c r="AC7" s="73"/>
+    </row>
+    <row r="8" spans="1:29" ht="16" thickBot="1">
+      <c r="A8" s="72"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
@@ -11206,188 +11298,194 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="90"/>
-      <c r="R8" s="91"/>
+      <c r="Q8" s="97"/>
+      <c r="R8" s="98"/>
       <c r="S8" s="4"/>
-      <c r="T8" s="89"/>
-      <c r="U8" s="89"/>
-      <c r="V8" s="89"/>
+      <c r="T8" s="125"/>
+      <c r="U8" s="125"/>
+      <c r="V8" s="125"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
       <c r="Z8" s="4"/>
       <c r="AA8" s="4"/>
       <c r="AB8" s="4"/>
-      <c r="AC8" s="109"/>
-    </row>
-    <row r="9" spans="1:31">
-      <c r="A9" s="108"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
+      <c r="AC8" s="73"/>
+    </row>
+    <row r="9" spans="1:29">
+      <c r="A9" s="72"/>
+      <c r="B9" s="185" t="s">
+        <v>370</v>
+      </c>
+      <c r="C9" s="171"/>
+      <c r="D9" s="171"/>
+      <c r="E9" s="171"/>
+      <c r="F9" s="171"/>
+      <c r="G9" s="171"/>
+      <c r="H9" s="171"/>
+      <c r="I9" s="171"/>
+      <c r="J9" s="171"/>
+      <c r="K9" s="171"/>
+      <c r="L9" s="172"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="90"/>
-      <c r="R9" s="91"/>
+      <c r="Q9" s="97"/>
+      <c r="R9" s="98"/>
       <c r="S9" s="4"/>
-      <c r="T9" s="89"/>
-      <c r="U9" s="89"/>
-      <c r="V9" s="89"/>
+      <c r="T9" s="125"/>
+      <c r="U9" s="125"/>
+      <c r="V9" s="125"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
       <c r="Z9" s="4"/>
       <c r="AA9" s="4"/>
       <c r="AB9" s="4"/>
-      <c r="AC9" s="109"/>
-    </row>
-    <row r="10" spans="1:31">
-      <c r="A10" s="108"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
+      <c r="AC9" s="73"/>
+    </row>
+    <row r="10" spans="1:29">
+      <c r="A10" s="72"/>
+      <c r="B10" s="186"/>
+      <c r="C10" s="170"/>
+      <c r="D10" s="170"/>
+      <c r="E10" s="170"/>
+      <c r="F10" s="170"/>
+      <c r="G10" s="170"/>
+      <c r="H10" s="170"/>
+      <c r="I10" s="170"/>
+      <c r="J10" s="170"/>
+      <c r="K10" s="170"/>
+      <c r="L10" s="173"/>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="90"/>
-      <c r="R10" s="91"/>
+      <c r="Q10" s="97"/>
+      <c r="R10" s="98"/>
       <c r="S10" s="4"/>
-      <c r="T10" s="89"/>
-      <c r="U10" s="89"/>
-      <c r="V10" s="89"/>
+      <c r="T10" s="125"/>
+      <c r="U10" s="125"/>
+      <c r="V10" s="125"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
       <c r="Z10" s="4"/>
       <c r="AA10" s="4"/>
       <c r="AB10" s="4"/>
-      <c r="AC10" s="109"/>
-    </row>
-    <row r="11" spans="1:31">
-      <c r="A11" s="108"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
+      <c r="AC10" s="73"/>
+    </row>
+    <row r="11" spans="1:29">
+      <c r="A11" s="72"/>
+      <c r="B11" s="186" t="s">
+        <v>371</v>
+      </c>
+      <c r="C11" s="170"/>
+      <c r="D11" s="170"/>
+      <c r="E11" s="170"/>
+      <c r="F11" s="170"/>
+      <c r="G11" s="170"/>
+      <c r="H11" s="170"/>
+      <c r="I11" s="170"/>
+      <c r="J11" s="170"/>
+      <c r="K11" s="170"/>
+      <c r="L11" s="173"/>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="90"/>
-      <c r="R11" s="91"/>
+      <c r="Q11" s="97"/>
+      <c r="R11" s="98"/>
       <c r="S11" s="4"/>
-      <c r="T11" s="89"/>
-      <c r="U11" s="89"/>
-      <c r="V11" s="89"/>
+      <c r="T11" s="125"/>
+      <c r="U11" s="125"/>
+      <c r="V11" s="125"/>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
       <c r="Z11" s="4"/>
       <c r="AA11" s="4"/>
       <c r="AB11" s="4"/>
-      <c r="AC11" s="109"/>
-    </row>
-    <row r="12" spans="1:31">
-      <c r="A12" s="108"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
+      <c r="AC11" s="73"/>
+    </row>
+    <row r="12" spans="1:29">
+      <c r="A12" s="72"/>
+      <c r="B12" s="186"/>
+      <c r="C12" s="170"/>
+      <c r="D12" s="170"/>
+      <c r="E12" s="170"/>
+      <c r="F12" s="170"/>
+      <c r="G12" s="170"/>
+      <c r="H12" s="170"/>
+      <c r="I12" s="170"/>
+      <c r="J12" s="170"/>
+      <c r="K12" s="170"/>
+      <c r="L12" s="173"/>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="90"/>
-      <c r="R12" s="91"/>
+      <c r="Q12" s="97"/>
+      <c r="R12" s="98"/>
       <c r="S12" s="4"/>
-      <c r="T12" s="89"/>
-      <c r="U12" s="89"/>
-      <c r="V12" s="89"/>
+      <c r="T12" s="125"/>
+      <c r="U12" s="125"/>
+      <c r="V12" s="125"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
       <c r="Z12" s="4"/>
       <c r="AA12" s="4"/>
       <c r="AB12" s="4"/>
-      <c r="AC12" s="109"/>
-    </row>
-    <row r="13" spans="1:31">
-      <c r="A13" s="108"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
+      <c r="AC12" s="73"/>
+    </row>
+    <row r="13" spans="1:29">
+      <c r="A13" s="72"/>
+      <c r="B13" s="186" t="s">
+        <v>372</v>
+      </c>
+      <c r="C13" s="170"/>
+      <c r="D13" s="170"/>
+      <c r="E13" s="170"/>
+      <c r="F13" s="170"/>
+      <c r="G13" s="170"/>
+      <c r="H13" s="170"/>
+      <c r="I13" s="170"/>
+      <c r="J13" s="170"/>
+      <c r="K13" s="170"/>
+      <c r="L13" s="173"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="82"/>
-      <c r="R13" s="83"/>
+      <c r="Q13" s="126"/>
+      <c r="R13" s="128"/>
       <c r="S13" s="4"/>
-      <c r="T13" s="89"/>
-      <c r="U13" s="89"/>
-      <c r="V13" s="89"/>
+      <c r="T13" s="125"/>
+      <c r="U13" s="125"/>
+      <c r="V13" s="125"/>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
       <c r="Z13" s="4"/>
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
-      <c r="AC13" s="109"/>
-    </row>
-    <row r="14" spans="1:31">
-      <c r="A14" s="108"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
+      <c r="AC13" s="73"/>
+    </row>
+    <row r="14" spans="1:29">
+      <c r="A14" s="72"/>
+      <c r="B14" s="186"/>
+      <c r="C14" s="170"/>
+      <c r="D14" s="170"/>
+      <c r="E14" s="170"/>
+      <c r="F14" s="170"/>
+      <c r="G14" s="170"/>
+      <c r="H14" s="170"/>
+      <c r="I14" s="170"/>
+      <c r="J14" s="170"/>
+      <c r="K14" s="170"/>
+      <c r="L14" s="173"/>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
@@ -11395,30 +11493,32 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
-      <c r="T14" s="89"/>
-      <c r="U14" s="89"/>
-      <c r="V14" s="89"/>
+      <c r="T14" s="125"/>
+      <c r="U14" s="125"/>
+      <c r="V14" s="125"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
       <c r="Z14" s="4"/>
       <c r="AA14" s="4"/>
       <c r="AB14" s="4"/>
-      <c r="AC14" s="109"/>
-    </row>
-    <row r="15" spans="1:31">
-      <c r="A15" s="108"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
+      <c r="AC14" s="73"/>
+    </row>
+    <row r="15" spans="1:29" ht="16" thickBot="1">
+      <c r="A15" s="72"/>
+      <c r="B15" s="187" t="s">
+        <v>373</v>
+      </c>
+      <c r="C15" s="174"/>
+      <c r="D15" s="174"/>
+      <c r="E15" s="174"/>
+      <c r="F15" s="174"/>
+      <c r="G15" s="174"/>
+      <c r="H15" s="174"/>
+      <c r="I15" s="174"/>
+      <c r="J15" s="174"/>
+      <c r="K15" s="174"/>
+      <c r="L15" s="175"/>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -11426,19 +11526,19 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
-      <c r="T15" s="89"/>
-      <c r="U15" s="89"/>
-      <c r="V15" s="89"/>
+      <c r="T15" s="125"/>
+      <c r="U15" s="125"/>
+      <c r="V15" s="125"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
       <c r="Z15" s="4"/>
       <c r="AA15" s="4"/>
       <c r="AB15" s="4"/>
-      <c r="AC15" s="109"/>
-    </row>
-    <row r="16" spans="1:31">
-      <c r="A16" s="108"/>
+      <c r="AC15" s="73"/>
+    </row>
+    <row r="16" spans="1:29">
+      <c r="A16" s="72"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
@@ -11457,19 +11557,19 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
-      <c r="T16" s="89"/>
-      <c r="U16" s="89"/>
-      <c r="V16" s="89"/>
+      <c r="T16" s="125"/>
+      <c r="U16" s="125"/>
+      <c r="V16" s="125"/>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
       <c r="Z16" s="4"/>
       <c r="AA16" s="4"/>
       <c r="AB16" s="4"/>
-      <c r="AC16" s="109"/>
-    </row>
-    <row r="17" spans="1:29">
-      <c r="A17" s="108"/>
+      <c r="AC16" s="73"/>
+    </row>
+    <row r="17" spans="1:32">
+      <c r="A17" s="72"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
@@ -11488,74 +11588,74 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
-      <c r="T17" s="89"/>
-      <c r="U17" s="89"/>
-      <c r="V17" s="89"/>
+      <c r="T17" s="125"/>
+      <c r="U17" s="125"/>
+      <c r="V17" s="125"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
       <c r="Z17" s="4"/>
       <c r="AA17" s="4"/>
       <c r="AB17" s="4"/>
-      <c r="AC17" s="109"/>
-    </row>
-    <row r="18" spans="1:29" ht="16" thickBot="1">
-      <c r="A18" s="111"/>
-      <c r="B18" s="112"/>
-      <c r="C18" s="112"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="112"/>
-      <c r="F18" s="112"/>
-      <c r="G18" s="112"/>
-      <c r="H18" s="112"/>
-      <c r="I18" s="112"/>
-      <c r="J18" s="112"/>
-      <c r="K18" s="112"/>
-      <c r="L18" s="112"/>
-      <c r="M18" s="112"/>
-      <c r="N18" s="112"/>
-      <c r="O18" s="112"/>
-      <c r="P18" s="112"/>
-      <c r="Q18" s="112"/>
-      <c r="R18" s="112"/>
-      <c r="S18" s="112"/>
-      <c r="T18" s="112"/>
-      <c r="U18" s="112"/>
-      <c r="V18" s="112"/>
-      <c r="W18" s="112"/>
-      <c r="X18" s="112"/>
-      <c r="Y18" s="112"/>
-      <c r="Z18" s="112"/>
-      <c r="AA18" s="112"/>
-      <c r="AB18" s="112"/>
-      <c r="AC18" s="113"/>
-    </row>
-    <row r="19" spans="1:29">
-      <c r="A19" s="104" t="s">
+      <c r="AC17" s="73"/>
+    </row>
+    <row r="18" spans="1:32" ht="16" thickBot="1">
+      <c r="A18" s="75"/>
+      <c r="B18" s="76"/>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="76"/>
+      <c r="K18" s="76"/>
+      <c r="L18" s="76"/>
+      <c r="M18" s="76"/>
+      <c r="N18" s="76"/>
+      <c r="O18" s="76"/>
+      <c r="P18" s="76"/>
+      <c r="Q18" s="76"/>
+      <c r="R18" s="76"/>
+      <c r="S18" s="76"/>
+      <c r="T18" s="76"/>
+      <c r="U18" s="76"/>
+      <c r="V18" s="76"/>
+      <c r="W18" s="76"/>
+      <c r="X18" s="76"/>
+      <c r="Y18" s="76"/>
+      <c r="Z18" s="76"/>
+      <c r="AA18" s="76"/>
+      <c r="AB18" s="76"/>
+      <c r="AC18" s="77"/>
+    </row>
+    <row r="19" spans="1:32">
+      <c r="A19" s="141" t="s">
         <v>313</v>
       </c>
-      <c r="B19" s="105"/>
-      <c r="C19" s="105"/>
-      <c r="D19" s="106"/>
-      <c r="E19" s="106"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="106"/>
-      <c r="I19" s="106"/>
-      <c r="J19" s="106"/>
-      <c r="K19" s="106"/>
-      <c r="L19" s="106"/>
-      <c r="M19" s="106"/>
-      <c r="N19" s="106"/>
-      <c r="O19" s="106"/>
-      <c r="P19" s="106"/>
-      <c r="Q19" s="106"/>
-      <c r="R19" s="106"/>
-      <c r="S19" s="106"/>
-      <c r="T19" s="106"/>
-      <c r="U19" s="106"/>
-      <c r="V19" s="106"/>
-      <c r="W19" s="107"/>
+      <c r="B19" s="142"/>
+      <c r="C19" s="142"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="70"/>
+      <c r="G19" s="70"/>
+      <c r="H19" s="70"/>
+      <c r="I19" s="70"/>
+      <c r="J19" s="70"/>
+      <c r="K19" s="70"/>
+      <c r="L19" s="70"/>
+      <c r="M19" s="70"/>
+      <c r="N19" s="70"/>
+      <c r="O19" s="70"/>
+      <c r="P19" s="70"/>
+      <c r="Q19" s="70"/>
+      <c r="R19" s="70"/>
+      <c r="S19" s="70"/>
+      <c r="T19" s="70"/>
+      <c r="U19" s="70"/>
+      <c r="V19" s="70"/>
+      <c r="W19" s="71"/>
       <c r="X19" s="4"/>
       <c r="Y19" s="4"/>
       <c r="Z19" s="4"/>
@@ -11563,8 +11663,8 @@
       <c r="AB19" s="4"/>
       <c r="AC19" s="4"/>
     </row>
-    <row r="20" spans="1:29">
-      <c r="A20" s="108"/>
+    <row r="20" spans="1:32">
+      <c r="A20" s="72"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
@@ -11586,76 +11686,76 @@
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
       <c r="V20" s="4"/>
-      <c r="W20" s="109"/>
-    </row>
-    <row r="21" spans="1:29" ht="15" customHeight="1">
-      <c r="A21" s="108"/>
-      <c r="B21" s="76" t="s">
+      <c r="W20" s="73"/>
+    </row>
+    <row r="21" spans="1:32" ht="15" customHeight="1">
+      <c r="A21" s="72"/>
+      <c r="B21" s="132" t="s">
         <v>322</v>
       </c>
-      <c r="C21" s="77"/>
+      <c r="C21" s="133"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="76" t="s">
+      <c r="E21" s="132" t="s">
         <v>325</v>
       </c>
-      <c r="F21" s="77"/>
+      <c r="F21" s="133"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="76" t="s">
+      <c r="H21" s="132" t="s">
         <v>323</v>
       </c>
-      <c r="I21" s="77"/>
+      <c r="I21" s="133"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="76" t="s">
+      <c r="K21" s="132" t="s">
         <v>325</v>
       </c>
-      <c r="L21" s="77"/>
+      <c r="L21" s="133"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="76" t="s">
+      <c r="N21" s="132" t="s">
         <v>329</v>
       </c>
-      <c r="O21" s="77"/>
+      <c r="O21" s="133"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="76" t="s">
+      <c r="Q21" s="132" t="s">
         <v>314</v>
       </c>
-      <c r="R21" s="77"/>
+      <c r="R21" s="133"/>
       <c r="S21" s="4"/>
-      <c r="T21" s="162" t="s">
-        <v>350</v>
-      </c>
-      <c r="U21" s="163"/>
-      <c r="V21" s="164"/>
-      <c r="W21" s="109"/>
-    </row>
-    <row r="22" spans="1:29">
-      <c r="A22" s="110" t="s">
+      <c r="T21" s="163" t="s">
+        <v>349</v>
+      </c>
+      <c r="U21" s="164"/>
+      <c r="V21" s="165"/>
+      <c r="W21" s="73"/>
+    </row>
+    <row r="22" spans="1:32" ht="16" thickBot="1">
+      <c r="A22" s="74" t="s">
         <v>302</v>
       </c>
-      <c r="B22" s="78"/>
-      <c r="C22" s="79"/>
-      <c r="D22" s="94"/>
-      <c r="E22" s="78"/>
-      <c r="F22" s="79"/>
-      <c r="G22" s="94"/>
-      <c r="H22" s="78"/>
-      <c r="I22" s="79"/>
-      <c r="J22" s="94"/>
-      <c r="K22" s="78"/>
-      <c r="L22" s="79"/>
-      <c r="M22" s="94"/>
-      <c r="N22" s="78"/>
-      <c r="O22" s="79"/>
-      <c r="P22" s="94"/>
-      <c r="Q22" s="78"/>
-      <c r="R22" s="79"/>
-      <c r="S22" s="94"/>
-      <c r="T22" s="165"/>
-      <c r="U22" s="166"/>
-      <c r="V22" s="167"/>
-      <c r="W22" s="109"/>
-    </row>
-    <row r="23" spans="1:29">
-      <c r="A23" s="108"/>
+      <c r="B22" s="136"/>
+      <c r="C22" s="137"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="136"/>
+      <c r="F22" s="137"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="136"/>
+      <c r="I22" s="137"/>
+      <c r="J22" s="69"/>
+      <c r="K22" s="136"/>
+      <c r="L22" s="137"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="136"/>
+      <c r="O22" s="137"/>
+      <c r="P22" s="69"/>
+      <c r="Q22" s="136"/>
+      <c r="R22" s="137"/>
+      <c r="S22" s="69"/>
+      <c r="T22" s="166"/>
+      <c r="U22" s="167"/>
+      <c r="V22" s="168"/>
+      <c r="W22" s="73"/>
+    </row>
+    <row r="23" spans="1:32">
+      <c r="A23" s="72"/>
       <c r="B23" s="38"/>
       <c r="C23" s="38"/>
       <c r="D23" s="4"/>
@@ -11677,25 +11777,35 @@
       <c r="T23" s="4"/>
       <c r="U23" s="4"/>
       <c r="V23" s="4"/>
-      <c r="W23" s="109"/>
-    </row>
-    <row r="24" spans="1:29" ht="15" customHeight="1">
-      <c r="A24" s="108"/>
-      <c r="B24" s="95" t="s">
+      <c r="W23" s="73"/>
+      <c r="Y23" s="184" t="s">
+        <v>374</v>
+      </c>
+      <c r="Z23" s="176"/>
+      <c r="AA23" s="176"/>
+      <c r="AB23" s="176"/>
+      <c r="AC23" s="176"/>
+      <c r="AD23" s="176"/>
+      <c r="AE23" s="176"/>
+      <c r="AF23" s="177"/>
+    </row>
+    <row r="24" spans="1:32" ht="15" customHeight="1">
+      <c r="A24" s="72"/>
+      <c r="B24" s="129" t="s">
         <v>315</v>
       </c>
-      <c r="C24" s="96"/>
+      <c r="C24" s="130"/>
       <c r="D24" s="38"/>
-      <c r="E24" s="95"/>
-      <c r="F24" s="96"/>
-      <c r="G24" s="94"/>
-      <c r="H24" s="95" t="s">
+      <c r="E24" s="129"/>
+      <c r="F24" s="130"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="129" t="s">
         <v>315</v>
       </c>
-      <c r="I24" s="96"/>
-      <c r="J24" s="94"/>
-      <c r="K24" s="95"/>
-      <c r="L24" s="96"/>
+      <c r="I24" s="130"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="129"/>
+      <c r="L24" s="130"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -11706,10 +11816,18 @@
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
       <c r="V24" s="4"/>
-      <c r="W24" s="109"/>
-    </row>
-    <row r="25" spans="1:29">
-      <c r="A25" s="108"/>
+      <c r="W24" s="73"/>
+      <c r="Y24" s="188"/>
+      <c r="Z24" s="179"/>
+      <c r="AA24" s="179"/>
+      <c r="AB24" s="179"/>
+      <c r="AC24" s="179"/>
+      <c r="AD24" s="179"/>
+      <c r="AE24" s="179"/>
+      <c r="AF24" s="180"/>
+    </row>
+    <row r="25" spans="1:32">
+      <c r="A25" s="72"/>
       <c r="B25" s="38"/>
       <c r="C25" s="38"/>
       <c r="D25" s="4"/>
@@ -11731,28 +11849,38 @@
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
-      <c r="W25" s="109"/>
-    </row>
-    <row r="26" spans="1:29">
-      <c r="A26" s="108"/>
-      <c r="B26" s="95" t="s">
+      <c r="W25" s="73"/>
+      <c r="Y25" s="188" t="s">
+        <v>375</v>
+      </c>
+      <c r="Z25" s="179"/>
+      <c r="AA25" s="179"/>
+      <c r="AB25" s="179"/>
+      <c r="AC25" s="179"/>
+      <c r="AD25" s="179"/>
+      <c r="AE25" s="179"/>
+      <c r="AF25" s="180"/>
+    </row>
+    <row r="26" spans="1:32">
+      <c r="A26" s="72"/>
+      <c r="B26" s="129" t="s">
         <v>316</v>
       </c>
-      <c r="C26" s="96"/>
+      <c r="C26" s="130"/>
       <c r="D26" s="38"/>
-      <c r="E26" s="95" t="s">
+      <c r="E26" s="129" t="s">
         <v>324</v>
       </c>
-      <c r="F26" s="96"/>
-      <c r="G26" s="94"/>
-      <c r="H26" s="95" t="s">
+      <c r="F26" s="130"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="129" t="s">
         <v>316</v>
       </c>
-      <c r="I26" s="96"/>
-      <c r="J26" s="94"/>
-      <c r="K26" s="95"/>
-      <c r="L26" s="96"/>
-      <c r="M26" s="114"/>
+      <c r="I26" s="130"/>
+      <c r="J26" s="69"/>
+      <c r="K26" s="129"/>
+      <c r="L26" s="130"/>
+      <c r="M26" s="78"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
@@ -11762,10 +11890,20 @@
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
       <c r="V26" s="4"/>
-      <c r="W26" s="109"/>
-    </row>
-    <row r="27" spans="1:29">
-      <c r="A27" s="108"/>
+      <c r="W26" s="73"/>
+      <c r="Y26" s="188" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z26" s="179"/>
+      <c r="AA26" s="179"/>
+      <c r="AB26" s="179"/>
+      <c r="AC26" s="179"/>
+      <c r="AD26" s="179"/>
+      <c r="AE26" s="179"/>
+      <c r="AF26" s="180"/>
+    </row>
+    <row r="27" spans="1:32">
+      <c r="A27" s="72"/>
       <c r="B27" s="38"/>
       <c r="C27" s="38"/>
       <c r="D27" s="4"/>
@@ -11787,25 +11925,35 @@
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
-      <c r="W27" s="109"/>
-    </row>
-    <row r="28" spans="1:29">
-      <c r="A28" s="108"/>
-      <c r="B28" s="95" t="s">
+      <c r="W27" s="73"/>
+      <c r="Y27" s="188" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z27" s="179"/>
+      <c r="AA27" s="179"/>
+      <c r="AB27" s="179"/>
+      <c r="AC27" s="179"/>
+      <c r="AD27" s="179"/>
+      <c r="AE27" s="179"/>
+      <c r="AF27" s="180"/>
+    </row>
+    <row r="28" spans="1:32">
+      <c r="A28" s="72"/>
+      <c r="B28" s="129" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="96"/>
+      <c r="C28" s="130"/>
       <c r="D28" s="38"/>
-      <c r="E28" s="95"/>
-      <c r="F28" s="96"/>
-      <c r="G28" s="94"/>
-      <c r="H28" s="95" t="s">
+      <c r="E28" s="129"/>
+      <c r="F28" s="130"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="129" t="s">
         <v>317</v>
       </c>
-      <c r="I28" s="96"/>
-      <c r="J28" s="94"/>
-      <c r="K28" s="95"/>
-      <c r="L28" s="96"/>
+      <c r="I28" s="130"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="129"/>
+      <c r="L28" s="130"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -11816,10 +11964,20 @@
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
       <c r="V28" s="4"/>
-      <c r="W28" s="109"/>
-    </row>
-    <row r="29" spans="1:29">
-      <c r="A29" s="108"/>
+      <c r="W28" s="73"/>
+      <c r="Y28" s="188" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z28" s="179"/>
+      <c r="AA28" s="179"/>
+      <c r="AB28" s="179"/>
+      <c r="AC28" s="179"/>
+      <c r="AD28" s="179"/>
+      <c r="AE28" s="179"/>
+      <c r="AF28" s="180"/>
+    </row>
+    <row r="29" spans="1:32">
+      <c r="A29" s="72"/>
       <c r="B29" s="38"/>
       <c r="C29" s="38"/>
       <c r="D29" s="4"/>
@@ -11841,29 +11999,39 @@
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
       <c r="V29" s="4"/>
-      <c r="W29" s="109"/>
-    </row>
-    <row r="30" spans="1:29">
-      <c r="A30" s="108"/>
-      <c r="B30" s="95" t="s">
+      <c r="W29" s="73"/>
+      <c r="Y29" s="188" t="s">
+        <v>380</v>
+      </c>
+      <c r="Z29" s="179"/>
+      <c r="AA29" s="179"/>
+      <c r="AB29" s="179"/>
+      <c r="AC29" s="179"/>
+      <c r="AD29" s="179"/>
+      <c r="AE29" s="179"/>
+      <c r="AF29" s="180"/>
+    </row>
+    <row r="30" spans="1:32">
+      <c r="A30" s="72"/>
+      <c r="B30" s="129" t="s">
         <v>318</v>
       </c>
-      <c r="C30" s="96"/>
+      <c r="C30" s="130"/>
       <c r="D30" s="38"/>
-      <c r="E30" s="95" t="s">
+      <c r="E30" s="129" t="s">
         <v>326</v>
       </c>
-      <c r="F30" s="96"/>
-      <c r="G30" s="94"/>
-      <c r="H30" s="95" t="s">
+      <c r="F30" s="130"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="129" t="s">
         <v>331</v>
       </c>
-      <c r="I30" s="96"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="95" t="s">
+      <c r="I30" s="130"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="129" t="s">
         <v>330</v>
       </c>
-      <c r="L30" s="96"/>
+      <c r="L30" s="130"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
@@ -11874,10 +12042,20 @@
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
       <c r="V30" s="4"/>
-      <c r="W30" s="109"/>
-    </row>
-    <row r="31" spans="1:29">
-      <c r="A31" s="108"/>
+      <c r="W30" s="73"/>
+      <c r="Y30" s="188" t="s">
+        <v>379</v>
+      </c>
+      <c r="Z30" s="179"/>
+      <c r="AA30" s="179"/>
+      <c r="AB30" s="179"/>
+      <c r="AC30" s="179"/>
+      <c r="AD30" s="179"/>
+      <c r="AE30" s="179"/>
+      <c r="AF30" s="180"/>
+    </row>
+    <row r="31" spans="1:32">
+      <c r="A31" s="72"/>
       <c r="B31" s="38"/>
       <c r="C31" s="38"/>
       <c r="D31" s="4"/>
@@ -11899,27 +12077,35 @@
       <c r="T31" s="4"/>
       <c r="U31" s="4"/>
       <c r="V31" s="4"/>
-      <c r="W31" s="109"/>
-    </row>
-    <row r="32" spans="1:29">
-      <c r="A32" s="108"/>
-      <c r="B32" s="97" t="s">
+      <c r="W31" s="73"/>
+      <c r="Y31" s="178"/>
+      <c r="Z31" s="179"/>
+      <c r="AA31" s="179"/>
+      <c r="AB31" s="179"/>
+      <c r="AC31" s="179"/>
+      <c r="AD31" s="179"/>
+      <c r="AE31" s="179"/>
+      <c r="AF31" s="180"/>
+    </row>
+    <row r="32" spans="1:32">
+      <c r="A32" s="72"/>
+      <c r="B32" s="157" t="s">
         <v>320</v>
       </c>
-      <c r="C32" s="98"/>
+      <c r="C32" s="158"/>
       <c r="D32" s="38"/>
-      <c r="E32" s="97" t="s">
+      <c r="E32" s="157" t="s">
         <v>327</v>
       </c>
-      <c r="F32" s="98"/>
-      <c r="G32" s="94"/>
-      <c r="H32" s="97" t="s">
+      <c r="F32" s="158"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="157" t="s">
         <v>320</v>
       </c>
-      <c r="I32" s="98"/>
-      <c r="J32" s="94"/>
-      <c r="K32" s="97"/>
-      <c r="L32" s="98"/>
+      <c r="I32" s="158"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="157"/>
+      <c r="L32" s="158"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
@@ -11930,21 +12116,29 @@
       <c r="T32" s="4"/>
       <c r="U32" s="4"/>
       <c r="V32" s="4"/>
-      <c r="W32" s="109"/>
-    </row>
-    <row r="33" spans="1:29">
-      <c r="A33" s="108"/>
-      <c r="B33" s="115"/>
-      <c r="C33" s="115"/>
+      <c r="W32" s="73"/>
+      <c r="Y32" s="178"/>
+      <c r="Z32" s="179"/>
+      <c r="AA32" s="179"/>
+      <c r="AB32" s="179"/>
+      <c r="AC32" s="179"/>
+      <c r="AD32" s="179"/>
+      <c r="AE32" s="179"/>
+      <c r="AF32" s="180"/>
+    </row>
+    <row r="33" spans="1:32">
+      <c r="A33" s="72"/>
+      <c r="B33" s="79"/>
+      <c r="C33" s="79"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="115"/>
-      <c r="F33" s="115"/>
+      <c r="E33" s="79"/>
+      <c r="F33" s="79"/>
       <c r="G33" s="4"/>
-      <c r="H33" s="115"/>
-      <c r="I33" s="115"/>
+      <c r="H33" s="79"/>
+      <c r="I33" s="79"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="115"/>
-      <c r="L33" s="115"/>
+      <c r="K33" s="79"/>
+      <c r="L33" s="79"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
@@ -11955,27 +12149,35 @@
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
-      <c r="W33" s="109"/>
-    </row>
-    <row r="34" spans="1:29">
-      <c r="A34" s="108"/>
-      <c r="B34" s="95" t="s">
+      <c r="W33" s="73"/>
+      <c r="Y33" s="178"/>
+      <c r="Z33" s="179"/>
+      <c r="AA33" s="179"/>
+      <c r="AB33" s="179"/>
+      <c r="AC33" s="179"/>
+      <c r="AD33" s="179"/>
+      <c r="AE33" s="179"/>
+      <c r="AF33" s="180"/>
+    </row>
+    <row r="34" spans="1:32" ht="16" thickBot="1">
+      <c r="A34" s="72"/>
+      <c r="B34" s="129" t="s">
         <v>319</v>
       </c>
-      <c r="C34" s="96"/>
-      <c r="D34" s="94"/>
-      <c r="E34" s="95" t="s">
+      <c r="C34" s="130"/>
+      <c r="D34" s="69"/>
+      <c r="E34" s="129" t="s">
         <v>328</v>
       </c>
-      <c r="F34" s="96"/>
-      <c r="G34" s="94"/>
-      <c r="H34" s="95" t="s">
+      <c r="F34" s="130"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="129" t="s">
         <v>321</v>
       </c>
-      <c r="I34" s="96"/>
-      <c r="J34" s="94"/>
-      <c r="K34" s="95"/>
-      <c r="L34" s="96"/>
+      <c r="I34" s="130"/>
+      <c r="J34" s="69"/>
+      <c r="K34" s="129"/>
+      <c r="L34" s="130"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
@@ -11986,21 +12188,29 @@
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
       <c r="V34" s="4"/>
-      <c r="W34" s="109"/>
-    </row>
-    <row r="35" spans="1:29">
-      <c r="A35" s="108"/>
-      <c r="B35" s="115"/>
-      <c r="C35" s="115"/>
+      <c r="W34" s="73"/>
+      <c r="Y34" s="181"/>
+      <c r="Z34" s="182"/>
+      <c r="AA34" s="182"/>
+      <c r="AB34" s="182"/>
+      <c r="AC34" s="182"/>
+      <c r="AD34" s="182"/>
+      <c r="AE34" s="182"/>
+      <c r="AF34" s="183"/>
+    </row>
+    <row r="35" spans="1:32">
+      <c r="A35" s="72"/>
+      <c r="B35" s="79"/>
+      <c r="C35" s="79"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="115"/>
-      <c r="F35" s="115"/>
+      <c r="E35" s="79"/>
+      <c r="F35" s="79"/>
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
-      <c r="K35" s="115"/>
-      <c r="L35" s="115"/>
+      <c r="K35" s="79"/>
+      <c r="L35" s="79"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
       <c r="O35" s="4"/>
@@ -12011,25 +12221,25 @@
       <c r="T35" s="4"/>
       <c r="U35" s="4"/>
       <c r="V35" s="4"/>
-      <c r="W35" s="109"/>
-    </row>
-    <row r="36" spans="1:29">
-      <c r="A36" s="108"/>
+      <c r="W35" s="73"/>
+    </row>
+    <row r="36" spans="1:32">
+      <c r="A36" s="72"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="80" t="s">
-        <v>364</v>
-      </c>
-      <c r="F36" s="81"/>
+      <c r="E36" s="95" t="s">
+        <v>363</v>
+      </c>
+      <c r="F36" s="96"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
-      <c r="K36" s="80" t="s">
-        <v>364</v>
-      </c>
-      <c r="L36" s="81"/>
+      <c r="K36" s="95" t="s">
+        <v>363</v>
+      </c>
+      <c r="L36" s="96"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
@@ -12040,99 +12250,99 @@
       <c r="T36" s="4"/>
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
-      <c r="W36" s="109"/>
-    </row>
-    <row r="37" spans="1:29" ht="15" customHeight="1">
-      <c r="A37" s="116" t="s">
+      <c r="W36" s="73"/>
+    </row>
+    <row r="37" spans="1:32" ht="15" customHeight="1">
+      <c r="A37" s="80" t="s">
         <v>303</v>
       </c>
-      <c r="B37" s="123" t="s">
-        <v>363</v>
-      </c>
-      <c r="C37" s="124"/>
-      <c r="D37" s="117"/>
-      <c r="E37" s="90"/>
-      <c r="F37" s="91"/>
-      <c r="G37" s="117"/>
-      <c r="H37" s="123" t="s">
-        <v>363</v>
-      </c>
-      <c r="I37" s="124"/>
-      <c r="J37" s="117"/>
-      <c r="K37" s="90"/>
-      <c r="L37" s="91"/>
-      <c r="M37" s="117"/>
-      <c r="N37" s="117"/>
-      <c r="O37" s="117"/>
-      <c r="P37" s="117"/>
-      <c r="Q37" s="117"/>
-      <c r="R37" s="117"/>
-      <c r="S37" s="117"/>
-      <c r="T37" s="117"/>
-      <c r="U37" s="117"/>
-      <c r="V37" s="117"/>
-      <c r="W37" s="109"/>
-    </row>
-    <row r="38" spans="1:29" ht="15" customHeight="1" thickBot="1">
-      <c r="A38" s="111"/>
-      <c r="B38" s="112"/>
-      <c r="C38" s="112"/>
-      <c r="D38" s="112"/>
-      <c r="E38" s="153"/>
-      <c r="F38" s="154"/>
-      <c r="G38" s="112"/>
-      <c r="H38" s="112"/>
-      <c r="I38" s="112"/>
-      <c r="J38" s="112"/>
-      <c r="K38" s="153"/>
-      <c r="L38" s="154"/>
-      <c r="M38" s="112"/>
-      <c r="N38" s="112"/>
-      <c r="O38" s="112"/>
-      <c r="P38" s="112"/>
-      <c r="Q38" s="112"/>
-      <c r="R38" s="112"/>
-      <c r="S38" s="112"/>
-      <c r="T38" s="112"/>
-      <c r="U38" s="112"/>
-      <c r="V38" s="112"/>
-      <c r="W38" s="113"/>
-    </row>
-    <row r="39" spans="1:29">
-      <c r="A39" s="104" t="s">
+      <c r="B37" s="93" t="s">
+        <v>362</v>
+      </c>
+      <c r="C37" s="94"/>
+      <c r="D37" s="81"/>
+      <c r="E37" s="97"/>
+      <c r="F37" s="98"/>
+      <c r="G37" s="81"/>
+      <c r="H37" s="93" t="s">
+        <v>362</v>
+      </c>
+      <c r="I37" s="94"/>
+      <c r="J37" s="81"/>
+      <c r="K37" s="97"/>
+      <c r="L37" s="98"/>
+      <c r="M37" s="81"/>
+      <c r="N37" s="81"/>
+      <c r="O37" s="81"/>
+      <c r="P37" s="81"/>
+      <c r="Q37" s="81"/>
+      <c r="R37" s="81"/>
+      <c r="S37" s="81"/>
+      <c r="T37" s="81"/>
+      <c r="U37" s="81"/>
+      <c r="V37" s="81"/>
+      <c r="W37" s="73"/>
+    </row>
+    <row r="38" spans="1:32" ht="15" customHeight="1" thickBot="1">
+      <c r="A38" s="75"/>
+      <c r="B38" s="76"/>
+      <c r="C38" s="76"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="99"/>
+      <c r="F38" s="100"/>
+      <c r="G38" s="76"/>
+      <c r="H38" s="76"/>
+      <c r="I38" s="76"/>
+      <c r="J38" s="76"/>
+      <c r="K38" s="99"/>
+      <c r="L38" s="100"/>
+      <c r="M38" s="76"/>
+      <c r="N38" s="76"/>
+      <c r="O38" s="76"/>
+      <c r="P38" s="76"/>
+      <c r="Q38" s="76"/>
+      <c r="R38" s="76"/>
+      <c r="S38" s="76"/>
+      <c r="T38" s="76"/>
+      <c r="U38" s="76"/>
+      <c r="V38" s="76"/>
+      <c r="W38" s="77"/>
+    </row>
+    <row r="39" spans="1:32">
+      <c r="A39" s="141" t="s">
         <v>332</v>
       </c>
-      <c r="B39" s="105"/>
-      <c r="C39" s="105"/>
-      <c r="D39" s="106"/>
-      <c r="E39" s="106"/>
-      <c r="F39" s="106"/>
-      <c r="G39" s="106"/>
-      <c r="H39" s="106"/>
-      <c r="I39" s="106"/>
-      <c r="J39" s="106"/>
-      <c r="K39" s="106"/>
-      <c r="L39" s="106"/>
-      <c r="M39" s="106"/>
-      <c r="N39" s="106"/>
-      <c r="O39" s="106"/>
-      <c r="P39" s="106"/>
-      <c r="Q39" s="106"/>
-      <c r="R39" s="106"/>
-      <c r="S39" s="106"/>
-      <c r="T39" s="106"/>
-      <c r="U39" s="106"/>
-      <c r="V39" s="106"/>
-      <c r="W39" s="106"/>
-      <c r="X39" s="106"/>
-      <c r="Y39" s="106"/>
-      <c r="Z39" s="106"/>
-      <c r="AA39" s="106"/>
-      <c r="AB39" s="106"/>
-      <c r="AC39" s="107"/>
-    </row>
-    <row r="40" spans="1:29">
-      <c r="A40" s="108"/>
+      <c r="B39" s="142"/>
+      <c r="C39" s="142"/>
+      <c r="D39" s="70"/>
+      <c r="E39" s="70"/>
+      <c r="F39" s="70"/>
+      <c r="G39" s="70"/>
+      <c r="H39" s="70"/>
+      <c r="I39" s="70"/>
+      <c r="J39" s="70"/>
+      <c r="K39" s="70"/>
+      <c r="L39" s="70"/>
+      <c r="M39" s="70"/>
+      <c r="N39" s="70"/>
+      <c r="O39" s="70"/>
+      <c r="P39" s="70"/>
+      <c r="Q39" s="70"/>
+      <c r="R39" s="70"/>
+      <c r="S39" s="70"/>
+      <c r="T39" s="70"/>
+      <c r="U39" s="70"/>
+      <c r="V39" s="70"/>
+      <c r="W39" s="70"/>
+      <c r="X39" s="70"/>
+      <c r="Y39" s="70"/>
+      <c r="Z39" s="70"/>
+      <c r="AA39" s="70"/>
+      <c r="AB39" s="70"/>
+      <c r="AC39" s="71"/>
+    </row>
+    <row r="40" spans="1:32">
+      <c r="A40" s="72"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -12160,104 +12370,104 @@
       <c r="Z40" s="4"/>
       <c r="AA40" s="4"/>
       <c r="AB40" s="4"/>
-      <c r="AC40" s="109"/>
-    </row>
-    <row r="41" spans="1:29" ht="15" customHeight="1">
-      <c r="A41" s="108"/>
-      <c r="B41" s="76" t="s">
+      <c r="AC40" s="73"/>
+    </row>
+    <row r="41" spans="1:32" ht="15" customHeight="1">
+      <c r="A41" s="72"/>
+      <c r="B41" s="132" t="s">
         <v>333</v>
       </c>
-      <c r="C41" s="77"/>
+      <c r="C41" s="133"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="76" t="s">
+      <c r="E41" s="132" t="s">
         <v>335</v>
       </c>
-      <c r="F41" s="77"/>
+      <c r="F41" s="133"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="76" t="s">
+      <c r="H41" s="132" t="s">
         <v>334</v>
       </c>
-      <c r="I41" s="77"/>
+      <c r="I41" s="133"/>
       <c r="J41" s="4"/>
-      <c r="K41" s="76" t="s">
+      <c r="K41" s="132" t="s">
         <v>340</v>
       </c>
-      <c r="L41" s="77"/>
+      <c r="L41" s="133"/>
       <c r="M41" s="4"/>
-      <c r="N41" s="76" t="s">
+      <c r="N41" s="132" t="s">
         <v>341</v>
       </c>
-      <c r="O41" s="77"/>
+      <c r="O41" s="133"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="168" t="s">
+      <c r="Q41" s="143" t="s">
+        <v>346</v>
+      </c>
+      <c r="R41" s="144"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="143" t="s">
         <v>347</v>
       </c>
-      <c r="R41" s="169"/>
-      <c r="S41" s="4"/>
-      <c r="T41" s="168" t="s">
+      <c r="U41" s="144"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="103" t="s">
         <v>348</v>
       </c>
-      <c r="U41" s="169"/>
-      <c r="V41" s="4"/>
-      <c r="W41" s="84" t="s">
-        <v>349</v>
-      </c>
-      <c r="X41" s="85"/>
+      <c r="X41" s="147"/>
       <c r="Y41" s="4"/>
-      <c r="Z41" s="156" t="s">
-        <v>366</v>
-      </c>
-      <c r="AA41" s="157"/>
+      <c r="Z41" s="150" t="s">
+        <v>365</v>
+      </c>
+      <c r="AA41" s="151"/>
       <c r="AB41" s="4"/>
     </row>
-    <row r="42" spans="1:29">
-      <c r="A42" s="110" t="s">
+    <row r="42" spans="1:32">
+      <c r="A42" s="74" t="s">
         <v>302</v>
       </c>
-      <c r="B42" s="78"/>
-      <c r="C42" s="79"/>
-      <c r="D42" s="94"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="79"/>
-      <c r="G42" s="94"/>
-      <c r="H42" s="78"/>
-      <c r="I42" s="79"/>
-      <c r="J42" s="94"/>
-      <c r="K42" s="121"/>
-      <c r="L42" s="122"/>
-      <c r="M42" s="94"/>
-      <c r="N42" s="121"/>
-      <c r="O42" s="122"/>
-      <c r="P42" s="94"/>
-      <c r="Q42" s="170"/>
-      <c r="R42" s="171"/>
-      <c r="S42" s="94"/>
-      <c r="T42" s="170"/>
-      <c r="U42" s="171"/>
-      <c r="V42" s="155" t="s">
-        <v>365</v>
-      </c>
-      <c r="W42" s="86"/>
-      <c r="X42" s="87"/>
-      <c r="Y42" s="94" t="s">
+      <c r="B42" s="136"/>
+      <c r="C42" s="137"/>
+      <c r="D42" s="69"/>
+      <c r="E42" s="136"/>
+      <c r="F42" s="137"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="136"/>
+      <c r="I42" s="137"/>
+      <c r="J42" s="69"/>
+      <c r="K42" s="134"/>
+      <c r="L42" s="135"/>
+      <c r="M42" s="69"/>
+      <c r="N42" s="134"/>
+      <c r="O42" s="135"/>
+      <c r="P42" s="69"/>
+      <c r="Q42" s="145"/>
+      <c r="R42" s="146"/>
+      <c r="S42" s="69"/>
+      <c r="T42" s="145"/>
+      <c r="U42" s="146"/>
+      <c r="V42" s="89" t="s">
+        <v>364</v>
+      </c>
+      <c r="W42" s="148"/>
+      <c r="X42" s="149"/>
+      <c r="Y42" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="Z42" s="158"/>
-      <c r="AA42" s="159"/>
-    </row>
-    <row r="43" spans="1:29" ht="16" customHeight="1">
-      <c r="A43" s="108"/>
-      <c r="E43" s="119"/>
-      <c r="F43" s="120"/>
+      <c r="Z42" s="152"/>
+      <c r="AA42" s="153"/>
+    </row>
+    <row r="43" spans="1:32" ht="16" customHeight="1">
+      <c r="A43" s="72"/>
+      <c r="E43" s="82"/>
+      <c r="F43" s="83"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="119"/>
-      <c r="I43" s="120"/>
+      <c r="H43" s="82"/>
+      <c r="I43" s="83"/>
       <c r="J43" s="4"/>
-      <c r="K43" s="78"/>
-      <c r="L43" s="79"/>
+      <c r="K43" s="136"/>
+      <c r="L43" s="137"/>
       <c r="M43" s="4"/>
-      <c r="N43" s="78"/>
-      <c r="O43" s="79"/>
+      <c r="N43" s="136"/>
+      <c r="O43" s="137"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
@@ -12265,20 +12475,20 @@
       <c r="T43" s="4"/>
       <c r="U43" s="4"/>
       <c r="V43" s="4"/>
-      <c r="Z43" s="160"/>
-      <c r="AA43" s="161"/>
-    </row>
-    <row r="44" spans="1:29" ht="15" customHeight="1">
-      <c r="A44" s="108"/>
-      <c r="E44" s="126" t="s">
+      <c r="Z43" s="154"/>
+      <c r="AA43" s="155"/>
+    </row>
+    <row r="44" spans="1:32" ht="15" customHeight="1">
+      <c r="A44" s="72"/>
+      <c r="E44" s="138" t="s">
         <v>345</v>
       </c>
-      <c r="F44" s="127"/>
+      <c r="F44" s="139"/>
       <c r="G44" s="38"/>
-      <c r="H44" s="95" t="s">
+      <c r="H44" s="129" t="s">
         <v>338</v>
       </c>
-      <c r="I44" s="96"/>
+      <c r="I44" s="130"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
@@ -12293,12 +12503,12 @@
       <c r="U44" s="4"/>
       <c r="V44" s="4"/>
     </row>
-    <row r="45" spans="1:29">
-      <c r="E45" s="119"/>
-      <c r="F45" s="120"/>
+    <row r="45" spans="1:32">
+      <c r="E45" s="82"/>
+      <c r="F45" s="83"/>
       <c r="G45" s="4"/>
-      <c r="H45" s="119"/>
-      <c r="I45" s="120"/>
+      <c r="H45" s="82"/>
+      <c r="I45" s="83"/>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
       <c r="S45" s="4"/>
@@ -12306,17 +12516,17 @@
       <c r="U45" s="4"/>
       <c r="V45" s="4"/>
     </row>
-    <row r="46" spans="1:29">
-      <c r="A46" s="108"/>
-      <c r="E46" s="95" t="s">
+    <row r="46" spans="1:32">
+      <c r="A46" s="72"/>
+      <c r="E46" s="129" t="s">
         <v>337</v>
       </c>
-      <c r="F46" s="118"/>
+      <c r="F46" s="131"/>
       <c r="G46" s="38"/>
-      <c r="H46" s="123" t="s">
+      <c r="H46" s="93" t="s">
         <v>342</v>
       </c>
-      <c r="I46" s="124"/>
+      <c r="I46" s="94"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
@@ -12331,13 +12541,13 @@
       <c r="U46" s="4"/>
       <c r="V46" s="4"/>
     </row>
-    <row r="47" spans="1:29">
-      <c r="A47" s="108"/>
-      <c r="E47" s="119"/>
-      <c r="F47" s="120"/>
+    <row r="47" spans="1:32">
+      <c r="A47" s="72"/>
+      <c r="E47" s="82"/>
+      <c r="F47" s="83"/>
       <c r="G47" s="4"/>
-      <c r="H47" s="119"/>
-      <c r="I47" s="120"/>
+      <c r="H47" s="82"/>
+      <c r="I47" s="83"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
       <c r="L47" s="4"/>
@@ -12352,17 +12562,17 @@
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
     </row>
-    <row r="48" spans="1:29">
-      <c r="A48" s="108"/>
-      <c r="E48" s="95" t="s">
+    <row r="48" spans="1:32">
+      <c r="A48" s="72"/>
+      <c r="E48" s="129" t="s">
         <v>336</v>
       </c>
-      <c r="F48" s="118"/>
+      <c r="F48" s="131"/>
       <c r="G48" s="38"/>
-      <c r="H48" s="95" t="s">
+      <c r="H48" s="129" t="s">
         <v>339</v>
       </c>
-      <c r="I48" s="118"/>
+      <c r="I48" s="131"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
@@ -12378,7 +12588,7 @@
       <c r="V48" s="4"/>
     </row>
     <row r="49" spans="1:29">
-      <c r="A49" s="108"/>
+      <c r="A49" s="72"/>
       <c r="E49" s="39"/>
       <c r="F49" s="41"/>
       <c r="G49" s="4"/>
@@ -12391,34 +12601,34 @@
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
-      <c r="Q49" s="80" t="s">
-        <v>369</v>
-      </c>
-      <c r="R49" s="88"/>
-      <c r="S49" s="88"/>
-      <c r="T49" s="88"/>
-      <c r="U49" s="88"/>
-      <c r="V49" s="88"/>
-      <c r="W49" s="88"/>
-      <c r="X49" s="88"/>
-      <c r="Y49" s="88"/>
-      <c r="Z49" s="88"/>
-      <c r="AA49" s="81"/>
+      <c r="Q49" s="95" t="s">
+        <v>368</v>
+      </c>
+      <c r="R49" s="124"/>
+      <c r="S49" s="124"/>
+      <c r="T49" s="124"/>
+      <c r="U49" s="124"/>
+      <c r="V49" s="124"/>
+      <c r="W49" s="124"/>
+      <c r="X49" s="124"/>
+      <c r="Y49" s="124"/>
+      <c r="Z49" s="124"/>
+      <c r="AA49" s="96"/>
     </row>
     <row r="50" spans="1:29">
-      <c r="A50" s="108"/>
+      <c r="A50" s="72"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="95" t="s">
+      <c r="E50" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="F50" s="118"/>
+      <c r="F50" s="131"/>
       <c r="G50" s="38"/>
-      <c r="H50" s="95" t="s">
+      <c r="H50" s="129" t="s">
         <v>344</v>
       </c>
-      <c r="I50" s="118"/>
+      <c r="I50" s="131"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
@@ -12426,121 +12636,121 @@
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
-      <c r="Q50" s="90"/>
-      <c r="R50" s="89"/>
-      <c r="S50" s="89"/>
-      <c r="T50" s="89"/>
-      <c r="U50" s="89"/>
-      <c r="V50" s="89"/>
-      <c r="W50" s="89"/>
-      <c r="X50" s="89"/>
-      <c r="Y50" s="89"/>
-      <c r="Z50" s="89"/>
-      <c r="AA50" s="91"/>
+      <c r="Q50" s="97"/>
+      <c r="R50" s="125"/>
+      <c r="S50" s="125"/>
+      <c r="T50" s="125"/>
+      <c r="U50" s="125"/>
+      <c r="V50" s="125"/>
+      <c r="W50" s="125"/>
+      <c r="X50" s="125"/>
+      <c r="Y50" s="125"/>
+      <c r="Z50" s="125"/>
+      <c r="AA50" s="98"/>
     </row>
     <row r="51" spans="1:29" ht="15" customHeight="1">
-      <c r="A51" s="108"/>
+      <c r="A51" s="72"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
-      <c r="H51" s="88" t="s">
+      <c r="H51" s="124" t="s">
         <v>343</v>
       </c>
-      <c r="I51" s="88"/>
-      <c r="J51" s="80" t="s">
-        <v>364</v>
-      </c>
-      <c r="K51" s="81"/>
+      <c r="I51" s="124"/>
+      <c r="J51" s="95" t="s">
+        <v>363</v>
+      </c>
+      <c r="K51" s="96"/>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
-      <c r="Q51" s="90"/>
-      <c r="R51" s="89"/>
-      <c r="S51" s="89"/>
-      <c r="T51" s="89"/>
-      <c r="U51" s="89"/>
-      <c r="V51" s="89"/>
-      <c r="W51" s="89"/>
-      <c r="X51" s="89"/>
-      <c r="Y51" s="89"/>
-      <c r="Z51" s="89"/>
-      <c r="AA51" s="91"/>
+      <c r="Q51" s="97"/>
+      <c r="R51" s="125"/>
+      <c r="S51" s="125"/>
+      <c r="T51" s="125"/>
+      <c r="U51" s="125"/>
+      <c r="V51" s="125"/>
+      <c r="W51" s="125"/>
+      <c r="X51" s="125"/>
+      <c r="Y51" s="125"/>
+      <c r="Z51" s="125"/>
+      <c r="AA51" s="98"/>
     </row>
     <row r="52" spans="1:29">
-      <c r="A52" s="116" t="s">
+      <c r="A52" s="80" t="s">
         <v>303</v>
       </c>
-      <c r="B52" s="117"/>
-      <c r="C52" s="117"/>
-      <c r="D52" s="117"/>
-      <c r="E52" s="117"/>
-      <c r="F52" s="117"/>
-      <c r="G52" s="117"/>
-      <c r="H52" s="89"/>
-      <c r="I52" s="89"/>
-      <c r="J52" s="90"/>
-      <c r="K52" s="91"/>
-      <c r="L52" s="117"/>
-      <c r="M52" s="117"/>
-      <c r="N52" s="117"/>
-      <c r="O52" s="117"/>
-      <c r="P52" s="117"/>
-      <c r="Q52" s="90"/>
-      <c r="R52" s="89"/>
-      <c r="S52" s="89"/>
-      <c r="T52" s="89"/>
-      <c r="U52" s="89"/>
-      <c r="V52" s="89"/>
-      <c r="W52" s="89"/>
-      <c r="X52" s="89"/>
-      <c r="Y52" s="89"/>
-      <c r="Z52" s="89"/>
-      <c r="AA52" s="91"/>
+      <c r="B52" s="81"/>
+      <c r="C52" s="81"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="81"/>
+      <c r="F52" s="81"/>
+      <c r="G52" s="81"/>
+      <c r="H52" s="125"/>
+      <c r="I52" s="125"/>
+      <c r="J52" s="97"/>
+      <c r="K52" s="98"/>
+      <c r="L52" s="81"/>
+      <c r="M52" s="81"/>
+      <c r="N52" s="81"/>
+      <c r="O52" s="81"/>
+      <c r="P52" s="81"/>
+      <c r="Q52" s="97"/>
+      <c r="R52" s="125"/>
+      <c r="S52" s="125"/>
+      <c r="T52" s="125"/>
+      <c r="U52" s="125"/>
+      <c r="V52" s="125"/>
+      <c r="W52" s="125"/>
+      <c r="X52" s="125"/>
+      <c r="Y52" s="125"/>
+      <c r="Z52" s="125"/>
+      <c r="AA52" s="98"/>
     </row>
     <row r="53" spans="1:29" ht="16" thickBot="1">
-      <c r="A53" s="108"/>
+      <c r="A53" s="72"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
-      <c r="H53" s="89"/>
-      <c r="I53" s="89"/>
-      <c r="J53" s="153"/>
-      <c r="K53" s="154"/>
+      <c r="H53" s="125"/>
+      <c r="I53" s="125"/>
+      <c r="J53" s="99"/>
+      <c r="K53" s="100"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
       <c r="P53" s="4"/>
-      <c r="Q53" s="90"/>
-      <c r="R53" s="89"/>
-      <c r="S53" s="89"/>
-      <c r="T53" s="89"/>
-      <c r="U53" s="89"/>
-      <c r="V53" s="89"/>
-      <c r="W53" s="89"/>
-      <c r="X53" s="89"/>
-      <c r="Y53" s="89"/>
-      <c r="Z53" s="89"/>
-      <c r="AA53" s="91"/>
+      <c r="Q53" s="97"/>
+      <c r="R53" s="125"/>
+      <c r="S53" s="125"/>
+      <c r="T53" s="125"/>
+      <c r="U53" s="125"/>
+      <c r="V53" s="125"/>
+      <c r="W53" s="125"/>
+      <c r="X53" s="125"/>
+      <c r="Y53" s="125"/>
+      <c r="Z53" s="125"/>
+      <c r="AA53" s="98"/>
     </row>
     <row r="54" spans="1:29">
-      <c r="A54" s="108"/>
+      <c r="A54" s="72"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
-      <c r="H54" s="89"/>
-      <c r="I54" s="89"/>
+      <c r="H54" s="125"/>
+      <c r="I54" s="125"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -12548,28 +12758,28 @@
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
       <c r="P54" s="4"/>
-      <c r="Q54" s="90"/>
-      <c r="R54" s="89"/>
-      <c r="S54" s="89"/>
-      <c r="T54" s="89"/>
-      <c r="U54" s="89"/>
-      <c r="V54" s="89"/>
-      <c r="W54" s="89"/>
-      <c r="X54" s="89"/>
-      <c r="Y54" s="89"/>
-      <c r="Z54" s="89"/>
-      <c r="AA54" s="91"/>
+      <c r="Q54" s="97"/>
+      <c r="R54" s="125"/>
+      <c r="S54" s="125"/>
+      <c r="T54" s="125"/>
+      <c r="U54" s="125"/>
+      <c r="V54" s="125"/>
+      <c r="W54" s="125"/>
+      <c r="X54" s="125"/>
+      <c r="Y54" s="125"/>
+      <c r="Z54" s="125"/>
+      <c r="AA54" s="98"/>
     </row>
     <row r="55" spans="1:29">
-      <c r="A55" s="108"/>
+      <c r="A55" s="72"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="89"/>
-      <c r="I55" s="89"/>
+      <c r="H55" s="125"/>
+      <c r="I55" s="125"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
@@ -12577,315 +12787,383 @@
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
       <c r="P55" s="4"/>
-      <c r="Q55" s="82"/>
-      <c r="R55" s="173"/>
-      <c r="S55" s="173"/>
-      <c r="T55" s="173"/>
-      <c r="U55" s="173"/>
-      <c r="V55" s="173"/>
-      <c r="W55" s="173"/>
-      <c r="X55" s="173"/>
-      <c r="Y55" s="173"/>
-      <c r="Z55" s="173"/>
-      <c r="AA55" s="83"/>
+      <c r="Q55" s="126"/>
+      <c r="R55" s="127"/>
+      <c r="S55" s="127"/>
+      <c r="T55" s="127"/>
+      <c r="U55" s="127"/>
+      <c r="V55" s="127"/>
+      <c r="W55" s="127"/>
+      <c r="X55" s="127"/>
+      <c r="Y55" s="127"/>
+      <c r="Z55" s="127"/>
+      <c r="AA55" s="128"/>
     </row>
     <row r="56" spans="1:29" ht="16" thickBot="1">
-      <c r="A56" s="111"/>
-      <c r="B56" s="112"/>
-      <c r="C56" s="112"/>
-      <c r="D56" s="112"/>
-      <c r="E56" s="112"/>
-      <c r="F56" s="112"/>
-      <c r="G56" s="112"/>
-      <c r="H56" s="125"/>
-      <c r="I56" s="125"/>
-      <c r="J56" s="112"/>
-      <c r="K56" s="112"/>
-      <c r="L56" s="112"/>
-      <c r="M56" s="112"/>
-      <c r="N56" s="112"/>
-      <c r="O56" s="112"/>
-      <c r="P56" s="112"/>
-      <c r="Q56" s="112"/>
-      <c r="R56" s="112"/>
-      <c r="S56" s="112"/>
-      <c r="T56" s="112"/>
-      <c r="U56" s="112"/>
-      <c r="V56" s="112"/>
-      <c r="W56" s="112"/>
-      <c r="X56" s="112"/>
-      <c r="Y56" s="112"/>
-      <c r="Z56" s="112"/>
-      <c r="AA56" s="112"/>
-      <c r="AB56" s="112"/>
-      <c r="AC56" s="113"/>
+      <c r="A56" s="75"/>
+      <c r="B56" s="76"/>
+      <c r="C56" s="76"/>
+      <c r="D56" s="76"/>
+      <c r="E56" s="76"/>
+      <c r="F56" s="76"/>
+      <c r="G56" s="76"/>
+      <c r="H56" s="140"/>
+      <c r="I56" s="140"/>
+      <c r="J56" s="76"/>
+      <c r="K56" s="76"/>
+      <c r="L56" s="76"/>
+      <c r="M56" s="76"/>
+      <c r="N56" s="76"/>
+      <c r="O56" s="76"/>
+      <c r="P56" s="76"/>
+      <c r="Q56" s="76"/>
+      <c r="R56" s="76"/>
+      <c r="S56" s="76"/>
+      <c r="T56" s="76"/>
+      <c r="U56" s="76"/>
+      <c r="V56" s="76"/>
+      <c r="W56" s="76"/>
+      <c r="X56" s="76"/>
+      <c r="Y56" s="76"/>
+      <c r="Z56" s="76"/>
+      <c r="AA56" s="76"/>
+      <c r="AB56" s="76"/>
+      <c r="AC56" s="77"/>
     </row>
     <row r="57" spans="1:29">
-      <c r="A57" s="104" t="s">
-        <v>370</v>
-      </c>
-      <c r="B57" s="105"/>
-      <c r="C57" s="105"/>
-      <c r="D57" s="106"/>
-      <c r="E57" s="106"/>
-      <c r="F57" s="106"/>
-      <c r="G57" s="106"/>
-      <c r="H57" s="106"/>
-      <c r="I57" s="106"/>
-      <c r="J57" s="106"/>
-      <c r="K57" s="106"/>
-      <c r="L57" s="106"/>
-      <c r="M57" s="106"/>
-      <c r="N57" s="106"/>
-      <c r="O57" s="106"/>
-      <c r="P57" s="106"/>
+      <c r="A57" s="141" t="s">
+        <v>369</v>
+      </c>
+      <c r="B57" s="142"/>
+      <c r="C57" s="142"/>
+      <c r="D57" s="70"/>
+      <c r="E57" s="70"/>
+      <c r="F57" s="70"/>
+      <c r="G57" s="70"/>
+      <c r="H57" s="70"/>
+      <c r="I57" s="70"/>
+      <c r="J57" s="70"/>
+      <c r="K57" s="70"/>
+      <c r="L57" s="70"/>
+      <c r="M57" s="70"/>
+      <c r="N57" s="70"/>
+      <c r="O57" s="70"/>
+      <c r="P57" s="70"/>
     </row>
     <row r="58" spans="1:29">
-      <c r="A58" s="108"/>
+      <c r="A58" s="72"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
     </row>
     <row r="59" spans="1:29" ht="15" customHeight="1">
-      <c r="A59" s="108"/>
-      <c r="B59" s="76" t="s">
+      <c r="A59" s="72"/>
+      <c r="B59" s="132" t="s">
         <v>311</v>
       </c>
-      <c r="C59" s="129"/>
+      <c r="C59" s="156"/>
     </row>
     <row r="60" spans="1:29">
-      <c r="A60" s="110" t="s">
+      <c r="A60" s="74" t="s">
         <v>302</v>
       </c>
-      <c r="B60" s="129"/>
-      <c r="C60" s="79"/>
+      <c r="B60" s="156"/>
+      <c r="C60" s="137"/>
     </row>
     <row r="61" spans="1:29">
       <c r="B61" s="38"/>
-      <c r="C61" s="130"/>
-      <c r="S61" s="144"/>
-      <c r="T61" s="144"/>
-      <c r="U61" s="144"/>
-      <c r="V61" s="144"/>
-      <c r="W61" s="144"/>
+      <c r="C61" s="84"/>
+      <c r="S61" s="87"/>
+      <c r="T61" s="87"/>
+      <c r="U61" s="87"/>
+      <c r="V61" s="87"/>
+      <c r="W61" s="87"/>
     </row>
     <row r="62" spans="1:29" ht="15" customHeight="1">
-      <c r="B62" s="76" t="s">
-        <v>352</v>
-      </c>
-      <c r="C62" s="77"/>
-      <c r="S62" s="144"/>
-      <c r="T62" s="144"/>
-      <c r="U62" s="144"/>
-      <c r="V62" s="144"/>
-      <c r="W62" s="144"/>
+      <c r="B62" s="132" t="s">
+        <v>351</v>
+      </c>
+      <c r="C62" s="133"/>
+      <c r="S62" s="87"/>
+      <c r="T62" s="87"/>
+      <c r="U62" s="87"/>
+      <c r="V62" s="87"/>
+      <c r="W62" s="87"/>
     </row>
     <row r="63" spans="1:29">
-      <c r="B63" s="78"/>
-      <c r="C63" s="79"/>
-      <c r="S63" s="144"/>
-      <c r="T63" s="147" t="s">
-        <v>355</v>
-      </c>
-      <c r="U63" s="147"/>
-      <c r="V63" s="147"/>
-      <c r="W63" s="147"/>
+      <c r="B63" s="136"/>
+      <c r="C63" s="137"/>
+      <c r="S63" s="87"/>
+      <c r="T63" s="88" t="s">
+        <v>354</v>
+      </c>
+      <c r="U63" s="88"/>
+      <c r="V63" s="88"/>
+      <c r="W63" s="88"/>
     </row>
     <row r="64" spans="1:29">
       <c r="B64" s="38"/>
-      <c r="C64" s="130"/>
-      <c r="E64" s="131"/>
-      <c r="F64" s="131"/>
-      <c r="G64" s="131"/>
-      <c r="H64" s="131"/>
-      <c r="I64" s="131"/>
-      <c r="J64" s="131"/>
-      <c r="K64" s="131"/>
-      <c r="L64" s="132"/>
-      <c r="S64" s="144"/>
-      <c r="T64" s="145" t="s">
-        <v>356</v>
-      </c>
-      <c r="U64" s="145"/>
-      <c r="V64" s="145"/>
-      <c r="W64" s="145"/>
+      <c r="C64" s="84"/>
+      <c r="E64" s="85"/>
+      <c r="F64" s="85"/>
+      <c r="G64" s="85"/>
+      <c r="H64" s="85"/>
+      <c r="I64" s="85"/>
+      <c r="J64" s="85"/>
+      <c r="K64" s="85"/>
+      <c r="L64" s="86"/>
+      <c r="S64" s="87"/>
+      <c r="T64" s="189" t="s">
+        <v>355</v>
+      </c>
+      <c r="U64" s="189"/>
+      <c r="V64" s="189"/>
+      <c r="W64" s="189"/>
     </row>
     <row r="65" spans="2:23" ht="15" customHeight="1">
-      <c r="B65" s="84" t="s">
-        <v>350</v>
-      </c>
-      <c r="C65" s="99"/>
+      <c r="B65" s="103" t="s">
+        <v>349</v>
+      </c>
+      <c r="C65" s="109"/>
       <c r="D65" s="52"/>
-      <c r="E65" s="72" t="s">
-        <v>353</v>
-      </c>
-      <c r="F65" s="133"/>
-      <c r="G65" s="133"/>
-      <c r="H65" s="133"/>
-      <c r="I65" s="133"/>
-      <c r="J65" s="133"/>
-      <c r="K65" s="133"/>
-      <c r="L65" s="73"/>
+      <c r="E65" s="111" t="s">
+        <v>352</v>
+      </c>
+      <c r="F65" s="112"/>
+      <c r="G65" s="112"/>
+      <c r="H65" s="112"/>
+      <c r="I65" s="112"/>
+      <c r="J65" s="112"/>
+      <c r="K65" s="112"/>
+      <c r="L65" s="113"/>
       <c r="M65" s="52"/>
       <c r="N65" s="52"/>
-      <c r="O65" s="135" t="s">
-        <v>354</v>
-      </c>
-      <c r="P65" s="136"/>
-      <c r="Q65" s="137"/>
-      <c r="S65" s="144"/>
-      <c r="T65" s="145" t="s">
-        <v>357</v>
-      </c>
-      <c r="U65" s="145"/>
-      <c r="V65" s="145"/>
-      <c r="W65" s="145"/>
+      <c r="O65" s="117" t="s">
+        <v>353</v>
+      </c>
+      <c r="P65" s="101"/>
+      <c r="Q65" s="118"/>
+      <c r="S65" s="87"/>
+      <c r="T65" s="189" t="s">
+        <v>356</v>
+      </c>
+      <c r="U65" s="189"/>
+      <c r="V65" s="189"/>
+      <c r="W65" s="189"/>
     </row>
     <row r="66" spans="2:23">
-      <c r="B66" s="101"/>
-      <c r="C66" s="102"/>
+      <c r="B66" s="107"/>
+      <c r="C66" s="110"/>
       <c r="D66" s="52"/>
-      <c r="E66" s="74"/>
-      <c r="F66" s="134"/>
-      <c r="G66" s="134"/>
-      <c r="H66" s="134"/>
-      <c r="I66" s="134"/>
-      <c r="J66" s="134"/>
-      <c r="K66" s="134"/>
-      <c r="L66" s="75"/>
+      <c r="E66" s="114"/>
+      <c r="F66" s="115"/>
+      <c r="G66" s="115"/>
+      <c r="H66" s="115"/>
+      <c r="I66" s="115"/>
+      <c r="J66" s="115"/>
+      <c r="K66" s="115"/>
+      <c r="L66" s="116"/>
       <c r="M66" s="52"/>
       <c r="N66" s="52"/>
-      <c r="O66" s="138"/>
-      <c r="P66" s="139"/>
-      <c r="Q66" s="140"/>
-      <c r="S66" s="144"/>
-      <c r="T66" s="146" t="s">
-        <v>358</v>
-      </c>
-      <c r="U66" s="146"/>
-      <c r="V66" s="146"/>
-      <c r="W66" s="146"/>
+      <c r="O66" s="119"/>
+      <c r="P66" s="102"/>
+      <c r="Q66" s="120"/>
+      <c r="S66" s="87"/>
+      <c r="T66" s="190" t="s">
+        <v>357</v>
+      </c>
+      <c r="U66" s="190"/>
+      <c r="V66" s="190"/>
+      <c r="W66" s="190"/>
     </row>
     <row r="67" spans="2:23">
       <c r="B67" s="38"/>
-      <c r="C67" s="130"/>
-      <c r="E67" s="131"/>
-      <c r="F67" s="131"/>
-      <c r="G67" s="131"/>
-      <c r="H67" s="131"/>
-      <c r="I67" s="131"/>
-      <c r="J67" s="131"/>
-      <c r="K67" s="131"/>
-      <c r="L67" s="132"/>
-      <c r="O67" s="141"/>
-      <c r="P67" s="142"/>
-      <c r="Q67" s="143"/>
-      <c r="S67" s="144"/>
-      <c r="T67" s="146"/>
-      <c r="U67" s="146"/>
-      <c r="V67" s="146"/>
-      <c r="W67" s="146"/>
+      <c r="C67" s="84"/>
+      <c r="E67" s="85"/>
+      <c r="F67" s="85"/>
+      <c r="G67" s="85"/>
+      <c r="H67" s="85"/>
+      <c r="I67" s="85"/>
+      <c r="J67" s="85"/>
+      <c r="K67" s="85"/>
+      <c r="L67" s="86"/>
+      <c r="O67" s="121"/>
+      <c r="P67" s="122"/>
+      <c r="Q67" s="123"/>
+      <c r="S67" s="87"/>
+      <c r="T67" s="190"/>
+      <c r="U67" s="190"/>
+      <c r="V67" s="190"/>
+      <c r="W67" s="190"/>
     </row>
     <row r="68" spans="2:23">
-      <c r="B68" s="84" t="s">
-        <v>351</v>
-      </c>
-      <c r="C68" s="100"/>
-      <c r="E68" s="131"/>
-      <c r="F68" s="131"/>
-      <c r="G68" s="131"/>
-      <c r="H68" s="131"/>
-      <c r="I68" s="131"/>
-      <c r="J68" s="131"/>
-      <c r="K68" s="131"/>
-      <c r="L68" s="132"/>
+      <c r="B68" s="103" t="s">
+        <v>350</v>
+      </c>
+      <c r="C68" s="104"/>
+      <c r="E68" s="85"/>
+      <c r="F68" s="85"/>
+      <c r="G68" s="85"/>
+      <c r="H68" s="85"/>
+      <c r="I68" s="85"/>
+      <c r="J68" s="85"/>
+      <c r="K68" s="85"/>
+      <c r="L68" s="86"/>
       <c r="P68" s="52"/>
-      <c r="S68" s="144"/>
-      <c r="T68" s="146"/>
-      <c r="U68" s="146"/>
-      <c r="V68" s="146"/>
-      <c r="W68" s="146"/>
+      <c r="S68" s="87"/>
+      <c r="T68" s="190"/>
+      <c r="U68" s="190"/>
+      <c r="V68" s="190"/>
+      <c r="W68" s="190"/>
     </row>
     <row r="69" spans="2:23" ht="15" customHeight="1">
-      <c r="B69" s="92"/>
-      <c r="C69" s="128"/>
-      <c r="E69" s="132"/>
-      <c r="F69" s="132"/>
-      <c r="G69" s="132"/>
-      <c r="H69" s="132"/>
-      <c r="I69" s="132"/>
-      <c r="J69" s="132"/>
-      <c r="K69" s="132"/>
-      <c r="L69" s="132"/>
-      <c r="O69" s="136" t="s">
+      <c r="B69" s="105"/>
+      <c r="C69" s="106"/>
+      <c r="E69" s="86"/>
+      <c r="F69" s="86"/>
+      <c r="G69" s="86"/>
+      <c r="H69" s="86"/>
+      <c r="I69" s="86"/>
+      <c r="J69" s="86"/>
+      <c r="K69" s="86"/>
+      <c r="L69" s="86"/>
+      <c r="O69" s="101" t="s">
+        <v>366</v>
+      </c>
+      <c r="P69" s="101"/>
+      <c r="Q69" s="101"/>
+      <c r="S69" s="87"/>
+      <c r="T69" s="190"/>
+      <c r="U69" s="190"/>
+      <c r="V69" s="190"/>
+      <c r="W69" s="190"/>
+    </row>
+    <row r="70" spans="2:23">
+      <c r="B70" s="107"/>
+      <c r="C70" s="108"/>
+      <c r="O70" s="102"/>
+      <c r="P70" s="102"/>
+      <c r="Q70" s="102"/>
+      <c r="S70" s="87"/>
+      <c r="T70" s="189" t="s">
+        <v>358</v>
+      </c>
+      <c r="U70" s="189"/>
+      <c r="V70" s="189"/>
+      <c r="W70" s="189"/>
+    </row>
+    <row r="71" spans="2:23">
+      <c r="O71" s="102"/>
+      <c r="P71" s="102"/>
+      <c r="Q71" s="102"/>
+      <c r="T71" s="189" t="s">
+        <v>359</v>
+      </c>
+      <c r="U71" s="189"/>
+      <c r="V71" s="189"/>
+      <c r="W71" s="189"/>
+    </row>
+    <row r="72" spans="2:23" ht="15" customHeight="1">
+      <c r="O72" s="102"/>
+      <c r="P72" s="102"/>
+      <c r="Q72" s="102"/>
+      <c r="T72" s="191" t="s">
         <v>367</v>
       </c>
-      <c r="P69" s="136"/>
-      <c r="Q69" s="136"/>
-      <c r="S69" s="144"/>
-      <c r="T69" s="146"/>
-      <c r="U69" s="146"/>
-      <c r="V69" s="146"/>
-      <c r="W69" s="146"/>
-    </row>
-    <row r="70" spans="2:23">
-      <c r="B70" s="101"/>
-      <c r="C70" s="103"/>
-      <c r="O70" s="139"/>
-      <c r="P70" s="139"/>
-      <c r="Q70" s="139"/>
-      <c r="S70" s="144"/>
-      <c r="T70" s="145" t="s">
-        <v>359</v>
-      </c>
-      <c r="U70" s="145"/>
-      <c r="V70" s="145"/>
-      <c r="W70" s="145"/>
-    </row>
-    <row r="71" spans="2:23">
-      <c r="O71" s="139"/>
-      <c r="P71" s="139"/>
-      <c r="Q71" s="139"/>
-      <c r="T71" s="145" t="s">
-        <v>360</v>
-      </c>
-      <c r="U71" s="145"/>
-      <c r="V71" s="145"/>
-      <c r="W71" s="145"/>
-    </row>
-    <row r="72" spans="2:23" ht="15" customHeight="1">
-      <c r="O72" s="139"/>
-      <c r="P72" s="139"/>
-      <c r="Q72" s="139"/>
-      <c r="T72" s="172" t="s">
-        <v>368</v>
-      </c>
-      <c r="U72" s="172"/>
-      <c r="V72" s="172"/>
-      <c r="W72" s="172"/>
+      <c r="U72" s="191"/>
+      <c r="V72" s="191"/>
+      <c r="W72" s="191"/>
     </row>
     <row r="73" spans="2:23">
-      <c r="O73" s="139"/>
-      <c r="P73" s="139"/>
-      <c r="Q73" s="139"/>
-      <c r="T73" s="148"/>
-      <c r="U73" s="148"/>
-      <c r="V73" s="148"/>
-      <c r="W73" s="148"/>
+      <c r="O73" s="102"/>
+      <c r="P73" s="102"/>
+      <c r="Q73" s="102"/>
+      <c r="T73" s="192"/>
+      <c r="U73" s="192"/>
+      <c r="V73" s="192"/>
+      <c r="W73" s="192"/>
     </row>
     <row r="74" spans="2:23">
-      <c r="T74" s="148"/>
-      <c r="U74" s="148"/>
-      <c r="V74" s="148"/>
-      <c r="W74" s="148"/>
+      <c r="T74" s="192"/>
+      <c r="U74" s="192"/>
+      <c r="V74" s="192"/>
+      <c r="W74" s="192"/>
     </row>
     <row r="75" spans="2:23">
-      <c r="T75" s="148"/>
-      <c r="U75" s="148"/>
-      <c r="V75" s="148"/>
-      <c r="W75" s="148"/>
+      <c r="T75" s="192"/>
+      <c r="U75" s="192"/>
+      <c r="V75" s="192"/>
+      <c r="W75" s="192"/>
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="T6:V17"/>
+    <mergeCell ref="T3:V4"/>
+    <mergeCell ref="AA3:AB4"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="N21:O22"/>
+    <mergeCell ref="T21:V22"/>
+    <mergeCell ref="Q21:R22"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="K3:L4"/>
+    <mergeCell ref="N3:O4"/>
+    <mergeCell ref="Q3:R4"/>
+    <mergeCell ref="Q6:R13"/>
+    <mergeCell ref="X3:Y4"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="K21:L22"/>
+    <mergeCell ref="E21:F22"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="T70:W70"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="B41:C42"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="H41:I42"/>
+    <mergeCell ref="B62:C63"/>
+    <mergeCell ref="W41:X42"/>
+    <mergeCell ref="T41:U42"/>
+    <mergeCell ref="Z41:AA43"/>
+    <mergeCell ref="B59:C60"/>
+    <mergeCell ref="T66:W69"/>
+    <mergeCell ref="H51:I56"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="Q41:R42"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="K41:L43"/>
+    <mergeCell ref="N41:O43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E46:F46"/>
     <mergeCell ref="T71:W71"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="E36:F38"/>
@@ -12902,74 +13180,6 @@
     <mergeCell ref="T64:W64"/>
     <mergeCell ref="T65:W65"/>
     <mergeCell ref="H44:I44"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="K41:L43"/>
-    <mergeCell ref="N41:O43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="H51:I56"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="Q41:R42"/>
-    <mergeCell ref="W41:X42"/>
-    <mergeCell ref="T41:U42"/>
-    <mergeCell ref="Z41:AA43"/>
-    <mergeCell ref="B59:C60"/>
-    <mergeCell ref="T66:W69"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="B41:C42"/>
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="H41:I42"/>
-    <mergeCell ref="B62:C63"/>
-    <mergeCell ref="T70:W70"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="K21:L22"/>
-    <mergeCell ref="E21:F22"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="AA3:AB4"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="N21:O22"/>
-    <mergeCell ref="T21:V22"/>
-    <mergeCell ref="Q21:R22"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="K3:L4"/>
-    <mergeCell ref="N3:O4"/>
-    <mergeCell ref="Q3:R4"/>
-    <mergeCell ref="Q6:R13"/>
-    <mergeCell ref="X3:Y4"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="E6:F7"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="T6:V17"/>
-    <mergeCell ref="T3:V4"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
More work on Yield re do
</commit_message>
<xml_diff>
--- a/Food_SR_Organization.xlsx
+++ b/Food_SR_Organization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35040" windowHeight="8760" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="8500" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="1.Food Need" sheetId="3" r:id="rId1"/>
@@ -1666,7 +1666,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="29">
+  <fills count="30">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1832,6 +1832,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2572,7 +2578,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2703,6 +2709,13 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2712,73 +2725,13 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2792,102 +2745,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2904,7 +2761,13 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2922,10 +2785,22 @@
     <xf numFmtId="0" fontId="8" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2949,16 +2824,149 @@
     <xf numFmtId="0" fontId="1" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="419">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -10254,7 +10262,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="110" t="s">
+      <c r="M14" s="117" t="s">
         <v>42</v>
       </c>
       <c r="N14" s="4"/>
@@ -10274,7 +10282,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="111"/>
+      <c r="M15" s="118"/>
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:26">
@@ -10292,7 +10300,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="111"/>
+      <c r="M16" s="118"/>
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14">
@@ -10310,7 +10318,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="22"/>
-      <c r="M17" s="111"/>
+      <c r="M17" s="118"/>
       <c r="N17" s="22"/>
     </row>
     <row r="18" spans="1:14">
@@ -10328,7 +10336,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="22"/>
-      <c r="M18" s="111"/>
+      <c r="M18" s="118"/>
       <c r="N18" s="22"/>
     </row>
     <row r="19" spans="1:14">
@@ -10346,7 +10354,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="22"/>
-      <c r="M19" s="111"/>
+      <c r="M19" s="118"/>
       <c r="N19" s="22"/>
     </row>
     <row r="20" spans="1:14">
@@ -10362,7 +10370,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="112"/>
+      <c r="M20" s="119"/>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:14">
@@ -11353,11 +11361,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="A1" s="113" t="s">
+      <c r="A1" s="172" t="s">
         <v>304</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="173"/>
+      <c r="C1" s="173"/>
       <c r="D1" s="70"/>
       <c r="E1" s="70"/>
       <c r="F1" s="70"/>
@@ -11418,84 +11426,84 @@
     </row>
     <row r="3" spans="1:29" ht="15" customHeight="1">
       <c r="A3" s="72"/>
-      <c r="B3" s="132" t="s">
+      <c r="B3" s="140" t="s">
         <v>299</v>
       </c>
-      <c r="C3" s="133"/>
+      <c r="C3" s="142"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="122" t="s">
+      <c r="E3" s="166" t="s">
         <v>300</v>
       </c>
-      <c r="F3" s="123"/>
+      <c r="F3" s="178"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="132" t="s">
+      <c r="H3" s="140" t="s">
         <v>305</v>
       </c>
-      <c r="I3" s="133"/>
+      <c r="I3" s="142"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="132" t="s">
+      <c r="K3" s="140" t="s">
         <v>306</v>
       </c>
-      <c r="L3" s="133"/>
+      <c r="L3" s="142"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="122" t="s">
+      <c r="N3" s="166" t="s">
         <v>307</v>
       </c>
-      <c r="O3" s="123"/>
+      <c r="O3" s="178"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="122" t="s">
+      <c r="Q3" s="166" t="s">
         <v>308</v>
       </c>
-      <c r="R3" s="123"/>
+      <c r="R3" s="178"/>
       <c r="S3" s="4"/>
-      <c r="T3" s="116" t="s">
+      <c r="T3" s="134" t="s">
         <v>310</v>
       </c>
-      <c r="U3" s="117"/>
-      <c r="V3" s="117"/>
+      <c r="U3" s="195"/>
+      <c r="V3" s="195"/>
       <c r="W3" s="4"/>
-      <c r="X3" s="118" t="s">
+      <c r="X3" s="196" t="s">
         <v>361</v>
       </c>
-      <c r="Y3" s="119"/>
+      <c r="Y3" s="197"/>
       <c r="Z3" s="4"/>
-      <c r="AA3" s="118" t="s">
+      <c r="AA3" s="196" t="s">
         <v>312</v>
       </c>
-      <c r="AB3" s="119"/>
+      <c r="AB3" s="197"/>
       <c r="AC3" s="73"/>
     </row>
     <row r="4" spans="1:29" ht="15" customHeight="1">
       <c r="A4" s="74" t="s">
         <v>302</v>
       </c>
-      <c r="B4" s="134"/>
-      <c r="C4" s="135"/>
+      <c r="B4" s="143"/>
+      <c r="C4" s="145"/>
       <c r="D4" s="69"/>
-      <c r="E4" s="124"/>
-      <c r="F4" s="125"/>
+      <c r="E4" s="181"/>
+      <c r="F4" s="168"/>
       <c r="G4" s="69"/>
-      <c r="H4" s="134"/>
-      <c r="I4" s="135"/>
+      <c r="H4" s="143"/>
+      <c r="I4" s="145"/>
       <c r="J4" s="69"/>
-      <c r="K4" s="134"/>
-      <c r="L4" s="135"/>
+      <c r="K4" s="143"/>
+      <c r="L4" s="145"/>
       <c r="M4" s="69"/>
-      <c r="N4" s="124"/>
-      <c r="O4" s="125"/>
+      <c r="N4" s="181"/>
+      <c r="O4" s="168"/>
       <c r="P4" s="69"/>
-      <c r="Q4" s="124"/>
-      <c r="R4" s="125"/>
+      <c r="Q4" s="181"/>
+      <c r="R4" s="168"/>
       <c r="S4" s="69"/>
-      <c r="T4" s="116"/>
-      <c r="U4" s="117"/>
-      <c r="V4" s="117"/>
+      <c r="T4" s="134"/>
+      <c r="U4" s="195"/>
+      <c r="V4" s="195"/>
       <c r="W4" s="69"/>
-      <c r="X4" s="120"/>
-      <c r="Y4" s="121"/>
+      <c r="X4" s="198"/>
+      <c r="Y4" s="199"/>
       <c r="Z4" s="69"/>
-      <c r="AA4" s="120"/>
-      <c r="AB4" s="121"/>
+      <c r="AA4" s="198"/>
+      <c r="AB4" s="199"/>
       <c r="AC4" s="73"/>
     </row>
     <row r="5" spans="1:29">
@@ -11534,10 +11542,10 @@
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="136" t="s">
+      <c r="E6" s="123" t="s">
         <v>301</v>
       </c>
-      <c r="F6" s="137"/>
+      <c r="F6" s="124"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -11548,16 +11556,16 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="136" t="s">
+      <c r="Q6" s="123" t="s">
         <v>309</v>
       </c>
-      <c r="R6" s="137"/>
+      <c r="R6" s="124"/>
       <c r="S6" s="4"/>
-      <c r="T6" s="115" t="s">
+      <c r="T6" s="154" t="s">
         <v>360</v>
       </c>
-      <c r="U6" s="115"/>
-      <c r="V6" s="115"/>
+      <c r="U6" s="154"/>
+      <c r="V6" s="154"/>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
@@ -11573,8 +11581,8 @@
       <c r="B7" s="69"/>
       <c r="C7" s="69"/>
       <c r="D7" s="69"/>
-      <c r="E7" s="140"/>
-      <c r="F7" s="141"/>
+      <c r="E7" s="155"/>
+      <c r="F7" s="157"/>
       <c r="G7" s="69"/>
       <c r="H7" s="69"/>
       <c r="I7" s="69"/>
@@ -11585,12 +11593,12 @@
       <c r="N7" s="69"/>
       <c r="O7" s="69"/>
       <c r="P7" s="69"/>
-      <c r="Q7" s="138"/>
-      <c r="R7" s="139"/>
+      <c r="Q7" s="125"/>
+      <c r="R7" s="126"/>
       <c r="S7" s="69"/>
-      <c r="T7" s="115"/>
-      <c r="U7" s="115"/>
-      <c r="V7" s="115"/>
+      <c r="T7" s="154"/>
+      <c r="U7" s="154"/>
+      <c r="V7" s="154"/>
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
@@ -11616,12 +11624,12 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="138"/>
-      <c r="R8" s="139"/>
+      <c r="Q8" s="125"/>
+      <c r="R8" s="126"/>
       <c r="S8" s="4"/>
-      <c r="T8" s="115"/>
-      <c r="U8" s="115"/>
-      <c r="V8" s="115"/>
+      <c r="T8" s="154"/>
+      <c r="U8" s="154"/>
+      <c r="V8" s="154"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
@@ -11649,12 +11657,12 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="138"/>
-      <c r="R9" s="139"/>
+      <c r="Q9" s="125"/>
+      <c r="R9" s="126"/>
       <c r="S9" s="4"/>
-      <c r="T9" s="115"/>
-      <c r="U9" s="115"/>
-      <c r="V9" s="115"/>
+      <c r="T9" s="154"/>
+      <c r="U9" s="154"/>
+      <c r="V9" s="154"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
@@ -11680,12 +11688,12 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="138"/>
-      <c r="R10" s="139"/>
+      <c r="Q10" s="125"/>
+      <c r="R10" s="126"/>
       <c r="S10" s="4"/>
-      <c r="T10" s="115"/>
-      <c r="U10" s="115"/>
-      <c r="V10" s="115"/>
+      <c r="T10" s="154"/>
+      <c r="U10" s="154"/>
+      <c r="V10" s="154"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
@@ -11713,12 +11721,12 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="138"/>
-      <c r="R11" s="139"/>
+      <c r="Q11" s="125"/>
+      <c r="R11" s="126"/>
       <c r="S11" s="4"/>
-      <c r="T11" s="115"/>
-      <c r="U11" s="115"/>
-      <c r="V11" s="115"/>
+      <c r="T11" s="154"/>
+      <c r="U11" s="154"/>
+      <c r="V11" s="154"/>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
@@ -11744,12 +11752,12 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="138"/>
-      <c r="R12" s="139"/>
+      <c r="Q12" s="125"/>
+      <c r="R12" s="126"/>
       <c r="S12" s="4"/>
-      <c r="T12" s="115"/>
-      <c r="U12" s="115"/>
-      <c r="V12" s="115"/>
+      <c r="T12" s="154"/>
+      <c r="U12" s="154"/>
+      <c r="V12" s="154"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
@@ -11777,12 +11785,12 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="140"/>
-      <c r="R13" s="141"/>
+      <c r="Q13" s="155"/>
+      <c r="R13" s="157"/>
       <c r="S13" s="4"/>
-      <c r="T13" s="115"/>
-      <c r="U13" s="115"/>
-      <c r="V13" s="115"/>
+      <c r="T13" s="154"/>
+      <c r="U13" s="154"/>
+      <c r="V13" s="154"/>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
@@ -11811,9 +11819,9 @@
       <c r="Q14" s="4"/>
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
-      <c r="T14" s="115"/>
-      <c r="U14" s="115"/>
-      <c r="V14" s="115"/>
+      <c r="T14" s="154"/>
+      <c r="U14" s="154"/>
+      <c r="V14" s="154"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
@@ -11844,9 +11852,9 @@
       <c r="Q15" s="4"/>
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
-      <c r="T15" s="115"/>
-      <c r="U15" s="115"/>
-      <c r="V15" s="115"/>
+      <c r="T15" s="154"/>
+      <c r="U15" s="154"/>
+      <c r="V15" s="154"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
@@ -11875,9 +11883,9 @@
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
-      <c r="T16" s="115"/>
-      <c r="U16" s="115"/>
-      <c r="V16" s="115"/>
+      <c r="T16" s="154"/>
+      <c r="U16" s="154"/>
+      <c r="V16" s="154"/>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
@@ -11906,9 +11914,9 @@
       <c r="Q17" s="4"/>
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
-      <c r="T17" s="115"/>
-      <c r="U17" s="115"/>
-      <c r="V17" s="115"/>
+      <c r="T17" s="154"/>
+      <c r="U17" s="154"/>
+      <c r="V17" s="154"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
@@ -11949,11 +11957,11 @@
       <c r="AC18" s="77"/>
     </row>
     <row r="19" spans="1:32">
-      <c r="A19" s="113" t="s">
+      <c r="A19" s="172" t="s">
         <v>313</v>
       </c>
-      <c r="B19" s="114"/>
-      <c r="C19" s="114"/>
+      <c r="B19" s="173"/>
+      <c r="C19" s="173"/>
       <c r="D19" s="70"/>
       <c r="E19" s="70"/>
       <c r="F19" s="70"/>
@@ -12008,68 +12016,68 @@
     </row>
     <row r="21" spans="1:32" ht="15" customHeight="1">
       <c r="A21" s="72"/>
-      <c r="B21" s="122" t="s">
+      <c r="B21" s="166" t="s">
         <v>322</v>
       </c>
-      <c r="C21" s="123"/>
+      <c r="C21" s="178"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="122" t="s">
+      <c r="E21" s="166" t="s">
         <v>325</v>
       </c>
-      <c r="F21" s="123"/>
+      <c r="F21" s="178"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="122" t="s">
+      <c r="H21" s="166" t="s">
         <v>323</v>
       </c>
-      <c r="I21" s="123"/>
+      <c r="I21" s="178"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="122" t="s">
+      <c r="K21" s="166" t="s">
         <v>325</v>
       </c>
-      <c r="L21" s="123"/>
+      <c r="L21" s="178"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="122" t="s">
+      <c r="N21" s="166" t="s">
         <v>329</v>
       </c>
-      <c r="O21" s="123"/>
+      <c r="O21" s="178"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="122" t="s">
+      <c r="Q21" s="166" t="s">
         <v>314</v>
       </c>
-      <c r="R21" s="123"/>
+      <c r="R21" s="178"/>
       <c r="S21" s="4"/>
-      <c r="T21" s="126" t="s">
+      <c r="T21" s="189" t="s">
         <v>349</v>
       </c>
-      <c r="U21" s="127"/>
-      <c r="V21" s="128"/>
+      <c r="U21" s="190"/>
+      <c r="V21" s="191"/>
       <c r="W21" s="73"/>
     </row>
     <row r="22" spans="1:32" ht="16" thickBot="1">
       <c r="A22" s="74" t="s">
         <v>302</v>
       </c>
-      <c r="B22" s="124"/>
-      <c r="C22" s="125"/>
+      <c r="B22" s="181"/>
+      <c r="C22" s="168"/>
       <c r="D22" s="69"/>
-      <c r="E22" s="124"/>
-      <c r="F22" s="125"/>
+      <c r="E22" s="181"/>
+      <c r="F22" s="168"/>
       <c r="G22" s="69"/>
-      <c r="H22" s="124"/>
-      <c r="I22" s="125"/>
+      <c r="H22" s="181"/>
+      <c r="I22" s="168"/>
       <c r="J22" s="69"/>
-      <c r="K22" s="124"/>
-      <c r="L22" s="125"/>
+      <c r="K22" s="181"/>
+      <c r="L22" s="168"/>
       <c r="M22" s="69"/>
-      <c r="N22" s="124"/>
-      <c r="O22" s="125"/>
+      <c r="N22" s="181"/>
+      <c r="O22" s="168"/>
       <c r="P22" s="69"/>
-      <c r="Q22" s="124"/>
-      <c r="R22" s="125"/>
+      <c r="Q22" s="181"/>
+      <c r="R22" s="168"/>
       <c r="S22" s="69"/>
-      <c r="T22" s="129"/>
-      <c r="U22" s="130"/>
-      <c r="V22" s="131"/>
+      <c r="T22" s="192"/>
+      <c r="U22" s="193"/>
+      <c r="V22" s="194"/>
       <c r="W22" s="73"/>
     </row>
     <row r="23" spans="1:32">
@@ -12109,21 +12117,21 @@
     </row>
     <row r="24" spans="1:32" ht="15" customHeight="1">
       <c r="A24" s="72"/>
-      <c r="B24" s="142" t="s">
+      <c r="B24" s="158" t="s">
         <v>315</v>
       </c>
-      <c r="C24" s="143"/>
+      <c r="C24" s="159"/>
       <c r="D24" s="38"/>
-      <c r="E24" s="142"/>
-      <c r="F24" s="143"/>
+      <c r="E24" s="158"/>
+      <c r="F24" s="159"/>
       <c r="G24" s="69"/>
-      <c r="H24" s="142" t="s">
+      <c r="H24" s="158" t="s">
         <v>315</v>
       </c>
-      <c r="I24" s="143"/>
+      <c r="I24" s="159"/>
       <c r="J24" s="69"/>
-      <c r="K24" s="142"/>
-      <c r="L24" s="143"/>
+      <c r="K24" s="158"/>
+      <c r="L24" s="159"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -12179,23 +12187,23 @@
     </row>
     <row r="26" spans="1:32">
       <c r="A26" s="72"/>
-      <c r="B26" s="142" t="s">
+      <c r="B26" s="158" t="s">
         <v>316</v>
       </c>
-      <c r="C26" s="143"/>
+      <c r="C26" s="159"/>
       <c r="D26" s="38"/>
-      <c r="E26" s="142" t="s">
+      <c r="E26" s="158" t="s">
         <v>324</v>
       </c>
-      <c r="F26" s="143"/>
+      <c r="F26" s="159"/>
       <c r="G26" s="69"/>
-      <c r="H26" s="142" t="s">
+      <c r="H26" s="158" t="s">
         <v>316</v>
       </c>
-      <c r="I26" s="143"/>
+      <c r="I26" s="159"/>
       <c r="J26" s="69"/>
-      <c r="K26" s="142"/>
-      <c r="L26" s="143"/>
+      <c r="K26" s="158"/>
+      <c r="L26" s="159"/>
       <c r="M26" s="78"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
@@ -12240,7 +12248,7 @@
       <c r="U27" s="4"/>
       <c r="V27" s="4"/>
       <c r="W27" s="73"/>
-      <c r="Y27" s="195" t="s">
+      <c r="Y27" s="112" t="s">
         <v>376</v>
       </c>
       <c r="Z27" s="8"/>
@@ -12249,25 +12257,25 @@
       <c r="AC27" s="8"/>
       <c r="AD27" s="8"/>
       <c r="AE27" s="8"/>
-      <c r="AF27" s="196"/>
+      <c r="AF27" s="113"/>
     </row>
     <row r="28" spans="1:32">
       <c r="A28" s="72"/>
-      <c r="B28" s="142" t="s">
+      <c r="B28" s="158" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="143"/>
+      <c r="C28" s="159"/>
       <c r="D28" s="38"/>
-      <c r="E28" s="142"/>
-      <c r="F28" s="143"/>
+      <c r="E28" s="158"/>
+      <c r="F28" s="159"/>
       <c r="G28" s="69"/>
-      <c r="H28" s="142" t="s">
+      <c r="H28" s="158" t="s">
         <v>317</v>
       </c>
-      <c r="I28" s="143"/>
+      <c r="I28" s="159"/>
       <c r="J28" s="69"/>
-      <c r="K28" s="142"/>
-      <c r="L28" s="143"/>
+      <c r="K28" s="158"/>
+      <c r="L28" s="159"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -12327,25 +12335,25 @@
     </row>
     <row r="30" spans="1:32">
       <c r="A30" s="72"/>
-      <c r="B30" s="142" t="s">
+      <c r="B30" s="158" t="s">
         <v>318</v>
       </c>
-      <c r="C30" s="143"/>
+      <c r="C30" s="159"/>
       <c r="D30" s="38"/>
-      <c r="E30" s="142" t="s">
+      <c r="E30" s="158" t="s">
         <v>326</v>
       </c>
-      <c r="F30" s="143"/>
+      <c r="F30" s="159"/>
       <c r="G30" s="69"/>
-      <c r="H30" s="142" t="s">
+      <c r="H30" s="158" t="s">
         <v>331</v>
       </c>
-      <c r="I30" s="143"/>
+      <c r="I30" s="159"/>
       <c r="J30" s="69"/>
-      <c r="K30" s="142" t="s">
+      <c r="K30" s="158" t="s">
         <v>330</v>
       </c>
-      <c r="L30" s="143"/>
+      <c r="L30" s="159"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
@@ -12403,23 +12411,23 @@
     </row>
     <row r="32" spans="1:32">
       <c r="A32" s="72"/>
-      <c r="B32" s="144" t="s">
+      <c r="B32" s="184" t="s">
         <v>320</v>
       </c>
-      <c r="C32" s="145"/>
+      <c r="C32" s="185"/>
       <c r="D32" s="38"/>
-      <c r="E32" s="144" t="s">
+      <c r="E32" s="184" t="s">
         <v>327</v>
       </c>
-      <c r="F32" s="145"/>
+      <c r="F32" s="185"/>
       <c r="G32" s="69"/>
-      <c r="H32" s="144" t="s">
+      <c r="H32" s="184" t="s">
         <v>320</v>
       </c>
-      <c r="I32" s="145"/>
+      <c r="I32" s="185"/>
       <c r="J32" s="69"/>
-      <c r="K32" s="144"/>
-      <c r="L32" s="145"/>
+      <c r="K32" s="184"/>
+      <c r="L32" s="185"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
@@ -12475,23 +12483,23 @@
     </row>
     <row r="34" spans="1:32" ht="16" thickBot="1">
       <c r="A34" s="72"/>
-      <c r="B34" s="142" t="s">
+      <c r="B34" s="158" t="s">
         <v>319</v>
       </c>
-      <c r="C34" s="143"/>
+      <c r="C34" s="159"/>
       <c r="D34" s="69"/>
-      <c r="E34" s="142" t="s">
+      <c r="E34" s="158" t="s">
         <v>328</v>
       </c>
-      <c r="F34" s="143"/>
+      <c r="F34" s="159"/>
       <c r="G34" s="69"/>
-      <c r="H34" s="142" t="s">
+      <c r="H34" s="158" t="s">
         <v>321</v>
       </c>
-      <c r="I34" s="143"/>
+      <c r="I34" s="159"/>
       <c r="J34" s="69"/>
-      <c r="K34" s="142"/>
-      <c r="L34" s="143"/>
+      <c r="K34" s="158"/>
+      <c r="L34" s="159"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
@@ -12542,18 +12550,18 @@
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="136" t="s">
+      <c r="E36" s="123" t="s">
         <v>363</v>
       </c>
-      <c r="F36" s="137"/>
+      <c r="F36" s="124"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
-      <c r="K36" s="136" t="s">
+      <c r="K36" s="123" t="s">
         <v>363</v>
       </c>
-      <c r="L36" s="137"/>
+      <c r="L36" s="124"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
       <c r="O36" s="4"/>
@@ -12570,21 +12578,21 @@
       <c r="A37" s="80" t="s">
         <v>303</v>
       </c>
-      <c r="B37" s="166" t="s">
+      <c r="B37" s="121" t="s">
         <v>362</v>
       </c>
-      <c r="C37" s="167"/>
+      <c r="C37" s="122"/>
       <c r="D37" s="81"/>
-      <c r="E37" s="138"/>
-      <c r="F37" s="139"/>
+      <c r="E37" s="125"/>
+      <c r="F37" s="126"/>
       <c r="G37" s="81"/>
-      <c r="H37" s="166" t="s">
+      <c r="H37" s="121" t="s">
         <v>362</v>
       </c>
-      <c r="I37" s="167"/>
+      <c r="I37" s="122"/>
       <c r="J37" s="81"/>
-      <c r="K37" s="138"/>
-      <c r="L37" s="139"/>
+      <c r="K37" s="125"/>
+      <c r="L37" s="126"/>
       <c r="M37" s="81"/>
       <c r="N37" s="81"/>
       <c r="O37" s="81"/>
@@ -12602,14 +12610,14 @@
       <c r="B38" s="76"/>
       <c r="C38" s="76"/>
       <c r="D38" s="76"/>
-      <c r="E38" s="172"/>
-      <c r="F38" s="173"/>
+      <c r="E38" s="127"/>
+      <c r="F38" s="128"/>
       <c r="G38" s="76"/>
       <c r="H38" s="76"/>
       <c r="I38" s="76"/>
       <c r="J38" s="76"/>
-      <c r="K38" s="172"/>
-      <c r="L38" s="173"/>
+      <c r="K38" s="127"/>
+      <c r="L38" s="128"/>
       <c r="M38" s="76"/>
       <c r="N38" s="76"/>
       <c r="O38" s="76"/>
@@ -12623,11 +12631,11 @@
       <c r="W38" s="77"/>
     </row>
     <row r="39" spans="1:32">
-      <c r="A39" s="113" t="s">
+      <c r="A39" s="172" t="s">
         <v>332</v>
       </c>
-      <c r="B39" s="114"/>
-      <c r="C39" s="114"/>
+      <c r="B39" s="173"/>
+      <c r="C39" s="173"/>
       <c r="D39" s="70"/>
       <c r="E39" s="70"/>
       <c r="F39" s="70"/>
@@ -12688,86 +12696,86 @@
     </row>
     <row r="41" spans="1:32" ht="15" customHeight="1">
       <c r="A41" s="72"/>
-      <c r="B41" s="122" t="s">
+      <c r="B41" s="166" t="s">
         <v>333</v>
       </c>
-      <c r="C41" s="123"/>
+      <c r="C41" s="178"/>
       <c r="D41" s="4"/>
-      <c r="E41" s="122" t="s">
+      <c r="E41" s="166" t="s">
         <v>335</v>
       </c>
-      <c r="F41" s="123"/>
+      <c r="F41" s="178"/>
       <c r="G41" s="4"/>
-      <c r="H41" s="122" t="s">
+      <c r="H41" s="166" t="s">
         <v>334</v>
       </c>
-      <c r="I41" s="123"/>
+      <c r="I41" s="178"/>
       <c r="J41" s="4"/>
-      <c r="K41" s="122" t="s">
+      <c r="K41" s="166" t="s">
         <v>340</v>
       </c>
-      <c r="L41" s="123"/>
+      <c r="L41" s="178"/>
       <c r="M41" s="4"/>
-      <c r="N41" s="122" t="s">
+      <c r="N41" s="166" t="s">
         <v>341</v>
       </c>
-      <c r="O41" s="123"/>
+      <c r="O41" s="178"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="151" t="s">
+      <c r="Q41" s="174" t="s">
         <v>346</v>
       </c>
-      <c r="R41" s="152"/>
+      <c r="R41" s="175"/>
       <c r="S41" s="4"/>
-      <c r="T41" s="151" t="s">
+      <c r="T41" s="174" t="s">
         <v>347</v>
       </c>
-      <c r="U41" s="152"/>
+      <c r="U41" s="175"/>
       <c r="V41" s="4"/>
-      <c r="W41" s="147" t="s">
+      <c r="W41" s="132" t="s">
         <v>348</v>
       </c>
-      <c r="X41" s="148"/>
+      <c r="X41" s="186"/>
       <c r="Y41" s="4"/>
-      <c r="Z41" s="155" t="s">
+      <c r="Z41" s="160" t="s">
         <v>365</v>
       </c>
-      <c r="AA41" s="156"/>
+      <c r="AA41" s="161"/>
       <c r="AB41" s="4"/>
     </row>
     <row r="42" spans="1:32">
       <c r="A42" s="74" t="s">
         <v>302</v>
       </c>
-      <c r="B42" s="124"/>
-      <c r="C42" s="125"/>
+      <c r="B42" s="181"/>
+      <c r="C42" s="168"/>
       <c r="D42" s="69"/>
-      <c r="E42" s="124"/>
-      <c r="F42" s="125"/>
+      <c r="E42" s="181"/>
+      <c r="F42" s="168"/>
       <c r="G42" s="69"/>
-      <c r="H42" s="124"/>
-      <c r="I42" s="125"/>
+      <c r="H42" s="181"/>
+      <c r="I42" s="168"/>
       <c r="J42" s="69"/>
-      <c r="K42" s="168"/>
-      <c r="L42" s="169"/>
+      <c r="K42" s="179"/>
+      <c r="L42" s="180"/>
       <c r="M42" s="69"/>
-      <c r="N42" s="168"/>
-      <c r="O42" s="169"/>
+      <c r="N42" s="179"/>
+      <c r="O42" s="180"/>
       <c r="P42" s="69"/>
-      <c r="Q42" s="153"/>
-      <c r="R42" s="154"/>
+      <c r="Q42" s="176"/>
+      <c r="R42" s="177"/>
       <c r="S42" s="69"/>
-      <c r="T42" s="153"/>
-      <c r="U42" s="154"/>
+      <c r="T42" s="176"/>
+      <c r="U42" s="177"/>
       <c r="V42" s="89" t="s">
         <v>364</v>
       </c>
-      <c r="W42" s="149"/>
-      <c r="X42" s="150"/>
+      <c r="W42" s="187"/>
+      <c r="X42" s="188"/>
       <c r="Y42" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="Z42" s="157"/>
-      <c r="AA42" s="158"/>
+      <c r="Z42" s="162"/>
+      <c r="AA42" s="163"/>
     </row>
     <row r="43" spans="1:32" ht="16" customHeight="1">
       <c r="A43" s="72"/>
@@ -12777,11 +12785,11 @@
       <c r="H43" s="82"/>
       <c r="I43" s="83"/>
       <c r="J43" s="4"/>
-      <c r="K43" s="124"/>
-      <c r="L43" s="125"/>
+      <c r="K43" s="181"/>
+      <c r="L43" s="168"/>
       <c r="M43" s="4"/>
-      <c r="N43" s="124"/>
-      <c r="O43" s="125"/>
+      <c r="N43" s="181"/>
+      <c r="O43" s="168"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
@@ -12789,20 +12797,20 @@
       <c r="T43" s="4"/>
       <c r="U43" s="4"/>
       <c r="V43" s="4"/>
-      <c r="Z43" s="159"/>
-      <c r="AA43" s="160"/>
+      <c r="Z43" s="164"/>
+      <c r="AA43" s="165"/>
     </row>
     <row r="44" spans="1:32" ht="15" customHeight="1">
       <c r="A44" s="72"/>
-      <c r="E44" s="170" t="s">
+      <c r="E44" s="182" t="s">
         <v>345</v>
       </c>
-      <c r="F44" s="171"/>
+      <c r="F44" s="183"/>
       <c r="G44" s="38"/>
-      <c r="H44" s="142" t="s">
+      <c r="H44" s="158" t="s">
         <v>338</v>
       </c>
-      <c r="I44" s="143"/>
+      <c r="I44" s="159"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
@@ -12832,15 +12840,15 @@
     </row>
     <row r="46" spans="1:32">
       <c r="A46" s="72"/>
-      <c r="E46" s="142" t="s">
+      <c r="E46" s="158" t="s">
         <v>337</v>
       </c>
-      <c r="F46" s="165"/>
+      <c r="F46" s="171"/>
       <c r="G46" s="38"/>
-      <c r="H46" s="166" t="s">
+      <c r="H46" s="121" t="s">
         <v>342</v>
       </c>
-      <c r="I46" s="167"/>
+      <c r="I46" s="122"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
       <c r="L46" s="4"/>
@@ -12878,15 +12886,15 @@
     </row>
     <row r="48" spans="1:32">
       <c r="A48" s="72"/>
-      <c r="E48" s="142" t="s">
+      <c r="E48" s="158" t="s">
         <v>336</v>
       </c>
-      <c r="F48" s="165"/>
+      <c r="F48" s="171"/>
       <c r="G48" s="38"/>
-      <c r="H48" s="142" t="s">
+      <c r="H48" s="158" t="s">
         <v>339</v>
       </c>
-      <c r="I48" s="165"/>
+      <c r="I48" s="171"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
       <c r="L48" s="4"/>
@@ -12915,34 +12923,34 @@
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
       <c r="P49" s="4"/>
-      <c r="Q49" s="136" t="s">
+      <c r="Q49" s="123" t="s">
         <v>368</v>
       </c>
-      <c r="R49" s="163"/>
-      <c r="S49" s="163"/>
-      <c r="T49" s="163"/>
-      <c r="U49" s="163"/>
-      <c r="V49" s="163"/>
-      <c r="W49" s="163"/>
-      <c r="X49" s="163"/>
-      <c r="Y49" s="163"/>
-      <c r="Z49" s="163"/>
-      <c r="AA49" s="137"/>
+      <c r="R49" s="153"/>
+      <c r="S49" s="153"/>
+      <c r="T49" s="153"/>
+      <c r="U49" s="153"/>
+      <c r="V49" s="153"/>
+      <c r="W49" s="153"/>
+      <c r="X49" s="153"/>
+      <c r="Y49" s="153"/>
+      <c r="Z49" s="153"/>
+      <c r="AA49" s="124"/>
     </row>
     <row r="50" spans="1:29">
       <c r="A50" s="72"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="142" t="s">
+      <c r="E50" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="F50" s="165"/>
+      <c r="F50" s="171"/>
       <c r="G50" s="38"/>
-      <c r="H50" s="142" t="s">
+      <c r="H50" s="158" t="s">
         <v>344</v>
       </c>
-      <c r="I50" s="165"/>
+      <c r="I50" s="171"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
       <c r="L50" s="4"/>
@@ -12950,17 +12958,17 @@
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
       <c r="P50" s="4"/>
-      <c r="Q50" s="138"/>
-      <c r="R50" s="115"/>
-      <c r="S50" s="115"/>
-      <c r="T50" s="115"/>
-      <c r="U50" s="115"/>
-      <c r="V50" s="115"/>
-      <c r="W50" s="115"/>
-      <c r="X50" s="115"/>
-      <c r="Y50" s="115"/>
-      <c r="Z50" s="115"/>
-      <c r="AA50" s="139"/>
+      <c r="Q50" s="125"/>
+      <c r="R50" s="154"/>
+      <c r="S50" s="154"/>
+      <c r="T50" s="154"/>
+      <c r="U50" s="154"/>
+      <c r="V50" s="154"/>
+      <c r="W50" s="154"/>
+      <c r="X50" s="154"/>
+      <c r="Y50" s="154"/>
+      <c r="Z50" s="154"/>
+      <c r="AA50" s="126"/>
     </row>
     <row r="51" spans="1:29" ht="15" customHeight="1">
       <c r="A51" s="72"/>
@@ -12970,30 +12978,30 @@
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
       <c r="G51" s="4"/>
-      <c r="H51" s="163" t="s">
+      <c r="H51" s="153" t="s">
         <v>343</v>
       </c>
-      <c r="I51" s="163"/>
-      <c r="J51" s="136" t="s">
+      <c r="I51" s="153"/>
+      <c r="J51" s="123" t="s">
         <v>363</v>
       </c>
-      <c r="K51" s="137"/>
+      <c r="K51" s="124"/>
       <c r="L51" s="4"/>
       <c r="M51" s="4"/>
       <c r="N51" s="4"/>
       <c r="O51" s="4"/>
       <c r="P51" s="4"/>
-      <c r="Q51" s="138"/>
-      <c r="R51" s="115"/>
-      <c r="S51" s="115"/>
-      <c r="T51" s="115"/>
-      <c r="U51" s="115"/>
-      <c r="V51" s="115"/>
-      <c r="W51" s="115"/>
-      <c r="X51" s="115"/>
-      <c r="Y51" s="115"/>
-      <c r="Z51" s="115"/>
-      <c r="AA51" s="139"/>
+      <c r="Q51" s="125"/>
+      <c r="R51" s="154"/>
+      <c r="S51" s="154"/>
+      <c r="T51" s="154"/>
+      <c r="U51" s="154"/>
+      <c r="V51" s="154"/>
+      <c r="W51" s="154"/>
+      <c r="X51" s="154"/>
+      <c r="Y51" s="154"/>
+      <c r="Z51" s="154"/>
+      <c r="AA51" s="126"/>
     </row>
     <row r="52" spans="1:29">
       <c r="A52" s="80" t="s">
@@ -13005,26 +13013,26 @@
       <c r="E52" s="81"/>
       <c r="F52" s="81"/>
       <c r="G52" s="81"/>
-      <c r="H52" s="115"/>
-      <c r="I52" s="115"/>
-      <c r="J52" s="138"/>
-      <c r="K52" s="139"/>
+      <c r="H52" s="154"/>
+      <c r="I52" s="154"/>
+      <c r="J52" s="125"/>
+      <c r="K52" s="126"/>
       <c r="L52" s="81"/>
       <c r="M52" s="81"/>
       <c r="N52" s="81"/>
       <c r="O52" s="81"/>
       <c r="P52" s="81"/>
-      <c r="Q52" s="138"/>
-      <c r="R52" s="115"/>
-      <c r="S52" s="115"/>
-      <c r="T52" s="115"/>
-      <c r="U52" s="115"/>
-      <c r="V52" s="115"/>
-      <c r="W52" s="115"/>
-      <c r="X52" s="115"/>
-      <c r="Y52" s="115"/>
-      <c r="Z52" s="115"/>
-      <c r="AA52" s="139"/>
+      <c r="Q52" s="125"/>
+      <c r="R52" s="154"/>
+      <c r="S52" s="154"/>
+      <c r="T52" s="154"/>
+      <c r="U52" s="154"/>
+      <c r="V52" s="154"/>
+      <c r="W52" s="154"/>
+      <c r="X52" s="154"/>
+      <c r="Y52" s="154"/>
+      <c r="Z52" s="154"/>
+      <c r="AA52" s="126"/>
     </row>
     <row r="53" spans="1:29" ht="16" thickBot="1">
       <c r="A53" s="72"/>
@@ -13034,26 +13042,26 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
-      <c r="H53" s="115"/>
-      <c r="I53" s="115"/>
-      <c r="J53" s="172"/>
-      <c r="K53" s="173"/>
+      <c r="H53" s="154"/>
+      <c r="I53" s="154"/>
+      <c r="J53" s="127"/>
+      <c r="K53" s="128"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
       <c r="P53" s="4"/>
-      <c r="Q53" s="138"/>
-      <c r="R53" s="115"/>
-      <c r="S53" s="115"/>
-      <c r="T53" s="115"/>
-      <c r="U53" s="115"/>
-      <c r="V53" s="115"/>
-      <c r="W53" s="115"/>
-      <c r="X53" s="115"/>
-      <c r="Y53" s="115"/>
-      <c r="Z53" s="115"/>
-      <c r="AA53" s="139"/>
+      <c r="Q53" s="125"/>
+      <c r="R53" s="154"/>
+      <c r="S53" s="154"/>
+      <c r="T53" s="154"/>
+      <c r="U53" s="154"/>
+      <c r="V53" s="154"/>
+      <c r="W53" s="154"/>
+      <c r="X53" s="154"/>
+      <c r="Y53" s="154"/>
+      <c r="Z53" s="154"/>
+      <c r="AA53" s="126"/>
     </row>
     <row r="54" spans="1:29">
       <c r="A54" s="72"/>
@@ -13063,8 +13071,8 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
-      <c r="H54" s="115"/>
-      <c r="I54" s="115"/>
+      <c r="H54" s="154"/>
+      <c r="I54" s="154"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -13072,17 +13080,17 @@
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
       <c r="P54" s="4"/>
-      <c r="Q54" s="138"/>
-      <c r="R54" s="115"/>
-      <c r="S54" s="115"/>
-      <c r="T54" s="115"/>
-      <c r="U54" s="115"/>
-      <c r="V54" s="115"/>
-      <c r="W54" s="115"/>
-      <c r="X54" s="115"/>
-      <c r="Y54" s="115"/>
-      <c r="Z54" s="115"/>
-      <c r="AA54" s="139"/>
+      <c r="Q54" s="125"/>
+      <c r="R54" s="154"/>
+      <c r="S54" s="154"/>
+      <c r="T54" s="154"/>
+      <c r="U54" s="154"/>
+      <c r="V54" s="154"/>
+      <c r="W54" s="154"/>
+      <c r="X54" s="154"/>
+      <c r="Y54" s="154"/>
+      <c r="Z54" s="154"/>
+      <c r="AA54" s="126"/>
     </row>
     <row r="55" spans="1:29">
       <c r="A55" s="72"/>
@@ -13092,8 +13100,8 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="115"/>
-      <c r="I55" s="115"/>
+      <c r="H55" s="154"/>
+      <c r="I55" s="154"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
@@ -13101,17 +13109,17 @@
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
       <c r="P55" s="4"/>
-      <c r="Q55" s="140"/>
-      <c r="R55" s="192"/>
-      <c r="S55" s="192"/>
-      <c r="T55" s="192"/>
-      <c r="U55" s="192"/>
-      <c r="V55" s="192"/>
-      <c r="W55" s="192"/>
-      <c r="X55" s="192"/>
-      <c r="Y55" s="192"/>
-      <c r="Z55" s="192"/>
-      <c r="AA55" s="141"/>
+      <c r="Q55" s="155"/>
+      <c r="R55" s="156"/>
+      <c r="S55" s="156"/>
+      <c r="T55" s="156"/>
+      <c r="U55" s="156"/>
+      <c r="V55" s="156"/>
+      <c r="W55" s="156"/>
+      <c r="X55" s="156"/>
+      <c r="Y55" s="156"/>
+      <c r="Z55" s="156"/>
+      <c r="AA55" s="157"/>
     </row>
     <row r="56" spans="1:29" ht="16" thickBot="1">
       <c r="A56" s="75"/>
@@ -13121,8 +13129,8 @@
       <c r="E56" s="76"/>
       <c r="F56" s="76"/>
       <c r="G56" s="76"/>
-      <c r="H56" s="164"/>
-      <c r="I56" s="164"/>
+      <c r="H56" s="170"/>
+      <c r="I56" s="170"/>
       <c r="J56" s="76"/>
       <c r="K56" s="76"/>
       <c r="L56" s="76"/>
@@ -13145,11 +13153,11 @@
       <c r="AC56" s="77"/>
     </row>
     <row r="57" spans="1:29">
-      <c r="A57" s="113" t="s">
+      <c r="A57" s="172" t="s">
         <v>369</v>
       </c>
-      <c r="B57" s="114"/>
-      <c r="C57" s="114"/>
+      <c r="B57" s="173"/>
+      <c r="C57" s="173"/>
       <c r="D57" s="70"/>
       <c r="E57" s="70"/>
       <c r="F57" s="70"/>
@@ -13171,17 +13179,17 @@
     </row>
     <row r="59" spans="1:29" ht="15" customHeight="1">
       <c r="A59" s="72"/>
-      <c r="B59" s="122" t="s">
+      <c r="B59" s="166" t="s">
         <v>311</v>
       </c>
-      <c r="C59" s="161"/>
+      <c r="C59" s="167"/>
     </row>
     <row r="60" spans="1:29">
       <c r="A60" s="74" t="s">
         <v>302</v>
       </c>
-      <c r="B60" s="161"/>
-      <c r="C60" s="125"/>
+      <c r="B60" s="167"/>
+      <c r="C60" s="168"/>
     </row>
     <row r="61" spans="1:29">
       <c r="B61" s="38"/>
@@ -13193,10 +13201,10 @@
       <c r="W61" s="87"/>
     </row>
     <row r="62" spans="1:29" ht="15" customHeight="1">
-      <c r="B62" s="122" t="s">
+      <c r="B62" s="166" t="s">
         <v>351</v>
       </c>
-      <c r="C62" s="123"/>
+      <c r="C62" s="178"/>
       <c r="S62" s="87"/>
       <c r="T62" s="87"/>
       <c r="U62" s="87"/>
@@ -13204,8 +13212,8 @@
       <c r="W62" s="87"/>
     </row>
     <row r="63" spans="1:29">
-      <c r="B63" s="124"/>
-      <c r="C63" s="125"/>
+      <c r="B63" s="181"/>
+      <c r="C63" s="168"/>
       <c r="S63" s="87"/>
       <c r="T63" s="88" t="s">
         <v>354</v>
@@ -13226,68 +13234,68 @@
       <c r="K64" s="85"/>
       <c r="L64" s="86"/>
       <c r="S64" s="87"/>
-      <c r="T64" s="146" t="s">
+      <c r="T64" s="120" t="s">
         <v>355</v>
       </c>
-      <c r="U64" s="146"/>
-      <c r="V64" s="146"/>
-      <c r="W64" s="146"/>
+      <c r="U64" s="120"/>
+      <c r="V64" s="120"/>
+      <c r="W64" s="120"/>
     </row>
     <row r="65" spans="2:23" ht="15" customHeight="1">
-      <c r="B65" s="147" t="s">
+      <c r="B65" s="132" t="s">
         <v>349</v>
       </c>
-      <c r="C65" s="181"/>
+      <c r="C65" s="138"/>
       <c r="D65" s="52"/>
-      <c r="E65" s="132" t="s">
+      <c r="E65" s="140" t="s">
         <v>352</v>
       </c>
-      <c r="F65" s="183"/>
-      <c r="G65" s="183"/>
-      <c r="H65" s="183"/>
-      <c r="I65" s="183"/>
-      <c r="J65" s="183"/>
-      <c r="K65" s="183"/>
-      <c r="L65" s="133"/>
+      <c r="F65" s="141"/>
+      <c r="G65" s="141"/>
+      <c r="H65" s="141"/>
+      <c r="I65" s="141"/>
+      <c r="J65" s="141"/>
+      <c r="K65" s="141"/>
+      <c r="L65" s="142"/>
       <c r="M65" s="52"/>
       <c r="N65" s="52"/>
-      <c r="O65" s="185" t="s">
+      <c r="O65" s="146" t="s">
         <v>353</v>
       </c>
-      <c r="P65" s="174"/>
-      <c r="Q65" s="186"/>
+      <c r="P65" s="129"/>
+      <c r="Q65" s="147"/>
       <c r="S65" s="87"/>
-      <c r="T65" s="146" t="s">
+      <c r="T65" s="120" t="s">
         <v>356</v>
       </c>
-      <c r="U65" s="146"/>
-      <c r="V65" s="146"/>
-      <c r="W65" s="146"/>
+      <c r="U65" s="120"/>
+      <c r="V65" s="120"/>
+      <c r="W65" s="120"/>
     </row>
     <row r="66" spans="2:23">
-      <c r="B66" s="179"/>
-      <c r="C66" s="182"/>
+      <c r="B66" s="136"/>
+      <c r="C66" s="139"/>
       <c r="D66" s="52"/>
-      <c r="E66" s="134"/>
-      <c r="F66" s="184"/>
-      <c r="G66" s="184"/>
-      <c r="H66" s="184"/>
-      <c r="I66" s="184"/>
-      <c r="J66" s="184"/>
-      <c r="K66" s="184"/>
-      <c r="L66" s="135"/>
+      <c r="E66" s="143"/>
+      <c r="F66" s="144"/>
+      <c r="G66" s="144"/>
+      <c r="H66" s="144"/>
+      <c r="I66" s="144"/>
+      <c r="J66" s="144"/>
+      <c r="K66" s="144"/>
+      <c r="L66" s="145"/>
       <c r="M66" s="52"/>
       <c r="N66" s="52"/>
-      <c r="O66" s="187"/>
-      <c r="P66" s="175"/>
-      <c r="Q66" s="188"/>
+      <c r="O66" s="148"/>
+      <c r="P66" s="130"/>
+      <c r="Q66" s="149"/>
       <c r="S66" s="87"/>
-      <c r="T66" s="162" t="s">
+      <c r="T66" s="169" t="s">
         <v>357</v>
       </c>
-      <c r="U66" s="162"/>
-      <c r="V66" s="162"/>
-      <c r="W66" s="162"/>
+      <c r="U66" s="169"/>
+      <c r="V66" s="169"/>
+      <c r="W66" s="169"/>
     </row>
     <row r="67" spans="2:23">
       <c r="B67" s="38"/>
@@ -13300,20 +13308,20 @@
       <c r="J67" s="85"/>
       <c r="K67" s="85"/>
       <c r="L67" s="86"/>
-      <c r="O67" s="189"/>
-      <c r="P67" s="190"/>
-      <c r="Q67" s="191"/>
+      <c r="O67" s="150"/>
+      <c r="P67" s="151"/>
+      <c r="Q67" s="152"/>
       <c r="S67" s="87"/>
-      <c r="T67" s="162"/>
-      <c r="U67" s="162"/>
-      <c r="V67" s="162"/>
-      <c r="W67" s="162"/>
+      <c r="T67" s="169"/>
+      <c r="U67" s="169"/>
+      <c r="V67" s="169"/>
+      <c r="W67" s="169"/>
     </row>
     <row r="68" spans="2:23">
-      <c r="B68" s="147" t="s">
+      <c r="B68" s="132" t="s">
         <v>350</v>
       </c>
-      <c r="C68" s="177"/>
+      <c r="C68" s="133"/>
       <c r="E68" s="85"/>
       <c r="F68" s="85"/>
       <c r="G68" s="85"/>
@@ -13324,14 +13332,14 @@
       <c r="L68" s="86"/>
       <c r="P68" s="52"/>
       <c r="S68" s="87"/>
-      <c r="T68" s="162"/>
-      <c r="U68" s="162"/>
-      <c r="V68" s="162"/>
-      <c r="W68" s="162"/>
+      <c r="T68" s="169"/>
+      <c r="U68" s="169"/>
+      <c r="V68" s="169"/>
+      <c r="W68" s="169"/>
     </row>
     <row r="69" spans="2:23" ht="15" customHeight="1">
-      <c r="B69" s="116"/>
-      <c r="C69" s="178"/>
+      <c r="B69" s="134"/>
+      <c r="C69" s="135"/>
       <c r="E69" s="86"/>
       <c r="F69" s="86"/>
       <c r="G69" s="86"/>
@@ -13340,57 +13348,57 @@
       <c r="J69" s="86"/>
       <c r="K69" s="86"/>
       <c r="L69" s="86"/>
-      <c r="O69" s="174" t="s">
+      <c r="O69" s="129" t="s">
         <v>366</v>
       </c>
-      <c r="P69" s="174"/>
-      <c r="Q69" s="174"/>
+      <c r="P69" s="129"/>
+      <c r="Q69" s="129"/>
       <c r="S69" s="87"/>
-      <c r="T69" s="162"/>
-      <c r="U69" s="162"/>
-      <c r="V69" s="162"/>
-      <c r="W69" s="162"/>
+      <c r="T69" s="169"/>
+      <c r="U69" s="169"/>
+      <c r="V69" s="169"/>
+      <c r="W69" s="169"/>
     </row>
     <row r="70" spans="2:23">
-      <c r="B70" s="179"/>
-      <c r="C70" s="180"/>
-      <c r="O70" s="175"/>
-      <c r="P70" s="175"/>
-      <c r="Q70" s="175"/>
+      <c r="B70" s="136"/>
+      <c r="C70" s="137"/>
+      <c r="O70" s="130"/>
+      <c r="P70" s="130"/>
+      <c r="Q70" s="130"/>
       <c r="S70" s="87"/>
-      <c r="T70" s="146" t="s">
+      <c r="T70" s="120" t="s">
         <v>358</v>
       </c>
-      <c r="U70" s="146"/>
-      <c r="V70" s="146"/>
-      <c r="W70" s="146"/>
+      <c r="U70" s="120"/>
+      <c r="V70" s="120"/>
+      <c r="W70" s="120"/>
     </row>
     <row r="71" spans="2:23">
-      <c r="O71" s="175"/>
-      <c r="P71" s="175"/>
-      <c r="Q71" s="175"/>
-      <c r="T71" s="146" t="s">
+      <c r="O71" s="130"/>
+      <c r="P71" s="130"/>
+      <c r="Q71" s="130"/>
+      <c r="T71" s="120" t="s">
         <v>359</v>
       </c>
-      <c r="U71" s="146"/>
-      <c r="V71" s="146"/>
-      <c r="W71" s="146"/>
+      <c r="U71" s="120"/>
+      <c r="V71" s="120"/>
+      <c r="W71" s="120"/>
     </row>
     <row r="72" spans="2:23" ht="15" customHeight="1">
-      <c r="O72" s="175"/>
-      <c r="P72" s="175"/>
-      <c r="Q72" s="175"/>
-      <c r="T72" s="176" t="s">
+      <c r="O72" s="130"/>
+      <c r="P72" s="130"/>
+      <c r="Q72" s="130"/>
+      <c r="T72" s="131" t="s">
         <v>367</v>
       </c>
-      <c r="U72" s="176"/>
-      <c r="V72" s="176"/>
-      <c r="W72" s="176"/>
+      <c r="U72" s="131"/>
+      <c r="V72" s="131"/>
+      <c r="W72" s="131"/>
     </row>
     <row r="73" spans="2:23">
-      <c r="O73" s="175"/>
-      <c r="P73" s="175"/>
-      <c r="Q73" s="175"/>
+      <c r="O73" s="130"/>
+      <c r="P73" s="130"/>
+      <c r="Q73" s="130"/>
       <c r="T73" s="109"/>
       <c r="U73" s="109"/>
       <c r="V73" s="109"/>
@@ -13410,6 +13418,74 @@
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="T6:V17"/>
+    <mergeCell ref="T3:V4"/>
+    <mergeCell ref="AA3:AB4"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="K3:L4"/>
+    <mergeCell ref="N3:O4"/>
+    <mergeCell ref="Q3:R4"/>
+    <mergeCell ref="Q6:R13"/>
+    <mergeCell ref="X3:Y4"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="N21:O22"/>
+    <mergeCell ref="T21:V22"/>
+    <mergeCell ref="Q21:R22"/>
+    <mergeCell ref="K21:L22"/>
+    <mergeCell ref="E21:F22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="T70:W70"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="W41:X42"/>
+    <mergeCell ref="T41:U42"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="B41:C42"/>
+    <mergeCell ref="E41:F42"/>
+    <mergeCell ref="H41:I42"/>
+    <mergeCell ref="B62:C63"/>
+    <mergeCell ref="Z41:AA43"/>
+    <mergeCell ref="B59:C60"/>
+    <mergeCell ref="T66:W69"/>
+    <mergeCell ref="H51:I56"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="H50:I50"/>
+    <mergeCell ref="A57:C57"/>
+    <mergeCell ref="Q41:R42"/>
+    <mergeCell ref="H46:I46"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="K41:L43"/>
+    <mergeCell ref="N41:O43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E46:F46"/>
     <mergeCell ref="T71:W71"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="E36:F38"/>
@@ -13426,74 +13502,6 @@
     <mergeCell ref="T64:W64"/>
     <mergeCell ref="T65:W65"/>
     <mergeCell ref="H44:I44"/>
-    <mergeCell ref="Z41:AA43"/>
-    <mergeCell ref="B59:C60"/>
-    <mergeCell ref="T66:W69"/>
-    <mergeCell ref="H51:I56"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="A57:C57"/>
-    <mergeCell ref="Q41:R42"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="K41:L43"/>
-    <mergeCell ref="N41:O43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="B41:C42"/>
-    <mergeCell ref="E41:F42"/>
-    <mergeCell ref="H41:I42"/>
-    <mergeCell ref="B62:C63"/>
-    <mergeCell ref="T70:W70"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="W41:X42"/>
-    <mergeCell ref="T41:U42"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="N21:O22"/>
-    <mergeCell ref="T21:V22"/>
-    <mergeCell ref="Q21:R22"/>
-    <mergeCell ref="K21:L22"/>
-    <mergeCell ref="E21:F22"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="T6:V17"/>
-    <mergeCell ref="T3:V4"/>
-    <mergeCell ref="AA3:AB4"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="K3:L4"/>
-    <mergeCell ref="N3:O4"/>
-    <mergeCell ref="Q3:R4"/>
-    <mergeCell ref="Q6:R13"/>
-    <mergeCell ref="X3:Y4"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="E6:F7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -13546,17 +13554,17 @@
       <c r="A3" s="29" t="s">
         <v>382</v>
       </c>
-      <c r="B3" s="193">
+      <c r="B3" s="110">
         <v>1070953</v>
       </c>
-      <c r="C3" s="193">
+      <c r="C3" s="110">
         <v>1097710</v>
       </c>
-      <c r="D3" s="193">
+      <c r="D3" s="110">
         <f>MAX(B3:C3)-MIN(B3:C3)</f>
         <v>26757</v>
       </c>
-      <c r="E3" s="194">
+      <c r="E3" s="111">
         <f>MIN(B3:C3)/MAX(B3:C3)</f>
         <v>0.97562470962276016</v>
       </c>
@@ -13565,13 +13573,13 @@
       <c r="A4" s="29" t="s">
         <v>383</v>
       </c>
-      <c r="B4" s="193">
+      <c r="B4" s="110">
         <v>225655</v>
       </c>
-      <c r="C4" s="193">
+      <c r="C4" s="110">
         <v>252861</v>
       </c>
-      <c r="D4" s="193">
+      <c r="D4" s="110">
         <f t="shared" ref="D4:D8" si="0">MAX(B4:C4)-MIN(B4:C4)</f>
         <v>27206</v>
       </c>
@@ -13584,13 +13592,13 @@
       <c r="A5" s="29" t="s">
         <v>384</v>
       </c>
-      <c r="B5" s="193">
+      <c r="B5" s="110">
         <v>323534</v>
       </c>
-      <c r="C5" s="193">
+      <c r="C5" s="110">
         <v>279948</v>
       </c>
-      <c r="D5" s="193">
+      <c r="D5" s="110">
         <f t="shared" si="0"/>
         <v>43586</v>
       </c>
@@ -13603,18 +13611,18 @@
       <c r="A6" s="29" t="s">
         <v>385</v>
       </c>
-      <c r="B6" s="193">
+      <c r="B6" s="110">
         <v>806519</v>
       </c>
-      <c r="C6" s="193">
+      <c r="C6" s="110">
         <v>806783</v>
       </c>
-      <c r="D6" s="193">
+      <c r="D6" s="110">
         <f t="shared" si="0"/>
         <v>264</v>
       </c>
-      <c r="E6" s="194">
-        <f t="shared" ref="E4:E11" si="1">MIN(B6:C6)/MAX(B6:C6)</f>
+      <c r="E6" s="111">
+        <f t="shared" ref="E6:E11" si="1">MIN(B6:C6)/MAX(B6:C6)</f>
         <v>0.99967277446351743</v>
       </c>
     </row>
@@ -13622,13 +13630,13 @@
       <c r="A7" s="29" t="s">
         <v>388</v>
       </c>
-      <c r="B7" s="193">
+      <c r="B7" s="110">
         <v>249241</v>
       </c>
-      <c r="C7" s="193">
+      <c r="C7" s="110">
         <v>188529</v>
       </c>
-      <c r="D7" s="193">
+      <c r="D7" s="110">
         <f t="shared" si="0"/>
         <v>60712</v>
       </c>
@@ -13641,18 +13649,18 @@
       <c r="A8" s="29" t="s">
         <v>386</v>
       </c>
-      <c r="B8" s="193">
+      <c r="B8" s="110">
         <v>2675902</v>
       </c>
-      <c r="C8" s="193">
+      <c r="C8" s="110">
         <f>SUM(C3:C7)</f>
         <v>2625831</v>
       </c>
-      <c r="D8" s="193">
+      <c r="D8" s="110">
         <f t="shared" si="0"/>
         <v>50071</v>
       </c>
-      <c r="E8" s="194">
+      <c r="E8" s="111">
         <f t="shared" si="1"/>
         <v>0.98128817871506502</v>
       </c>
@@ -13661,10 +13669,10 @@
       <c r="A10" s="29" t="s">
         <v>390</v>
       </c>
-      <c r="B10" s="193">
+      <c r="B10" s="110">
         <v>2673344</v>
       </c>
-      <c r="C10" s="193">
+      <c r="C10" s="110">
         <v>2673344</v>
       </c>
       <c r="D10">
@@ -13691,7 +13699,7 @@
         <f>B11-C11</f>
         <v>1.8729725766680083E-2</v>
       </c>
-      <c r="E11" s="194">
+      <c r="E11" s="111">
         <f t="shared" si="1"/>
         <v>0.98128817871506524</v>
       </c>
@@ -13711,8 +13719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R397"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13731,10 +13739,10 @@
       <c r="B1" s="52" t="s">
         <v>394</v>
       </c>
-      <c r="C1" s="198" t="s">
+      <c r="C1" s="115" t="s">
         <v>395</v>
       </c>
-      <c r="D1" s="198" t="s">
+      <c r="D1" s="115" t="s">
         <v>396</v>
       </c>
       <c r="E1" s="52" t="s">
@@ -13746,25 +13754,25 @@
       <c r="H1" s="52" t="s">
         <v>394</v>
       </c>
-      <c r="I1" s="198" t="s">
+      <c r="I1" s="115" t="s">
         <v>420</v>
       </c>
-      <c r="J1" s="198" t="s">
+      <c r="J1" s="115" t="s">
         <v>421</v>
       </c>
       <c r="K1" s="52" t="s">
         <v>397</v>
       </c>
-      <c r="M1" s="197" t="s">
+      <c r="M1" s="200" t="s">
         <v>393</v>
       </c>
-      <c r="N1" s="197" t="s">
+      <c r="N1" s="200" t="s">
         <v>394</v>
       </c>
-      <c r="O1" s="199" t="s">
+      <c r="O1" s="200" t="s">
         <v>395</v>
       </c>
-      <c r="P1" s="197" t="s">
+      <c r="P1" s="200" t="s">
         <v>397</v>
       </c>
     </row>
@@ -13799,16 +13807,16 @@
       <c r="K2" s="52">
         <v>54600</v>
       </c>
-      <c r="M2" s="197">
+      <c r="M2" s="200">
         <v>2014</v>
       </c>
-      <c r="N2" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O2" s="197" t="s">
+      <c r="N2" s="200" t="s">
+        <v>398</v>
+      </c>
+      <c r="O2" s="116" t="s">
         <v>441</v>
       </c>
-      <c r="P2" s="197">
+      <c r="P2" s="200">
         <v>2487</v>
       </c>
     </row>
@@ -13843,16 +13851,16 @@
       <c r="K3" s="52">
         <v>46500</v>
       </c>
-      <c r="M3" s="197">
+      <c r="M3" s="200">
         <v>2014</v>
       </c>
-      <c r="N3" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O3" s="197" t="s">
+      <c r="N3" s="200" t="s">
+        <v>398</v>
+      </c>
+      <c r="O3" s="116" t="s">
         <v>442</v>
       </c>
-      <c r="P3" s="197">
+      <c r="P3" s="200">
         <v>51371</v>
       </c>
     </row>
@@ -13951,16 +13959,16 @@
       <c r="K6" s="52">
         <v>24600</v>
       </c>
-      <c r="M6" s="52" t="s">
+      <c r="M6" s="201" t="s">
         <v>393</v>
       </c>
-      <c r="N6" s="52" t="s">
+      <c r="N6" s="201" t="s">
         <v>394</v>
       </c>
-      <c r="O6" s="198" t="s">
+      <c r="O6" s="201" t="s">
         <v>395</v>
       </c>
-      <c r="P6" s="52" t="s">
+      <c r="P6" s="201" t="s">
         <v>397</v>
       </c>
     </row>
@@ -13995,16 +14003,16 @@
       <c r="K7" s="52">
         <v>34400</v>
       </c>
-      <c r="M7" s="52">
+      <c r="M7" s="201">
         <v>2014</v>
       </c>
-      <c r="N7" s="52" t="s">
-        <v>398</v>
-      </c>
-      <c r="O7" s="52" t="s">
+      <c r="N7" s="201" t="s">
+        <v>398</v>
+      </c>
+      <c r="O7" s="115" t="s">
         <v>443</v>
       </c>
-      <c r="P7" s="52">
+      <c r="P7" s="201">
         <v>5890</v>
       </c>
     </row>
@@ -14039,16 +14047,16 @@
       <c r="K8" s="52">
         <v>32400</v>
       </c>
-      <c r="M8" s="52">
+      <c r="M8" s="201">
         <v>2014</v>
       </c>
-      <c r="N8" s="52" t="s">
-        <v>398</v>
-      </c>
-      <c r="O8" s="52" t="s">
+      <c r="N8" s="201" t="s">
+        <v>398</v>
+      </c>
+      <c r="O8" s="115" t="s">
         <v>444</v>
       </c>
-      <c r="P8" s="52">
+      <c r="P8" s="201">
         <v>1563</v>
       </c>
     </row>
@@ -14153,13 +14161,13 @@
       <c r="N11" s="52" t="s">
         <v>394</v>
       </c>
-      <c r="O11" s="198" t="s">
+      <c r="O11" s="115" t="s">
         <v>396</v>
       </c>
-      <c r="P11" s="198" t="s">
+      <c r="P11" s="115" t="s">
         <v>445</v>
       </c>
-      <c r="Q11" s="198" t="s">
+      <c r="Q11" s="115" t="s">
         <v>446</v>
       </c>
       <c r="R11" s="52" t="s">
@@ -15079,22 +15087,22 @@
       <c r="K30" s="52">
         <v>26000</v>
       </c>
-      <c r="M30" s="197" t="s">
+      <c r="M30" s="114" t="s">
         <v>463</v>
       </c>
-      <c r="N30" s="197" t="s">
+      <c r="N30" s="114" t="s">
         <v>464</v>
       </c>
-      <c r="O30" s="199" t="s">
+      <c r="O30" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="P30" s="199" t="s">
+      <c r="P30" s="116" t="s">
         <v>61</v>
       </c>
-      <c r="Q30" s="197" t="s">
+      <c r="Q30" s="114" t="s">
         <v>465</v>
       </c>
-      <c r="R30" s="197" t="s">
+      <c r="R30" s="114" t="s">
         <v>466</v>
       </c>
     </row>
@@ -15129,22 +15137,22 @@
       <c r="K31" s="52">
         <v>28300</v>
       </c>
-      <c r="M31" s="197">
+      <c r="M31" s="114">
         <v>2014</v>
       </c>
-      <c r="N31" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O31" s="197" t="s">
+      <c r="N31" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O31" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P31" s="197" t="s">
+      <c r="P31" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="Q31" s="197" t="s">
+      <c r="Q31" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R31" s="197">
+      <c r="R31" s="114">
         <v>110257</v>
       </c>
     </row>
@@ -15179,22 +15187,22 @@
       <c r="K32" s="52">
         <v>24300</v>
       </c>
-      <c r="M32" s="197">
+      <c r="M32" s="114">
         <v>2014</v>
       </c>
-      <c r="N32" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O32" s="197" t="s">
+      <c r="N32" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O32" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P32" s="197" t="s">
+      <c r="P32" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="Q32" s="197" t="s">
+      <c r="Q32" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R32" s="197">
+      <c r="R32" s="114">
         <v>703</v>
       </c>
     </row>
@@ -15229,22 +15237,22 @@
       <c r="K33" s="52">
         <v>30400</v>
       </c>
-      <c r="M33" s="197">
+      <c r="M33" s="114">
         <v>2014</v>
       </c>
-      <c r="N33" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O33" s="197" t="s">
+      <c r="N33" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O33" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P33" s="197" t="s">
+      <c r="P33" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="Q33" s="197" t="s">
+      <c r="Q33" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R33" s="197">
+      <c r="R33" s="114">
         <v>72168</v>
       </c>
     </row>
@@ -15279,22 +15287,22 @@
       <c r="K34" s="52">
         <v>40500</v>
       </c>
-      <c r="M34" s="197">
+      <c r="M34" s="114">
         <v>2014</v>
       </c>
-      <c r="N34" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O34" s="197" t="s">
+      <c r="N34" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O34" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P34" s="197" t="s">
+      <c r="P34" s="114" t="s">
         <v>459</v>
       </c>
-      <c r="Q34" s="197" t="s">
+      <c r="Q34" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R34" s="197" t="s">
+      <c r="R34" s="114" t="s">
         <v>408</v>
       </c>
     </row>
@@ -15329,22 +15337,22 @@
       <c r="K35" s="52">
         <v>35800</v>
       </c>
-      <c r="M35" s="197">
+      <c r="M35" s="114">
         <v>2014</v>
       </c>
-      <c r="N35" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O35" s="197" t="s">
+      <c r="N35" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O35" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P35" s="197" t="s">
+      <c r="P35" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="Q35" s="197" t="s">
+      <c r="Q35" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R35" s="197">
+      <c r="R35" s="114">
         <v>15424</v>
       </c>
     </row>
@@ -15379,22 +15387,22 @@
       <c r="K36" s="52">
         <v>48600</v>
       </c>
-      <c r="M36" s="197">
+      <c r="M36" s="114">
         <v>2014</v>
       </c>
-      <c r="N36" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O36" s="197" t="s">
+      <c r="N36" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O36" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P36" s="197" t="s">
+      <c r="P36" s="114" t="s">
         <v>72</v>
       </c>
-      <c r="Q36" s="197" t="s">
+      <c r="Q36" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R36" s="197">
+      <c r="R36" s="114">
         <v>47154</v>
       </c>
     </row>
@@ -15429,22 +15437,22 @@
       <c r="K37" s="52">
         <v>40500</v>
       </c>
-      <c r="M37" s="197">
+      <c r="M37" s="114">
         <v>2014</v>
       </c>
-      <c r="N37" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O37" s="197" t="s">
+      <c r="N37" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O37" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P37" s="197" t="s">
+      <c r="P37" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="Q37" s="197" t="s">
+      <c r="Q37" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R37" s="197">
+      <c r="R37" s="114">
         <v>28794</v>
       </c>
     </row>
@@ -15479,22 +15487,22 @@
       <c r="K38" s="52">
         <v>10100</v>
       </c>
-      <c r="M38" s="197">
+      <c r="M38" s="114">
         <v>2014</v>
       </c>
-      <c r="N38" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O38" s="197" t="s">
+      <c r="N38" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O38" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P38" s="197" t="s">
+      <c r="P38" s="114" t="s">
         <v>460</v>
       </c>
-      <c r="Q38" s="197" t="s">
+      <c r="Q38" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R38" s="197">
+      <c r="R38" s="114">
         <v>957</v>
       </c>
     </row>
@@ -15529,22 +15537,22 @@
       <c r="K39" s="52">
         <v>10100</v>
       </c>
-      <c r="M39" s="197">
+      <c r="M39" s="114">
         <v>2014</v>
       </c>
-      <c r="N39" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O39" s="197" t="s">
+      <c r="N39" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O39" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P39" s="197" t="s">
+      <c r="P39" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="Q39" s="197" t="s">
+      <c r="Q39" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R39" s="197">
+      <c r="R39" s="114">
         <v>5805</v>
       </c>
     </row>
@@ -15579,22 +15587,22 @@
       <c r="K40" s="52">
         <v>12100</v>
       </c>
-      <c r="M40" s="197">
+      <c r="M40" s="114">
         <v>2014</v>
       </c>
-      <c r="N40" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O40" s="197" t="s">
+      <c r="N40" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O40" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P40" s="197" t="s">
+      <c r="P40" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="Q40" s="197" t="s">
+      <c r="Q40" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R40" s="197">
+      <c r="R40" s="114">
         <v>4901</v>
       </c>
     </row>
@@ -15629,22 +15637,22 @@
       <c r="K41" s="52">
         <v>12100</v>
       </c>
-      <c r="M41" s="197">
+      <c r="M41" s="114">
         <v>2014</v>
       </c>
-      <c r="N41" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O41" s="197" t="s">
+      <c r="N41" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O41" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P41" s="197" t="s">
+      <c r="P41" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="Q41" s="197" t="s">
+      <c r="Q41" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R41" s="197">
+      <c r="R41" s="114">
         <v>1703</v>
       </c>
     </row>
@@ -15679,22 +15687,22 @@
       <c r="K42" s="52">
         <v>12900</v>
       </c>
-      <c r="M42" s="197">
+      <c r="M42" s="114">
         <v>2014</v>
       </c>
-      <c r="N42" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O42" s="197" t="s">
+      <c r="N42" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O42" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P42" s="197" t="s">
+      <c r="P42" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="Q42" s="197" t="s">
+      <c r="Q42" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R42" s="197">
+      <c r="R42" s="114">
         <v>11306</v>
       </c>
     </row>
@@ -15729,22 +15737,22 @@
       <c r="K43" s="52">
         <v>12100</v>
       </c>
-      <c r="M43" s="197">
+      <c r="M43" s="114">
         <v>2014</v>
       </c>
-      <c r="N43" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O43" s="197" t="s">
+      <c r="N43" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O43" s="114" t="s">
         <v>457</v>
       </c>
-      <c r="P43" s="197" t="s">
+      <c r="P43" s="114" t="s">
         <v>78</v>
       </c>
-      <c r="Q43" s="197" t="s">
+      <c r="Q43" s="114" t="s">
         <v>458</v>
       </c>
-      <c r="R43" s="197">
+      <c r="R43" s="114">
         <v>1577</v>
       </c>
     </row>
@@ -15779,22 +15787,22 @@
       <c r="K44" s="52">
         <v>12100</v>
       </c>
-      <c r="M44" s="197">
+      <c r="M44" s="114">
         <v>2014</v>
       </c>
-      <c r="N44" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O44" s="197" t="s">
+      <c r="N44" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O44" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P44" s="197" t="s">
+      <c r="P44" s="114" t="s">
         <v>68</v>
       </c>
-      <c r="Q44" s="197" t="s">
+      <c r="Q44" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R44" s="197">
+      <c r="R44" s="114">
         <v>3698</v>
       </c>
     </row>
@@ -15829,22 +15837,22 @@
       <c r="K45" s="52">
         <v>14200</v>
       </c>
-      <c r="M45" s="197">
+      <c r="M45" s="114">
         <v>2014</v>
       </c>
-      <c r="N45" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O45" s="197" t="s">
+      <c r="N45" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O45" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P45" s="197" t="s">
+      <c r="P45" s="114" t="s">
         <v>69</v>
       </c>
-      <c r="Q45" s="197" t="s">
+      <c r="Q45" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R45" s="197">
+      <c r="R45" s="114">
         <v>73</v>
       </c>
     </row>
@@ -15879,22 +15887,22 @@
       <c r="K46" s="52">
         <v>14200</v>
       </c>
-      <c r="M46" s="197">
+      <c r="M46" s="114">
         <v>2014</v>
       </c>
-      <c r="N46" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O46" s="197" t="s">
+      <c r="N46" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O46" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P46" s="197" t="s">
+      <c r="P46" s="114" t="s">
         <v>70</v>
       </c>
-      <c r="Q46" s="197" t="s">
+      <c r="Q46" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R46" s="197">
+      <c r="R46" s="114">
         <v>8452</v>
       </c>
     </row>
@@ -15929,22 +15937,22 @@
       <c r="K47" s="52">
         <v>13800</v>
       </c>
-      <c r="M47" s="197">
+      <c r="M47" s="114">
         <v>2014</v>
       </c>
-      <c r="N47" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O47" s="197" t="s">
+      <c r="N47" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O47" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P47" s="197" t="s">
+      <c r="P47" s="114" t="s">
         <v>459</v>
       </c>
-      <c r="Q47" s="197" t="s">
+      <c r="Q47" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R47" s="197" t="s">
+      <c r="R47" s="114" t="s">
         <v>408</v>
       </c>
     </row>
@@ -15979,22 +15987,22 @@
       <c r="K48" s="52">
         <v>14200</v>
       </c>
-      <c r="M48" s="197">
+      <c r="M48" s="114">
         <v>2014</v>
       </c>
-      <c r="N48" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O48" s="197" t="s">
+      <c r="N48" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O48" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P48" s="197" t="s">
+      <c r="P48" s="114" t="s">
         <v>71</v>
       </c>
-      <c r="Q48" s="197" t="s">
+      <c r="Q48" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R48" s="197">
+      <c r="R48" s="114">
         <v>1376</v>
       </c>
     </row>
@@ -16029,22 +16037,22 @@
       <c r="K49" s="52">
         <v>16200</v>
       </c>
-      <c r="M49" s="197">
+      <c r="M49" s="114">
         <v>2014</v>
       </c>
-      <c r="N49" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O49" s="197" t="s">
+      <c r="N49" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O49" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P49" s="197" t="s">
+      <c r="P49" s="114" t="s">
         <v>72</v>
       </c>
-      <c r="Q49" s="197" t="s">
+      <c r="Q49" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R49" s="197">
+      <c r="R49" s="114">
         <v>2611</v>
       </c>
     </row>
@@ -16079,22 +16087,22 @@
       <c r="K50" s="52" t="s">
         <v>424</v>
       </c>
-      <c r="M50" s="197">
+      <c r="M50" s="114">
         <v>2014</v>
       </c>
-      <c r="N50" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O50" s="197" t="s">
+      <c r="N50" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O50" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P50" s="197" t="s">
+      <c r="P50" s="114" t="s">
         <v>73</v>
       </c>
-      <c r="Q50" s="197" t="s">
+      <c r="Q50" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R50" s="197">
+      <c r="R50" s="114">
         <v>4122</v>
       </c>
     </row>
@@ -16129,22 +16137,22 @@
       <c r="K51" s="52" t="s">
         <v>424</v>
       </c>
-      <c r="M51" s="197">
+      <c r="M51" s="114">
         <v>2014</v>
       </c>
-      <c r="N51" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O51" s="197" t="s">
+      <c r="N51" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O51" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P51" s="197" t="s">
+      <c r="P51" s="114" t="s">
         <v>460</v>
       </c>
-      <c r="Q51" s="197" t="s">
+      <c r="Q51" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R51" s="197">
+      <c r="R51" s="114">
         <v>80</v>
       </c>
     </row>
@@ -16179,22 +16187,22 @@
       <c r="K52" s="52" t="s">
         <v>424</v>
       </c>
-      <c r="M52" s="197">
+      <c r="M52" s="114">
         <v>2014</v>
       </c>
-      <c r="N52" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O52" s="197" t="s">
+      <c r="N52" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O52" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P52" s="197" t="s">
+      <c r="P52" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="Q52" s="197" t="s">
+      <c r="Q52" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R52" s="197">
+      <c r="R52" s="114">
         <v>427</v>
       </c>
     </row>
@@ -16229,22 +16237,22 @@
       <c r="K53" s="52" t="s">
         <v>424</v>
       </c>
-      <c r="M53" s="197">
+      <c r="M53" s="114">
         <v>2014</v>
       </c>
-      <c r="N53" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O53" s="197" t="s">
+      <c r="N53" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O53" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P53" s="197" t="s">
+      <c r="P53" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="Q53" s="197" t="s">
+      <c r="Q53" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R53" s="197">
+      <c r="R53" s="114">
         <v>184</v>
       </c>
     </row>
@@ -16279,22 +16287,22 @@
       <c r="K54" s="52" t="s">
         <v>424</v>
       </c>
-      <c r="M54" s="197">
+      <c r="M54" s="114">
         <v>2014</v>
       </c>
-      <c r="N54" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O54" s="197" t="s">
+      <c r="N54" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O54" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P54" s="197" t="s">
+      <c r="P54" s="114" t="s">
         <v>76</v>
       </c>
-      <c r="Q54" s="197" t="s">
+      <c r="Q54" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R54" s="197">
+      <c r="R54" s="114">
         <v>138</v>
       </c>
     </row>
@@ -16329,22 +16337,22 @@
       <c r="K55" s="52" t="s">
         <v>424</v>
       </c>
-      <c r="M55" s="197">
+      <c r="M55" s="114">
         <v>2014</v>
       </c>
-      <c r="N55" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O55" s="197" t="s">
+      <c r="N55" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O55" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P55" s="197" t="s">
+      <c r="P55" s="114" t="s">
         <v>77</v>
       </c>
-      <c r="Q55" s="197" t="s">
+      <c r="Q55" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R55" s="197">
+      <c r="R55" s="114">
         <v>1437</v>
       </c>
     </row>
@@ -16379,22 +16387,22 @@
       <c r="K56" s="52" t="s">
         <v>424</v>
       </c>
-      <c r="M56" s="197">
+      <c r="M56" s="114">
         <v>2014</v>
       </c>
-      <c r="N56" s="197" t="s">
-        <v>398</v>
-      </c>
-      <c r="O56" s="197" t="s">
+      <c r="N56" s="114" t="s">
+        <v>398</v>
+      </c>
+      <c r="O56" s="114" t="s">
         <v>461</v>
       </c>
-      <c r="P56" s="197" t="s">
+      <c r="P56" s="114" t="s">
         <v>78</v>
       </c>
-      <c r="Q56" s="197" t="s">
+      <c r="Q56" s="114" t="s">
         <v>462</v>
       </c>
-      <c r="R56" s="197">
+      <c r="R56" s="114">
         <v>275</v>
       </c>
     </row>

</xml_diff>

<commit_message>
this is a pain
</commit_message>
<xml_diff>
--- a/Food_SR_Organization.xlsx
+++ b/Food_SR_Organization.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17500" tabRatio="500" firstSheet="5" activeTab="5"/>
+    <workbookView xWindow="-60" yWindow="3100" windowWidth="28800" windowHeight="10840" tabRatio="500" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="1.Food Need" sheetId="3" r:id="rId1"/>
@@ -23,9 +23,10 @@
     <sheet name="Results Check" sheetId="14" r:id="rId14"/>
     <sheet name="Fats and Oils Check" sheetId="15" r:id="rId15"/>
     <sheet name="Email Caitlin" sheetId="16" r:id="rId16"/>
+    <sheet name="Caitlin's Results" sheetId="17" r:id="rId17"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -195,6 +196,65 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
+    <author>James McGough</author>
+  </authors>
+  <commentList>
+    <comment ref="AI76" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>James McGough:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+putting eggs at 100% would change this
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AI82" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>James McGough:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+putting chicken at 100% would change this.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
     <author>Caitlin Dorward</author>
   </authors>
   <commentList>
@@ -322,7 +382,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Caitlin Dorward</author>
@@ -382,7 +442,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="741">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2832" uniqueCount="748">
   <si>
     <t>ALL LOCAL</t>
   </si>
@@ -2668,12 +2728,33 @@
   <si>
     <t>z</t>
   </si>
+  <si>
+    <t>Meat &amp; Alternatives</t>
+  </si>
+  <si>
+    <t>Milk &amp; Alternatives</t>
+  </si>
+  <si>
+    <t>My Results</t>
+  </si>
+  <si>
+    <t>Food Need</t>
+  </si>
+  <si>
+    <t>Food Yield</t>
+  </si>
+  <si>
+    <t>ISFS - Food Need</t>
+  </si>
+  <si>
+    <t>ISFS -Food Yield</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -2683,8 +2764,9 @@
     <numFmt numFmtId="168" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0.0000000_-;\-* #,##0.0000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2845,6 +2927,17 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
   </fonts>
@@ -3036,7 +3129,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -3527,8 +3620,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1428">
+  <cellStyleXfs count="1460">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4957,8 +5092,40 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="368">
+  <cellXfs count="403">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -5286,16 +5453,10 @@
     <xf numFmtId="10" fontId="22" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="17" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="17" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="17" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5333,18 +5494,6 @@
     <xf numFmtId="0" fontId="3" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="22" fillId="21" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="21" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="22" fillId="21" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -5352,9 +5501,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="22" fillId="17" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5411,83 +5557,56 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="22" fillId="17" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="17" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="17" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="22" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5501,14 +5620,29 @@
     <xf numFmtId="0" fontId="10" fillId="19" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5522,6 +5656,96 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="17" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="17" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="17" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -5530,6 +5754,15 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5561,119 +5794,44 @@
     <xf numFmtId="0" fontId="3" fillId="31" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5693,26 +5851,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="10" fontId="22" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -5720,17 +5866,141 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="22" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="22" fillId="10" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="22" fillId="10" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="24" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="24" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="22" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="22" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="17" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="21" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="21" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="17" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="17" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="21" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="17" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="17" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="10" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="10" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="22" fillId="10" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="16" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="22" fillId="16" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="8" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="24" fillId="8" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1428">
+  <cellStyles count="1460">
     <cellStyle name="Comma" xfId="419" builtinId="3"/>
     <cellStyle name="Comma 3" xfId="689"/>
     <cellStyle name="Currency" xfId="649" builtinId="4"/>
@@ -6445,6 +6715,22 @@
     <cellStyle name="Followed Hyperlink" xfId="1423" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1425" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1427" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1429" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1431" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1433" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1435" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1437" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1439" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1441" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1443" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1445" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1447" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1449" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1451" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1453" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1455" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1457" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1459" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -7156,6 +7442,22 @@
     <cellStyle name="Hyperlink" xfId="1422" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1424" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1426" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1428" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1430" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1432" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1434" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1436" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1438" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1440" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1442" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1444" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1446" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1448" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1450" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1452" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1454" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1456" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1458" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 9" xfId="510"/>
     <cellStyle name="Percent" xfId="650" builtinId="5"/>
@@ -17432,7 +17734,7 @@
       </c>
     </row>
     <row r="11" spans="1:16">
-      <c r="A11" s="364" t="s">
+      <c r="A11" s="357" t="s">
         <v>520</v>
       </c>
       <c r="B11" s="118" t="s">
@@ -17463,7 +17765,7 @@
       </c>
     </row>
     <row r="12" spans="1:16">
-      <c r="A12" s="364"/>
+      <c r="A12" s="357"/>
       <c r="B12" s="118" t="s">
         <v>47</v>
       </c>
@@ -17492,7 +17794,7 @@
       </c>
     </row>
     <row r="13" spans="1:16">
-      <c r="A13" s="364"/>
+      <c r="A13" s="357"/>
       <c r="B13" s="118" t="s">
         <v>48</v>
       </c>
@@ -17521,7 +17823,7 @@
       </c>
     </row>
     <row r="14" spans="1:16">
-      <c r="A14" s="364"/>
+      <c r="A14" s="357"/>
       <c r="B14" s="118" t="s">
         <v>49</v>
       </c>
@@ -17550,7 +17852,7 @@
       </c>
     </row>
     <row r="15" spans="1:16">
-      <c r="A15" s="364"/>
+      <c r="A15" s="357"/>
       <c r="B15" s="118" t="s">
         <v>50</v>
       </c>
@@ -17579,7 +17881,7 @@
       </c>
     </row>
     <row r="16" spans="1:16">
-      <c r="A16" s="364"/>
+      <c r="A16" s="357"/>
       <c r="B16" s="118" t="s">
         <v>51</v>
       </c>
@@ -17608,7 +17910,7 @@
       </c>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="364"/>
+      <c r="A17" s="357"/>
       <c r="B17" s="118" t="s">
         <v>52</v>
       </c>
@@ -17637,7 +17939,7 @@
       </c>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="364" t="s">
+      <c r="A18" s="357" t="s">
         <v>521</v>
       </c>
       <c r="B18" s="118" t="s">
@@ -17668,7 +17970,7 @@
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="364"/>
+      <c r="A19" s="357"/>
       <c r="B19" s="118" t="s">
         <v>47</v>
       </c>
@@ -17697,7 +17999,7 @@
       </c>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="364"/>
+      <c r="A20" s="357"/>
       <c r="B20" s="118" t="s">
         <v>48</v>
       </c>
@@ -17726,7 +18028,7 @@
       </c>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="364"/>
+      <c r="A21" s="357"/>
       <c r="B21" s="118" t="s">
         <v>49</v>
       </c>
@@ -17755,7 +18057,7 @@
       </c>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="364"/>
+      <c r="A22" s="357"/>
       <c r="B22" s="118" t="s">
         <v>50</v>
       </c>
@@ -17784,7 +18086,7 @@
       </c>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="364"/>
+      <c r="A23" s="357"/>
       <c r="B23" s="118" t="s">
         <v>51</v>
       </c>
@@ -17813,7 +18115,7 @@
       </c>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="364"/>
+      <c r="A24" s="357"/>
       <c r="B24" s="118" t="s">
         <v>52</v>
       </c>
@@ -18624,10 +18926,10 @@
       <c r="C53" s="47">
         <v>57824</v>
       </c>
-      <c r="F53" s="258" t="s">
+      <c r="F53" s="251" t="s">
         <v>737</v>
       </c>
-      <c r="G53" s="258">
+      <c r="G53" s="251">
         <v>16381069</v>
       </c>
     </row>
@@ -24500,6 +24802,134 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" t="s">
+        <v>744</v>
+      </c>
+      <c r="C1" t="s">
+        <v>745</v>
+      </c>
+      <c r="D1" t="s">
+        <v>746</v>
+      </c>
+      <c r="E1" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2">
+        <v>132525.52438470401</v>
+      </c>
+      <c r="C2">
+        <v>288.75</v>
+      </c>
+      <c r="D2">
+        <v>49290</v>
+      </c>
+      <c r="E2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3">
+        <v>1172971.11713408</v>
+      </c>
+      <c r="C3">
+        <v>262398.46881802101</v>
+      </c>
+      <c r="D3">
+        <v>610544</v>
+      </c>
+      <c r="E3">
+        <v>337821</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B4">
+        <v>253670.72494848</v>
+      </c>
+      <c r="C4">
+        <v>6953.7182781675601</v>
+      </c>
+      <c r="D4">
+        <v>129870</v>
+      </c>
+      <c r="E4">
+        <v>3252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5">
+        <v>354053.09684039099</v>
+      </c>
+      <c r="C5">
+        <v>90721.254589271994</v>
+      </c>
+      <c r="D5">
+        <v>366787</v>
+      </c>
+      <c r="E5">
+        <v>162518</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6">
+        <v>806782.53276746196</v>
+      </c>
+      <c r="C6">
+        <v>856952.09</v>
+      </c>
+      <c r="D6">
+        <v>204002</v>
+      </c>
+      <c r="E6">
+        <v>366787</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H64"/>
@@ -29754,7 +30184,7 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
-      <c r="M14" s="259" t="s">
+      <c r="M14" s="252" t="s">
         <v>42</v>
       </c>
       <c r="N14" s="4"/>
@@ -29774,7 +30204,7 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="260"/>
+      <c r="M15" s="253"/>
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:26">
@@ -29792,7 +30222,7 @@
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
-      <c r="M16" s="260"/>
+      <c r="M16" s="253"/>
       <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14">
@@ -29810,7 +30240,7 @@
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
       <c r="L17" s="22"/>
-      <c r="M17" s="260"/>
+      <c r="M17" s="253"/>
       <c r="N17" s="22"/>
     </row>
     <row r="18" spans="1:14">
@@ -29828,7 +30258,7 @@
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
       <c r="L18" s="22"/>
-      <c r="M18" s="260"/>
+      <c r="M18" s="253"/>
       <c r="N18" s="22"/>
     </row>
     <row r="19" spans="1:14">
@@ -29846,7 +30276,7 @@
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
       <c r="L19" s="22"/>
-      <c r="M19" s="260"/>
+      <c r="M19" s="253"/>
       <c r="N19" s="22"/>
     </row>
     <row r="20" spans="1:14">
@@ -29862,7 +30292,7 @@
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
-      <c r="M20" s="261"/>
+      <c r="M20" s="254"/>
       <c r="N20" s="4"/>
     </row>
     <row r="21" spans="1:14">
@@ -30829,11 +31259,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN96"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AU96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T58" workbookViewId="0">
-      <selection activeCell="AD94" sqref="AD94"/>
+    <sheetView topLeftCell="G65" workbookViewId="0">
+      <selection activeCell="S70" sqref="S70:S72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -30852,14 +31282,19 @@
     <col min="26" max="26" width="8.6640625" customWidth="1"/>
     <col min="27" max="27" width="8.83203125" customWidth="1"/>
     <col min="28" max="28" width="11.1640625" customWidth="1"/>
+    <col min="42" max="42" width="11.83203125" customWidth="1"/>
+    <col min="43" max="43" width="10.1640625" customWidth="1"/>
+    <col min="44" max="45" width="12.83203125" customWidth="1"/>
+    <col min="46" max="46" width="10.83203125" customWidth="1"/>
+    <col min="47" max="47" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
-      <c r="A1" s="338" t="s">
+      <c r="A1" s="255" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="339"/>
-      <c r="C1" s="339"/>
+      <c r="B1" s="256"/>
+      <c r="C1" s="256"/>
       <c r="D1" s="56"/>
       <c r="E1" s="56"/>
       <c r="F1" s="56"/>
@@ -30920,84 +31355,84 @@
     </row>
     <row r="3" spans="1:29" ht="15" customHeight="1">
       <c r="A3" s="58"/>
-      <c r="B3" s="329" t="s">
+      <c r="B3" s="264" t="s">
         <v>291</v>
       </c>
-      <c r="C3" s="331"/>
+      <c r="C3" s="265"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="333" t="s">
+      <c r="E3" s="268" t="s">
         <v>292</v>
       </c>
-      <c r="F3" s="342"/>
+      <c r="F3" s="269"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="329" t="s">
+      <c r="H3" s="264" t="s">
         <v>296</v>
       </c>
-      <c r="I3" s="331"/>
+      <c r="I3" s="265"/>
       <c r="J3" s="4"/>
-      <c r="K3" s="329" t="s">
+      <c r="K3" s="264" t="s">
         <v>297</v>
       </c>
-      <c r="L3" s="331"/>
+      <c r="L3" s="265"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="333" t="s">
+      <c r="N3" s="268" t="s">
         <v>298</v>
       </c>
-      <c r="O3" s="342"/>
+      <c r="O3" s="269"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="333" t="s">
+      <c r="Q3" s="268" t="s">
         <v>299</v>
       </c>
-      <c r="R3" s="342"/>
+      <c r="R3" s="269"/>
       <c r="S3" s="4"/>
-      <c r="T3" s="324" t="s">
+      <c r="T3" s="258" t="s">
         <v>300</v>
       </c>
-      <c r="U3" s="356"/>
-      <c r="V3" s="356"/>
+      <c r="U3" s="259"/>
+      <c r="V3" s="259"/>
       <c r="W3" s="4"/>
-      <c r="X3" s="357" t="s">
+      <c r="X3" s="260" t="s">
         <v>341</v>
       </c>
-      <c r="Y3" s="358"/>
+      <c r="Y3" s="261"/>
       <c r="Z3" s="4"/>
-      <c r="AA3" s="357" t="s">
+      <c r="AA3" s="260" t="s">
         <v>302</v>
       </c>
-      <c r="AB3" s="358"/>
+      <c r="AB3" s="261"/>
       <c r="AC3" s="59"/>
     </row>
     <row r="4" spans="1:29" ht="15" customHeight="1">
       <c r="A4" s="60" t="s">
         <v>293</v>
       </c>
-      <c r="B4" s="361"/>
-      <c r="C4" s="362"/>
+      <c r="B4" s="266"/>
+      <c r="C4" s="267"/>
       <c r="D4" s="55"/>
-      <c r="E4" s="343"/>
-      <c r="F4" s="335"/>
+      <c r="E4" s="270"/>
+      <c r="F4" s="271"/>
       <c r="G4" s="55"/>
-      <c r="H4" s="361"/>
-      <c r="I4" s="362"/>
+      <c r="H4" s="266"/>
+      <c r="I4" s="267"/>
       <c r="J4" s="55"/>
-      <c r="K4" s="361"/>
-      <c r="L4" s="362"/>
+      <c r="K4" s="266"/>
+      <c r="L4" s="267"/>
       <c r="M4" s="55"/>
-      <c r="N4" s="343"/>
-      <c r="O4" s="335"/>
+      <c r="N4" s="270"/>
+      <c r="O4" s="271"/>
       <c r="P4" s="55"/>
-      <c r="Q4" s="343"/>
-      <c r="R4" s="335"/>
+      <c r="Q4" s="270"/>
+      <c r="R4" s="271"/>
       <c r="S4" s="55"/>
-      <c r="T4" s="324"/>
-      <c r="U4" s="356"/>
-      <c r="V4" s="356"/>
+      <c r="T4" s="258"/>
+      <c r="U4" s="259"/>
+      <c r="V4" s="259"/>
       <c r="W4" s="55"/>
-      <c r="X4" s="359"/>
-      <c r="Y4" s="360"/>
+      <c r="X4" s="262"/>
+      <c r="Y4" s="263"/>
       <c r="Z4" s="55"/>
-      <c r="AA4" s="359"/>
-      <c r="AB4" s="360"/>
+      <c r="AA4" s="262"/>
+      <c r="AB4" s="263"/>
       <c r="AC4" s="59"/>
     </row>
     <row r="5" spans="1:29">
@@ -31036,10 +31471,10 @@
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="292" t="s">
+      <c r="E6" s="311" t="s">
         <v>708</v>
       </c>
-      <c r="F6" s="292"/>
+      <c r="F6" s="311"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
@@ -31050,16 +31485,16 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-      <c r="Q6" s="284" t="s">
+      <c r="Q6" s="345" t="s">
         <v>725</v>
       </c>
-      <c r="R6" s="284"/>
+      <c r="R6" s="345"/>
       <c r="S6" s="4"/>
-      <c r="T6" s="293" t="s">
+      <c r="T6" s="257" t="s">
         <v>340</v>
       </c>
-      <c r="U6" s="293"/>
-      <c r="V6" s="293"/>
+      <c r="U6" s="257"/>
+      <c r="V6" s="257"/>
       <c r="W6" s="4"/>
       <c r="X6" s="4"/>
       <c r="Y6" s="4"/>
@@ -31075,8 +31510,8 @@
       <c r="B7" s="55"/>
       <c r="C7" s="55"/>
       <c r="D7" s="55"/>
-      <c r="E7" s="293"/>
-      <c r="F7" s="293"/>
+      <c r="E7" s="257"/>
+      <c r="F7" s="257"/>
       <c r="G7" s="55"/>
       <c r="H7" s="55"/>
       <c r="I7" s="55"/>
@@ -31087,12 +31522,12 @@
       <c r="N7" s="55"/>
       <c r="O7" s="55"/>
       <c r="P7" s="55"/>
-      <c r="Q7" s="285"/>
-      <c r="R7" s="285"/>
+      <c r="Q7" s="346"/>
+      <c r="R7" s="346"/>
       <c r="S7" s="55"/>
-      <c r="T7" s="293"/>
-      <c r="U7" s="293"/>
-      <c r="V7" s="293"/>
+      <c r="T7" s="257"/>
+      <c r="U7" s="257"/>
+      <c r="V7" s="257"/>
       <c r="W7" s="4"/>
       <c r="X7" s="4"/>
       <c r="Y7" s="4"/>
@@ -31106,8 +31541,8 @@
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="293"/>
-      <c r="F8" s="293"/>
+      <c r="E8" s="257"/>
+      <c r="F8" s="257"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
@@ -31118,12 +31553,12 @@
       <c r="N8" s="17"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="285"/>
-      <c r="R8" s="285"/>
+      <c r="Q8" s="346"/>
+      <c r="R8" s="346"/>
       <c r="S8" s="4"/>
-      <c r="T8" s="293"/>
-      <c r="U8" s="293"/>
-      <c r="V8" s="293"/>
+      <c r="T8" s="257"/>
+      <c r="U8" s="257"/>
+      <c r="V8" s="257"/>
       <c r="W8" s="4"/>
       <c r="X8" s="4"/>
       <c r="Y8" s="4"/>
@@ -31137,8 +31572,8 @@
       <c r="B9" s="19"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="293"/>
-      <c r="F9" s="293"/>
+      <c r="E9" s="257"/>
+      <c r="F9" s="257"/>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
@@ -31149,12 +31584,12 @@
       <c r="N9" s="17"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-      <c r="Q9" s="285"/>
-      <c r="R9" s="285"/>
+      <c r="Q9" s="346"/>
+      <c r="R9" s="346"/>
       <c r="S9" s="4"/>
-      <c r="T9" s="293"/>
-      <c r="U9" s="293"/>
-      <c r="V9" s="293"/>
+      <c r="T9" s="257"/>
+      <c r="U9" s="257"/>
+      <c r="V9" s="257"/>
       <c r="W9" s="4"/>
       <c r="X9" s="4"/>
       <c r="Y9" s="4"/>
@@ -31168,8 +31603,8 @@
       <c r="B10" s="19"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="293"/>
-      <c r="F10" s="293"/>
+      <c r="E10" s="257"/>
+      <c r="F10" s="257"/>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
@@ -31180,12 +31615,12 @@
       <c r="N10" s="17"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-      <c r="Q10" s="285"/>
-      <c r="R10" s="285"/>
+      <c r="Q10" s="346"/>
+      <c r="R10" s="346"/>
       <c r="S10" s="4"/>
-      <c r="T10" s="293"/>
-      <c r="U10" s="293"/>
-      <c r="V10" s="293"/>
+      <c r="T10" s="257"/>
+      <c r="U10" s="257"/>
+      <c r="V10" s="257"/>
       <c r="W10" s="4"/>
       <c r="X10" s="4"/>
       <c r="Y10" s="4"/>
@@ -31199,8 +31634,8 @@
       <c r="B11" s="19"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="293"/>
-      <c r="F11" s="293"/>
+      <c r="E11" s="257"/>
+      <c r="F11" s="257"/>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
@@ -31211,12 +31646,12 @@
       <c r="N11" s="17"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-      <c r="Q11" s="285"/>
-      <c r="R11" s="285"/>
+      <c r="Q11" s="346"/>
+      <c r="R11" s="346"/>
       <c r="S11" s="4"/>
-      <c r="T11" s="293"/>
-      <c r="U11" s="293"/>
-      <c r="V11" s="293"/>
+      <c r="T11" s="257"/>
+      <c r="U11" s="257"/>
+      <c r="V11" s="257"/>
       <c r="W11" s="4"/>
       <c r="X11" s="4"/>
       <c r="Y11" s="4"/>
@@ -31230,8 +31665,8 @@
       <c r="B12" s="19"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
-      <c r="E12" s="293"/>
-      <c r="F12" s="293"/>
+      <c r="E12" s="257"/>
+      <c r="F12" s="257"/>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
@@ -31242,12 +31677,12 @@
       <c r="N12" s="17"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-      <c r="Q12" s="285"/>
-      <c r="R12" s="285"/>
+      <c r="Q12" s="346"/>
+      <c r="R12" s="346"/>
       <c r="S12" s="4"/>
-      <c r="T12" s="293"/>
-      <c r="U12" s="293"/>
-      <c r="V12" s="293"/>
+      <c r="T12" s="257"/>
+      <c r="U12" s="257"/>
+      <c r="V12" s="257"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
       <c r="Y12" s="4"/>
@@ -31261,8 +31696,8 @@
       <c r="B13" s="19"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
-      <c r="E13" s="293"/>
-      <c r="F13" s="293"/>
+      <c r="E13" s="257"/>
+      <c r="F13" s="257"/>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
@@ -31273,12 +31708,12 @@
       <c r="N13" s="17"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-      <c r="Q13" s="285"/>
-      <c r="R13" s="285"/>
+      <c r="Q13" s="346"/>
+      <c r="R13" s="346"/>
       <c r="S13" s="4"/>
-      <c r="T13" s="293"/>
-      <c r="U13" s="293"/>
-      <c r="V13" s="293"/>
+      <c r="T13" s="257"/>
+      <c r="U13" s="257"/>
+      <c r="V13" s="257"/>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
@@ -31292,8 +31727,8 @@
       <c r="B14" s="19"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
-      <c r="E14" s="293"/>
-      <c r="F14" s="293"/>
+      <c r="E14" s="257"/>
+      <c r="F14" s="257"/>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
@@ -31304,12 +31739,12 @@
       <c r="N14" s="17"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-      <c r="Q14" s="285"/>
-      <c r="R14" s="285"/>
+      <c r="Q14" s="346"/>
+      <c r="R14" s="346"/>
       <c r="S14" s="4"/>
-      <c r="T14" s="293"/>
-      <c r="U14" s="293"/>
-      <c r="V14" s="293"/>
+      <c r="T14" s="257"/>
+      <c r="U14" s="257"/>
+      <c r="V14" s="257"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
@@ -31323,8 +31758,8 @@
       <c r="B15" s="19"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
-      <c r="E15" s="293"/>
-      <c r="F15" s="293"/>
+      <c r="E15" s="257"/>
+      <c r="F15" s="257"/>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
@@ -31335,12 +31770,12 @@
       <c r="N15" s="17"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
-      <c r="Q15" s="285"/>
-      <c r="R15" s="285"/>
+      <c r="Q15" s="346"/>
+      <c r="R15" s="346"/>
       <c r="S15" s="4"/>
-      <c r="T15" s="293"/>
-      <c r="U15" s="293"/>
-      <c r="V15" s="293"/>
+      <c r="T15" s="257"/>
+      <c r="U15" s="257"/>
+      <c r="V15" s="257"/>
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
@@ -31354,8 +31789,8 @@
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="293"/>
-      <c r="F16" s="293"/>
+      <c r="E16" s="257"/>
+      <c r="F16" s="257"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -31366,12 +31801,12 @@
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
-      <c r="Q16" s="285"/>
-      <c r="R16" s="285"/>
+      <c r="Q16" s="346"/>
+      <c r="R16" s="346"/>
       <c r="S16" s="4"/>
-      <c r="T16" s="293"/>
-      <c r="U16" s="293"/>
-      <c r="V16" s="293"/>
+      <c r="T16" s="257"/>
+      <c r="U16" s="257"/>
+      <c r="V16" s="257"/>
       <c r="W16" s="4"/>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
@@ -31385,8 +31820,8 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="293"/>
-      <c r="F17" s="293"/>
+      <c r="E17" s="257"/>
+      <c r="F17" s="257"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -31397,12 +31832,12 @@
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-      <c r="Q17" s="285"/>
-      <c r="R17" s="285"/>
+      <c r="Q17" s="346"/>
+      <c r="R17" s="346"/>
       <c r="S17" s="4"/>
-      <c r="T17" s="293"/>
-      <c r="U17" s="293"/>
-      <c r="V17" s="293"/>
+      <c r="T17" s="257"/>
+      <c r="U17" s="257"/>
+      <c r="V17" s="257"/>
       <c r="W17" s="4"/>
       <c r="X17" s="4"/>
       <c r="Y17" s="4"/>
@@ -31416,8 +31851,8 @@
       <c r="B18" s="62"/>
       <c r="C18" s="62"/>
       <c r="D18" s="62"/>
-      <c r="E18" s="294"/>
-      <c r="F18" s="294"/>
+      <c r="E18" s="312"/>
+      <c r="F18" s="312"/>
       <c r="G18" s="62"/>
       <c r="H18" s="62"/>
       <c r="I18" s="62"/>
@@ -31443,11 +31878,11 @@
       <c r="AC18" s="63"/>
     </row>
     <row r="19" spans="1:29">
-      <c r="A19" s="338" t="s">
+      <c r="A19" s="255" t="s">
         <v>303</v>
       </c>
-      <c r="B19" s="339"/>
-      <c r="C19" s="339"/>
+      <c r="B19" s="256"/>
+      <c r="C19" s="256"/>
       <c r="D19" s="56"/>
       <c r="E19" s="56"/>
       <c r="F19" s="56"/>
@@ -31502,68 +31937,68 @@
     </row>
     <row r="21" spans="1:29" ht="15" customHeight="1">
       <c r="A21" s="58"/>
-      <c r="B21" s="333" t="s">
+      <c r="B21" s="268" t="s">
         <v>312</v>
       </c>
-      <c r="C21" s="342"/>
+      <c r="C21" s="269"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="333" t="s">
+      <c r="E21" s="268" t="s">
         <v>315</v>
       </c>
-      <c r="F21" s="342"/>
+      <c r="F21" s="269"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="333" t="s">
+      <c r="H21" s="268" t="s">
         <v>313</v>
       </c>
-      <c r="I21" s="342"/>
+      <c r="I21" s="269"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="333" t="s">
+      <c r="K21" s="268" t="s">
         <v>315</v>
       </c>
-      <c r="L21" s="342"/>
+      <c r="L21" s="269"/>
       <c r="M21" s="4"/>
-      <c r="N21" s="333" t="s">
+      <c r="N21" s="268" t="s">
         <v>319</v>
       </c>
-      <c r="O21" s="342"/>
+      <c r="O21" s="269"/>
       <c r="P21" s="4"/>
-      <c r="Q21" s="333" t="s">
+      <c r="Q21" s="268" t="s">
         <v>304</v>
       </c>
-      <c r="R21" s="342"/>
+      <c r="R21" s="269"/>
       <c r="S21" s="4"/>
-      <c r="T21" s="344" t="s">
+      <c r="T21" s="276" t="s">
         <v>336</v>
       </c>
-      <c r="U21" s="345"/>
-      <c r="V21" s="346"/>
+      <c r="U21" s="277"/>
+      <c r="V21" s="278"/>
       <c r="W21" s="59"/>
     </row>
     <row r="22" spans="1:29">
       <c r="A22" s="60" t="s">
         <v>293</v>
       </c>
-      <c r="B22" s="343"/>
-      <c r="C22" s="335"/>
+      <c r="B22" s="270"/>
+      <c r="C22" s="271"/>
       <c r="D22" s="55"/>
-      <c r="E22" s="343"/>
-      <c r="F22" s="335"/>
+      <c r="E22" s="270"/>
+      <c r="F22" s="271"/>
       <c r="G22" s="55"/>
-      <c r="H22" s="343"/>
-      <c r="I22" s="335"/>
+      <c r="H22" s="270"/>
+      <c r="I22" s="271"/>
       <c r="J22" s="55"/>
-      <c r="K22" s="343"/>
-      <c r="L22" s="335"/>
+      <c r="K22" s="270"/>
+      <c r="L22" s="271"/>
       <c r="M22" s="55"/>
-      <c r="N22" s="343"/>
-      <c r="O22" s="335"/>
+      <c r="N22" s="270"/>
+      <c r="O22" s="271"/>
       <c r="P22" s="55"/>
-      <c r="Q22" s="343"/>
-      <c r="R22" s="335"/>
+      <c r="Q22" s="270"/>
+      <c r="R22" s="271"/>
       <c r="S22" s="55"/>
-      <c r="T22" s="347"/>
-      <c r="U22" s="348"/>
-      <c r="V22" s="349"/>
+      <c r="T22" s="279"/>
+      <c r="U22" s="280"/>
+      <c r="V22" s="281"/>
       <c r="W22" s="59"/>
     </row>
     <row r="23" spans="1:29">
@@ -31593,21 +32028,21 @@
     </row>
     <row r="24" spans="1:29" ht="15" customHeight="1">
       <c r="A24" s="58"/>
-      <c r="B24" s="288" t="s">
+      <c r="B24" s="272" t="s">
         <v>305</v>
       </c>
-      <c r="C24" s="289"/>
+      <c r="C24" s="273"/>
       <c r="D24" s="38"/>
-      <c r="E24" s="288"/>
-      <c r="F24" s="289"/>
+      <c r="E24" s="272"/>
+      <c r="F24" s="273"/>
       <c r="G24" s="55"/>
-      <c r="H24" s="288" t="s">
+      <c r="H24" s="272" t="s">
         <v>305</v>
       </c>
-      <c r="I24" s="289"/>
+      <c r="I24" s="273"/>
       <c r="J24" s="55"/>
-      <c r="K24" s="288"/>
-      <c r="L24" s="289"/>
+      <c r="K24" s="272"/>
+      <c r="L24" s="273"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -31647,30 +32082,30 @@
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="58"/>
-      <c r="B26" s="288" t="s">
+      <c r="B26" s="272" t="s">
         <v>306</v>
       </c>
-      <c r="C26" s="289"/>
+      <c r="C26" s="273"/>
       <c r="D26" s="38"/>
-      <c r="E26" s="288" t="s">
+      <c r="E26" s="272" t="s">
         <v>314</v>
       </c>
-      <c r="F26" s="289"/>
+      <c r="F26" s="273"/>
       <c r="G26" s="55"/>
-      <c r="H26" s="288" t="s">
+      <c r="H26" s="272" t="s">
         <v>306</v>
       </c>
-      <c r="I26" s="289"/>
+      <c r="I26" s="273"/>
       <c r="J26" s="55"/>
-      <c r="K26" s="288"/>
-      <c r="L26" s="289"/>
+      <c r="K26" s="272"/>
+      <c r="L26" s="273"/>
       <c r="M26" s="64"/>
       <c r="N26" s="4"/>
-      <c r="O26" s="295" t="s">
+      <c r="O26" s="284" t="s">
         <v>698</v>
       </c>
-      <c r="P26" s="292"/>
-      <c r="Q26" s="296"/>
+      <c r="P26" s="311"/>
+      <c r="Q26" s="285"/>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
@@ -31693,9 +32128,9 @@
       <c r="L27" s="38"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
-      <c r="O27" s="297"/>
-      <c r="P27" s="293"/>
-      <c r="Q27" s="298"/>
+      <c r="O27" s="286"/>
+      <c r="P27" s="257"/>
+      <c r="Q27" s="287"/>
       <c r="R27" s="4"/>
       <c r="S27" s="4"/>
       <c r="T27" s="4"/>
@@ -31705,26 +32140,26 @@
     </row>
     <row r="28" spans="1:29" ht="15" customHeight="1">
       <c r="A28" s="58"/>
-      <c r="B28" s="288" t="s">
+      <c r="B28" s="272" t="s">
         <v>307</v>
       </c>
-      <c r="C28" s="289"/>
+      <c r="C28" s="273"/>
       <c r="D28" s="38"/>
-      <c r="E28" s="288"/>
-      <c r="F28" s="289"/>
+      <c r="E28" s="272"/>
+      <c r="F28" s="273"/>
       <c r="G28" s="55"/>
-      <c r="H28" s="288" t="s">
+      <c r="H28" s="272" t="s">
         <v>307</v>
       </c>
-      <c r="I28" s="289"/>
+      <c r="I28" s="273"/>
       <c r="J28" s="55"/>
-      <c r="K28" s="288"/>
-      <c r="L28" s="289"/>
+      <c r="K28" s="272"/>
+      <c r="L28" s="273"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
-      <c r="O28" s="297"/>
-      <c r="P28" s="293"/>
-      <c r="Q28" s="298"/>
+      <c r="O28" s="286"/>
+      <c r="P28" s="257"/>
+      <c r="Q28" s="287"/>
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
       <c r="T28" s="4"/>
@@ -31747,9 +32182,9 @@
       <c r="L29" s="38"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
-      <c r="O29" s="297"/>
-      <c r="P29" s="293"/>
-      <c r="Q29" s="298"/>
+      <c r="O29" s="286"/>
+      <c r="P29" s="257"/>
+      <c r="Q29" s="287"/>
       <c r="R29" s="4"/>
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
@@ -31759,30 +32194,30 @@
     </row>
     <row r="30" spans="1:29">
       <c r="A30" s="58"/>
-      <c r="B30" s="288" t="s">
+      <c r="B30" s="272" t="s">
         <v>308</v>
       </c>
-      <c r="C30" s="289"/>
+      <c r="C30" s="273"/>
       <c r="D30" s="38"/>
-      <c r="E30" s="288" t="s">
+      <c r="E30" s="272" t="s">
         <v>316</v>
       </c>
-      <c r="F30" s="289"/>
+      <c r="F30" s="273"/>
       <c r="G30" s="55"/>
-      <c r="H30" s="288" t="s">
+      <c r="H30" s="272" t="s">
         <v>321</v>
       </c>
-      <c r="I30" s="289"/>
+      <c r="I30" s="273"/>
       <c r="J30" s="55"/>
-      <c r="K30" s="288" t="s">
+      <c r="K30" s="272" t="s">
         <v>320</v>
       </c>
-      <c r="L30" s="289"/>
+      <c r="L30" s="273"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
-      <c r="O30" s="297"/>
-      <c r="P30" s="293"/>
-      <c r="Q30" s="298"/>
+      <c r="O30" s="286"/>
+      <c r="P30" s="257"/>
+      <c r="Q30" s="287"/>
       <c r="R30" s="4"/>
       <c r="S30" s="4"/>
       <c r="T30" s="4"/>
@@ -31805,9 +32240,9 @@
       <c r="L31" s="38"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
-      <c r="O31" s="297"/>
-      <c r="P31" s="293"/>
-      <c r="Q31" s="298"/>
+      <c r="O31" s="286"/>
+      <c r="P31" s="257"/>
+      <c r="Q31" s="287"/>
       <c r="R31" s="4"/>
       <c r="S31" s="4"/>
       <c r="T31" s="4"/>
@@ -31817,28 +32252,28 @@
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="58"/>
-      <c r="B32" s="290" t="s">
+      <c r="B32" s="274" t="s">
         <v>310</v>
       </c>
-      <c r="C32" s="291"/>
+      <c r="C32" s="275"/>
       <c r="D32" s="38"/>
-      <c r="E32" s="290" t="s">
+      <c r="E32" s="274" t="s">
         <v>317</v>
       </c>
-      <c r="F32" s="291"/>
+      <c r="F32" s="275"/>
       <c r="G32" s="55"/>
-      <c r="H32" s="290" t="s">
+      <c r="H32" s="274" t="s">
         <v>310</v>
       </c>
-      <c r="I32" s="291"/>
+      <c r="I32" s="275"/>
       <c r="J32" s="55"/>
-      <c r="K32" s="290"/>
-      <c r="L32" s="291"/>
+      <c r="K32" s="274"/>
+      <c r="L32" s="275"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
-      <c r="O32" s="297"/>
-      <c r="P32" s="293"/>
-      <c r="Q32" s="298"/>
+      <c r="O32" s="286"/>
+      <c r="P32" s="257"/>
+      <c r="Q32" s="287"/>
       <c r="R32" s="4"/>
       <c r="S32" s="4"/>
       <c r="T32" s="4"/>
@@ -31861,9 +32296,9 @@
       <c r="L33" s="65"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
-      <c r="O33" s="297"/>
-      <c r="P33" s="293"/>
-      <c r="Q33" s="298"/>
+      <c r="O33" s="286"/>
+      <c r="P33" s="257"/>
+      <c r="Q33" s="287"/>
       <c r="R33" s="4"/>
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
@@ -31873,28 +32308,28 @@
     </row>
     <row r="34" spans="1:29">
       <c r="A34" s="58"/>
-      <c r="B34" s="288" t="s">
+      <c r="B34" s="272" t="s">
         <v>309</v>
       </c>
-      <c r="C34" s="289"/>
+      <c r="C34" s="273"/>
       <c r="D34" s="55"/>
-      <c r="E34" s="288" t="s">
+      <c r="E34" s="272" t="s">
         <v>318</v>
       </c>
-      <c r="F34" s="289"/>
+      <c r="F34" s="273"/>
       <c r="G34" s="55"/>
-      <c r="H34" s="288" t="s">
+      <c r="H34" s="272" t="s">
         <v>311</v>
       </c>
-      <c r="I34" s="289"/>
+      <c r="I34" s="273"/>
       <c r="J34" s="55"/>
-      <c r="K34" s="288"/>
-      <c r="L34" s="289"/>
+      <c r="K34" s="272"/>
+      <c r="L34" s="273"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
-      <c r="O34" s="297"/>
-      <c r="P34" s="293"/>
-      <c r="Q34" s="298"/>
+      <c r="O34" s="286"/>
+      <c r="P34" s="257"/>
+      <c r="Q34" s="287"/>
       <c r="R34" s="4"/>
       <c r="S34" s="4"/>
       <c r="T34" s="4"/>
@@ -31917,9 +32352,9 @@
       <c r="L35" s="65"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
-      <c r="O35" s="297"/>
-      <c r="P35" s="293"/>
-      <c r="Q35" s="298"/>
+      <c r="O35" s="286"/>
+      <c r="P35" s="257"/>
+      <c r="Q35" s="287"/>
       <c r="R35" s="4"/>
       <c r="S35" s="4"/>
       <c r="T35" s="4"/>
@@ -31932,21 +32367,21 @@
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="295" t="s">
+      <c r="E36" s="284" t="s">
         <v>342</v>
       </c>
-      <c r="F36" s="296"/>
+      <c r="F36" s="285"/>
       <c r="G36" s="4"/>
-      <c r="H36" s="295" t="s">
+      <c r="H36" s="284" t="s">
         <v>709</v>
       </c>
-      <c r="I36" s="296"/>
+      <c r="I36" s="285"/>
       <c r="J36" s="4"/>
       <c r="M36" s="4"/>
       <c r="N36" s="4"/>
-      <c r="O36" s="297"/>
-      <c r="P36" s="293"/>
-      <c r="Q36" s="298"/>
+      <c r="O36" s="286"/>
+      <c r="P36" s="257"/>
+      <c r="Q36" s="287"/>
       <c r="R36" s="4"/>
       <c r="S36" s="4"/>
       <c r="T36" s="4"/>
@@ -31958,22 +32393,22 @@
       <c r="A37" s="66" t="s">
         <v>294</v>
       </c>
-      <c r="B37" s="286"/>
-      <c r="C37" s="287"/>
+      <c r="B37" s="282"/>
+      <c r="C37" s="283"/>
       <c r="D37" s="55"/>
-      <c r="E37" s="297"/>
-      <c r="F37" s="298"/>
+      <c r="E37" s="286"/>
+      <c r="F37" s="287"/>
       <c r="G37" s="67"/>
-      <c r="H37" s="297"/>
-      <c r="I37" s="298"/>
+      <c r="H37" s="286"/>
+      <c r="I37" s="287"/>
       <c r="J37" s="67"/>
-      <c r="K37" s="286"/>
-      <c r="L37" s="287"/>
+      <c r="K37" s="282"/>
+      <c r="L37" s="283"/>
       <c r="M37" s="67"/>
       <c r="N37" s="67"/>
-      <c r="O37" s="299"/>
-      <c r="P37" s="300"/>
-      <c r="Q37" s="301"/>
+      <c r="O37" s="318"/>
+      <c r="P37" s="319"/>
+      <c r="Q37" s="320"/>
       <c r="R37" s="67"/>
       <c r="S37" s="67"/>
       <c r="T37" s="67"/>
@@ -31986,11 +32421,11 @@
       <c r="B38" s="62"/>
       <c r="C38" s="62"/>
       <c r="D38" s="62"/>
-      <c r="E38" s="320"/>
-      <c r="F38" s="321"/>
+      <c r="E38" s="288"/>
+      <c r="F38" s="289"/>
       <c r="G38" s="62"/>
-      <c r="H38" s="320"/>
-      <c r="I38" s="321"/>
+      <c r="H38" s="288"/>
+      <c r="I38" s="289"/>
       <c r="J38" s="62"/>
       <c r="M38" s="62"/>
       <c r="N38" s="62"/>
@@ -32005,11 +32440,11 @@
       <c r="W38" s="63"/>
     </row>
     <row r="39" spans="1:29">
-      <c r="A39" s="338" t="s">
+      <c r="A39" s="255" t="s">
         <v>322</v>
       </c>
-      <c r="B39" s="339"/>
-      <c r="C39" s="339"/>
+      <c r="B39" s="256"/>
+      <c r="C39" s="256"/>
       <c r="D39" s="56"/>
       <c r="E39" s="56"/>
       <c r="F39" s="56"/>
@@ -32039,20 +32474,20 @@
     </row>
     <row r="40" spans="1:29">
       <c r="A40" s="58"/>
-      <c r="B40" s="229"/>
-      <c r="C40" s="230"/>
-      <c r="D40" s="230"/>
-      <c r="E40" s="230"/>
-      <c r="F40" s="230"/>
-      <c r="G40" s="230"/>
-      <c r="H40" s="230"/>
-      <c r="I40" s="230"/>
-      <c r="J40" s="230"/>
-      <c r="K40" s="230"/>
-      <c r="L40" s="230"/>
-      <c r="M40" s="230"/>
-      <c r="N40" s="230"/>
-      <c r="O40" s="231"/>
+      <c r="B40" s="227"/>
+      <c r="C40" s="228"/>
+      <c r="D40" s="228"/>
+      <c r="E40" s="228"/>
+      <c r="F40" s="228"/>
+      <c r="G40" s="228"/>
+      <c r="H40" s="228"/>
+      <c r="I40" s="228"/>
+      <c r="J40" s="228"/>
+      <c r="K40" s="228"/>
+      <c r="L40" s="228"/>
+      <c r="M40" s="228"/>
+      <c r="N40" s="228"/>
+      <c r="O40" s="229"/>
       <c r="P40" s="4"/>
       <c r="Q40" s="4"/>
       <c r="R40" s="4"/>
@@ -32070,45 +32505,45 @@
     </row>
     <row r="41" spans="1:29" ht="15" customHeight="1">
       <c r="A41" s="58"/>
-      <c r="B41" s="312" t="s">
+      <c r="B41" s="303" t="s">
         <v>323</v>
       </c>
-      <c r="C41" s="313"/>
+      <c r="C41" s="304"/>
       <c r="D41" s="64"/>
-      <c r="E41" s="312" t="s">
+      <c r="E41" s="303" t="s">
         <v>325</v>
       </c>
-      <c r="F41" s="313"/>
+      <c r="F41" s="304"/>
       <c r="G41" s="64"/>
-      <c r="H41" s="312" t="s">
+      <c r="H41" s="303" t="s">
         <v>324</v>
       </c>
-      <c r="I41" s="313"/>
+      <c r="I41" s="304"/>
       <c r="J41" s="64"/>
-      <c r="K41" s="312" t="s">
+      <c r="K41" s="303" t="s">
         <v>330</v>
       </c>
-      <c r="L41" s="313"/>
+      <c r="L41" s="304"/>
       <c r="M41" s="64"/>
-      <c r="N41" s="312" t="s">
+      <c r="N41" s="303" t="s">
         <v>331</v>
       </c>
-      <c r="O41" s="313"/>
+      <c r="O41" s="304"/>
       <c r="P41" s="4"/>
-      <c r="Q41" s="308" t="s">
+      <c r="Q41" s="330" t="s">
         <v>707</v>
       </c>
-      <c r="R41" s="309"/>
+      <c r="R41" s="331"/>
       <c r="S41" s="4"/>
       <c r="T41" s="172" t="s">
         <v>335</v>
       </c>
       <c r="U41" s="173"/>
       <c r="V41" s="4"/>
-      <c r="W41" s="302" t="s">
+      <c r="W41" s="324" t="s">
         <v>343</v>
       </c>
-      <c r="X41" s="303"/>
+      <c r="X41" s="325"/>
       <c r="AB41" s="4"/>
       <c r="AC41" s="59"/>
     </row>
@@ -32116,23 +32551,23 @@
       <c r="A42" s="60" t="s">
         <v>293</v>
       </c>
-      <c r="B42" s="316"/>
-      <c r="C42" s="317"/>
+      <c r="B42" s="307"/>
+      <c r="C42" s="308"/>
       <c r="D42" s="64"/>
-      <c r="E42" s="316"/>
-      <c r="F42" s="317"/>
+      <c r="E42" s="307"/>
+      <c r="F42" s="308"/>
       <c r="G42" s="64"/>
-      <c r="H42" s="316"/>
-      <c r="I42" s="317"/>
+      <c r="H42" s="307"/>
+      <c r="I42" s="308"/>
       <c r="J42" s="64"/>
-      <c r="K42" s="314"/>
-      <c r="L42" s="315"/>
+      <c r="K42" s="305"/>
+      <c r="L42" s="306"/>
       <c r="M42" s="64"/>
-      <c r="N42" s="314"/>
-      <c r="O42" s="315"/>
+      <c r="N42" s="305"/>
+      <c r="O42" s="306"/>
       <c r="P42" s="55"/>
-      <c r="Q42" s="310"/>
-      <c r="R42" s="311"/>
+      <c r="Q42" s="332"/>
+      <c r="R42" s="333"/>
       <c r="S42" s="72" t="s">
         <v>103</v>
       </c>
@@ -32141,54 +32576,54 @@
       <c r="V42" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="W42" s="304"/>
-      <c r="X42" s="305"/>
+      <c r="W42" s="326"/>
+      <c r="X42" s="327"/>
       <c r="AC42" s="59"/>
     </row>
     <row r="43" spans="1:29" ht="16" customHeight="1">
       <c r="A43" s="58"/>
-      <c r="B43" s="225"/>
+      <c r="B43" s="223"/>
       <c r="C43" s="64"/>
       <c r="D43" s="64"/>
-      <c r="E43" s="225"/>
-      <c r="F43" s="226"/>
+      <c r="E43" s="223"/>
+      <c r="F43" s="224"/>
       <c r="G43" s="64"/>
-      <c r="H43" s="225"/>
-      <c r="I43" s="226"/>
+      <c r="H43" s="223"/>
+      <c r="I43" s="224"/>
       <c r="J43" s="64"/>
-      <c r="K43" s="316"/>
-      <c r="L43" s="317"/>
+      <c r="K43" s="307"/>
+      <c r="L43" s="308"/>
       <c r="M43" s="64"/>
-      <c r="N43" s="316"/>
-      <c r="O43" s="317"/>
+      <c r="N43" s="307"/>
+      <c r="O43" s="308"/>
       <c r="P43" s="4"/>
       <c r="Q43" s="4"/>
       <c r="R43" s="4"/>
       <c r="S43" s="4"/>
-      <c r="W43" s="306"/>
-      <c r="X43" s="307"/>
+      <c r="W43" s="328"/>
+      <c r="X43" s="329"/>
       <c r="AC43" s="59"/>
     </row>
     <row r="44" spans="1:29" ht="15" customHeight="1">
       <c r="A44" s="58"/>
-      <c r="B44" s="225"/>
+      <c r="B44" s="223"/>
       <c r="C44" s="64"/>
       <c r="D44" s="64"/>
-      <c r="E44" s="340" t="s">
+      <c r="E44" s="309" t="s">
         <v>334</v>
       </c>
-      <c r="F44" s="341"/>
+      <c r="F44" s="310"/>
       <c r="G44" s="64"/>
-      <c r="H44" s="318" t="s">
+      <c r="H44" s="297" t="s">
         <v>328</v>
       </c>
-      <c r="I44" s="332"/>
+      <c r="I44" s="298"/>
       <c r="J44" s="64"/>
       <c r="K44" s="64"/>
       <c r="L44" s="64"/>
       <c r="M44" s="64"/>
       <c r="N44" s="64"/>
-      <c r="O44" s="226"/>
+      <c r="O44" s="224"/>
       <c r="P44" s="4"/>
       <c r="Q44" s="4"/>
       <c r="R44" s="4"/>
@@ -32196,20 +32631,20 @@
       <c r="AC44" s="59"/>
     </row>
     <row r="45" spans="1:29">
-      <c r="B45" s="225"/>
+      <c r="B45" s="223"/>
       <c r="C45" s="64"/>
       <c r="D45" s="64"/>
-      <c r="E45" s="225"/>
-      <c r="F45" s="226"/>
+      <c r="E45" s="223"/>
+      <c r="F45" s="224"/>
       <c r="G45" s="64"/>
-      <c r="H45" s="225"/>
-      <c r="I45" s="226"/>
+      <c r="H45" s="223"/>
+      <c r="I45" s="224"/>
       <c r="J45" s="64"/>
       <c r="K45" s="64"/>
       <c r="L45" s="64"/>
       <c r="M45" s="64"/>
       <c r="N45" s="64"/>
-      <c r="O45" s="226"/>
+      <c r="O45" s="224"/>
       <c r="Q45" s="4"/>
       <c r="R45" s="4"/>
       <c r="S45" s="17"/>
@@ -32222,78 +32657,78 @@
     </row>
     <row r="46" spans="1:29" ht="15" customHeight="1">
       <c r="A46" s="58"/>
-      <c r="B46" s="225"/>
+      <c r="B46" s="223"/>
       <c r="C46" s="64"/>
       <c r="D46" s="64"/>
-      <c r="E46" s="318" t="s">
+      <c r="E46" s="297" t="s">
         <v>502</v>
       </c>
-      <c r="F46" s="319"/>
+      <c r="F46" s="300"/>
       <c r="G46" s="64"/>
-      <c r="H46" s="318" t="s">
+      <c r="H46" s="297" t="s">
         <v>332</v>
       </c>
-      <c r="I46" s="332"/>
+      <c r="I46" s="298"/>
       <c r="J46" s="64"/>
       <c r="K46" s="64"/>
       <c r="L46" s="64"/>
       <c r="M46" s="64"/>
       <c r="N46" s="64"/>
-      <c r="O46" s="226"/>
+      <c r="O46" s="224"/>
       <c r="P46" s="4"/>
       <c r="S46" s="17"/>
-      <c r="T46" s="222"/>
-      <c r="U46" s="222"/>
+      <c r="T46" s="220"/>
+      <c r="U46" s="220"/>
       <c r="V46" s="17"/>
-      <c r="W46" s="222"/>
-      <c r="X46" s="222"/>
+      <c r="W46" s="220"/>
+      <c r="X46" s="220"/>
       <c r="AC46" s="59"/>
     </row>
     <row r="47" spans="1:29">
       <c r="A47" s="58"/>
-      <c r="B47" s="225"/>
+      <c r="B47" s="223"/>
       <c r="C47" s="64"/>
       <c r="D47" s="64"/>
-      <c r="E47" s="225"/>
-      <c r="F47" s="226"/>
+      <c r="E47" s="223"/>
+      <c r="F47" s="224"/>
       <c r="G47" s="64"/>
-      <c r="H47" s="225"/>
-      <c r="I47" s="226"/>
+      <c r="H47" s="223"/>
+      <c r="I47" s="224"/>
       <c r="J47" s="64"/>
       <c r="K47" s="64"/>
       <c r="L47" s="64"/>
       <c r="M47" s="64"/>
       <c r="N47" s="64"/>
-      <c r="O47" s="226"/>
+      <c r="O47" s="224"/>
       <c r="P47" s="17"/>
-      <c r="S47" s="221"/>
-      <c r="T47" s="222"/>
-      <c r="U47" s="222"/>
+      <c r="S47" s="219"/>
+      <c r="T47" s="220"/>
+      <c r="U47" s="220"/>
       <c r="V47" s="17"/>
-      <c r="W47" s="222"/>
-      <c r="X47" s="222"/>
+      <c r="W47" s="220"/>
+      <c r="X47" s="220"/>
       <c r="AC47" s="59"/>
     </row>
     <row r="48" spans="1:29">
       <c r="A48" s="58"/>
-      <c r="B48" s="225"/>
+      <c r="B48" s="223"/>
       <c r="C48" s="64"/>
       <c r="D48" s="64"/>
-      <c r="E48" s="318" t="s">
+      <c r="E48" s="297" t="s">
         <v>326</v>
       </c>
-      <c r="F48" s="319"/>
+      <c r="F48" s="300"/>
       <c r="G48" s="64"/>
-      <c r="H48" s="318" t="s">
+      <c r="H48" s="297" t="s">
         <v>329</v>
       </c>
-      <c r="I48" s="319"/>
+      <c r="I48" s="300"/>
       <c r="J48" s="64"/>
       <c r="K48" s="64"/>
       <c r="L48" s="64"/>
       <c r="M48" s="64"/>
       <c r="N48" s="64"/>
-      <c r="O48" s="226"/>
+      <c r="O48" s="224"/>
       <c r="P48" s="4"/>
       <c r="Q48" s="4"/>
       <c r="R48" s="4"/>
@@ -32301,107 +32736,107 @@
       <c r="T48" s="17"/>
       <c r="U48" s="17"/>
       <c r="V48" s="17"/>
-      <c r="W48" s="222"/>
-      <c r="X48" s="222"/>
+      <c r="W48" s="220"/>
+      <c r="X48" s="220"/>
       <c r="AC48" s="59"/>
     </row>
-    <row r="49" spans="1:38">
+    <row r="49" spans="1:47">
       <c r="A49" s="58"/>
-      <c r="B49" s="225"/>
+      <c r="B49" s="223"/>
       <c r="C49" s="64"/>
       <c r="D49" s="64"/>
-      <c r="E49" s="227"/>
-      <c r="F49" s="228"/>
+      <c r="E49" s="225"/>
+      <c r="F49" s="226"/>
       <c r="G49" s="64"/>
-      <c r="H49" s="227"/>
-      <c r="I49" s="228"/>
+      <c r="H49" s="225"/>
+      <c r="I49" s="226"/>
       <c r="J49" s="64"/>
       <c r="K49" s="64"/>
       <c r="L49" s="64"/>
       <c r="M49" s="64"/>
       <c r="N49" s="64"/>
-      <c r="O49" s="226"/>
+      <c r="O49" s="224"/>
       <c r="P49" s="4"/>
-      <c r="Q49" s="295" t="s">
+      <c r="Q49" s="284" t="s">
         <v>699</v>
       </c>
-      <c r="R49" s="292"/>
-      <c r="S49" s="293"/>
-      <c r="T49" s="293"/>
-      <c r="U49" s="293"/>
-      <c r="V49" s="293"/>
-      <c r="W49" s="293"/>
-      <c r="X49" s="293"/>
-      <c r="Y49" s="292"/>
-      <c r="Z49" s="292"/>
-      <c r="AA49" s="296"/>
+      <c r="R49" s="311"/>
+      <c r="S49" s="257"/>
+      <c r="T49" s="257"/>
+      <c r="U49" s="257"/>
+      <c r="V49" s="257"/>
+      <c r="W49" s="257"/>
+      <c r="X49" s="257"/>
+      <c r="Y49" s="311"/>
+      <c r="Z49" s="311"/>
+      <c r="AA49" s="285"/>
       <c r="AC49" s="59"/>
     </row>
-    <row r="50" spans="1:38">
+    <row r="50" spans="1:47">
       <c r="A50" s="58"/>
-      <c r="B50" s="225"/>
+      <c r="B50" s="223"/>
       <c r="C50" s="64"/>
       <c r="D50" s="64"/>
-      <c r="E50" s="318" t="s">
+      <c r="E50" s="297" t="s">
         <v>9</v>
       </c>
-      <c r="F50" s="319"/>
+      <c r="F50" s="300"/>
       <c r="G50" s="64"/>
-      <c r="H50" s="336" t="s">
+      <c r="H50" s="301" t="s">
         <v>333</v>
       </c>
-      <c r="I50" s="337"/>
+      <c r="I50" s="302"/>
       <c r="J50" s="64"/>
       <c r="K50" s="64"/>
       <c r="L50" s="64"/>
       <c r="M50" s="64"/>
       <c r="N50" s="64"/>
-      <c r="O50" s="226"/>
+      <c r="O50" s="224"/>
       <c r="P50" s="4"/>
-      <c r="Q50" s="297"/>
-      <c r="R50" s="293"/>
-      <c r="S50" s="293"/>
-      <c r="T50" s="293"/>
-      <c r="U50" s="293"/>
-      <c r="V50" s="293"/>
-      <c r="W50" s="293"/>
-      <c r="X50" s="293"/>
-      <c r="Y50" s="293"/>
-      <c r="Z50" s="293"/>
-      <c r="AA50" s="298"/>
+      <c r="Q50" s="286"/>
+      <c r="R50" s="257"/>
+      <c r="S50" s="257"/>
+      <c r="T50" s="257"/>
+      <c r="U50" s="257"/>
+      <c r="V50" s="257"/>
+      <c r="W50" s="257"/>
+      <c r="X50" s="257"/>
+      <c r="Y50" s="257"/>
+      <c r="Z50" s="257"/>
+      <c r="AA50" s="287"/>
       <c r="AC50" s="59"/>
     </row>
-    <row r="51" spans="1:38" ht="15" customHeight="1">
+    <row r="51" spans="1:47" ht="15" customHeight="1">
       <c r="A51" s="58"/>
-      <c r="B51" s="227"/>
-      <c r="C51" s="232"/>
-      <c r="D51" s="232"/>
-      <c r="E51" s="232"/>
-      <c r="F51" s="232"/>
-      <c r="G51" s="232"/>
-      <c r="H51" s="233"/>
-      <c r="I51" s="233"/>
-      <c r="J51" s="233"/>
-      <c r="K51" s="233"/>
-      <c r="L51" s="232"/>
-      <c r="M51" s="232"/>
-      <c r="N51" s="232"/>
-      <c r="O51" s="228"/>
+      <c r="B51" s="225"/>
+      <c r="C51" s="230"/>
+      <c r="D51" s="230"/>
+      <c r="E51" s="230"/>
+      <c r="F51" s="230"/>
+      <c r="G51" s="230"/>
+      <c r="H51" s="231"/>
+      <c r="I51" s="231"/>
+      <c r="J51" s="231"/>
+      <c r="K51" s="231"/>
+      <c r="L51" s="230"/>
+      <c r="M51" s="230"/>
+      <c r="N51" s="230"/>
+      <c r="O51" s="226"/>
       <c r="P51" s="4"/>
-      <c r="Q51" s="297"/>
-      <c r="R51" s="293"/>
-      <c r="S51" s="293"/>
-      <c r="T51" s="293"/>
-      <c r="U51" s="293"/>
-      <c r="V51" s="293"/>
-      <c r="W51" s="293"/>
-      <c r="X51" s="293"/>
-      <c r="Y51" s="293"/>
-      <c r="Z51" s="293"/>
-      <c r="AA51" s="298"/>
+      <c r="Q51" s="286"/>
+      <c r="R51" s="257"/>
+      <c r="S51" s="257"/>
+      <c r="T51" s="257"/>
+      <c r="U51" s="257"/>
+      <c r="V51" s="257"/>
+      <c r="W51" s="257"/>
+      <c r="X51" s="257"/>
+      <c r="Y51" s="257"/>
+      <c r="Z51" s="257"/>
+      <c r="AA51" s="287"/>
       <c r="AC51" s="59"/>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:47">
       <c r="A52" s="66" t="s">
         <v>294</v>
       </c>
@@ -32420,20 +32855,20 @@
       <c r="N52" s="67"/>
       <c r="O52" s="67"/>
       <c r="P52" s="67"/>
-      <c r="Q52" s="297"/>
-      <c r="R52" s="293"/>
-      <c r="S52" s="293"/>
-      <c r="T52" s="293"/>
-      <c r="U52" s="293"/>
-      <c r="V52" s="293"/>
-      <c r="W52" s="293"/>
-      <c r="X52" s="293"/>
-      <c r="Y52" s="293"/>
-      <c r="Z52" s="293"/>
-      <c r="AA52" s="298"/>
+      <c r="Q52" s="286"/>
+      <c r="R52" s="257"/>
+      <c r="S52" s="257"/>
+      <c r="T52" s="257"/>
+      <c r="U52" s="257"/>
+      <c r="V52" s="257"/>
+      <c r="W52" s="257"/>
+      <c r="X52" s="257"/>
+      <c r="Y52" s="257"/>
+      <c r="Z52" s="257"/>
+      <c r="AA52" s="287"/>
       <c r="AC52" s="59"/>
     </row>
-    <row r="53" spans="1:38">
+    <row r="53" spans="1:47">
       <c r="A53" s="58"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -32441,29 +32876,29 @@
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
       <c r="G53" s="4"/>
-      <c r="H53" s="223"/>
-      <c r="I53" s="223"/>
-      <c r="J53" s="223"/>
-      <c r="K53" s="223"/>
+      <c r="H53" s="221"/>
+      <c r="I53" s="221"/>
+      <c r="J53" s="221"/>
+      <c r="K53" s="221"/>
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
       <c r="P53" s="4"/>
-      <c r="Q53" s="297"/>
-      <c r="R53" s="293"/>
-      <c r="S53" s="293"/>
-      <c r="T53" s="293"/>
-      <c r="U53" s="293"/>
-      <c r="V53" s="293"/>
-      <c r="W53" s="293"/>
-      <c r="X53" s="293"/>
-      <c r="Y53" s="293"/>
-      <c r="Z53" s="293"/>
-      <c r="AA53" s="298"/>
+      <c r="Q53" s="286"/>
+      <c r="R53" s="257"/>
+      <c r="S53" s="257"/>
+      <c r="T53" s="257"/>
+      <c r="U53" s="257"/>
+      <c r="V53" s="257"/>
+      <c r="W53" s="257"/>
+      <c r="X53" s="257"/>
+      <c r="Y53" s="257"/>
+      <c r="Z53" s="257"/>
+      <c r="AA53" s="287"/>
       <c r="AC53" s="59"/>
     </row>
-    <row r="54" spans="1:38">
+    <row r="54" spans="1:47">
       <c r="A54" s="58"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -32471,8 +32906,8 @@
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
-      <c r="H54" s="223"/>
-      <c r="I54" s="223"/>
+      <c r="H54" s="221"/>
+      <c r="I54" s="221"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
       <c r="L54" s="4"/>
@@ -32480,20 +32915,20 @@
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
       <c r="P54" s="4"/>
-      <c r="Q54" s="297"/>
-      <c r="R54" s="293"/>
-      <c r="S54" s="293"/>
-      <c r="T54" s="293"/>
-      <c r="U54" s="293"/>
-      <c r="V54" s="293"/>
-      <c r="W54" s="293"/>
-      <c r="X54" s="293"/>
-      <c r="Y54" s="293"/>
-      <c r="Z54" s="293"/>
-      <c r="AA54" s="298"/>
+      <c r="Q54" s="286"/>
+      <c r="R54" s="257"/>
+      <c r="S54" s="257"/>
+      <c r="T54" s="257"/>
+      <c r="U54" s="257"/>
+      <c r="V54" s="257"/>
+      <c r="W54" s="257"/>
+      <c r="X54" s="257"/>
+      <c r="Y54" s="257"/>
+      <c r="Z54" s="257"/>
+      <c r="AA54" s="287"/>
       <c r="AC54" s="59"/>
     </row>
-    <row r="55" spans="1:38">
+    <row r="55" spans="1:47">
       <c r="A55" s="58"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -32501,8 +32936,8 @@
       <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
-      <c r="H55" s="223"/>
-      <c r="I55" s="223"/>
+      <c r="H55" s="221"/>
+      <c r="I55" s="221"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
       <c r="L55" s="4"/>
@@ -32510,20 +32945,20 @@
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
       <c r="P55" s="4"/>
-      <c r="Q55" s="299"/>
-      <c r="R55" s="300"/>
-      <c r="S55" s="300"/>
-      <c r="T55" s="300"/>
-      <c r="U55" s="300"/>
-      <c r="V55" s="300"/>
-      <c r="W55" s="300"/>
-      <c r="X55" s="300"/>
-      <c r="Y55" s="300"/>
-      <c r="Z55" s="300"/>
-      <c r="AA55" s="301"/>
+      <c r="Q55" s="318"/>
+      <c r="R55" s="319"/>
+      <c r="S55" s="319"/>
+      <c r="T55" s="319"/>
+      <c r="U55" s="319"/>
+      <c r="V55" s="319"/>
+      <c r="W55" s="319"/>
+      <c r="X55" s="319"/>
+      <c r="Y55" s="319"/>
+      <c r="Z55" s="319"/>
+      <c r="AA55" s="320"/>
       <c r="AC55" s="59"/>
     </row>
-    <row r="56" spans="1:38" ht="16" thickBot="1">
+    <row r="56" spans="1:47" ht="16" thickBot="1">
       <c r="A56" s="61"/>
       <c r="B56" s="62"/>
       <c r="C56" s="62"/>
@@ -32531,8 +32966,8 @@
       <c r="E56" s="62"/>
       <c r="F56" s="62"/>
       <c r="G56" s="62"/>
-      <c r="H56" s="224"/>
-      <c r="I56" s="224"/>
+      <c r="H56" s="222"/>
+      <c r="I56" s="222"/>
       <c r="J56" s="62"/>
       <c r="K56" s="62"/>
       <c r="L56" s="62"/>
@@ -32554,12 +32989,12 @@
       <c r="AB56" s="62"/>
       <c r="AC56" s="63"/>
     </row>
-    <row r="57" spans="1:38">
-      <c r="A57" s="338" t="s">
+    <row r="57" spans="1:47">
+      <c r="A57" s="255" t="s">
         <v>344</v>
       </c>
-      <c r="B57" s="339"/>
-      <c r="C57" s="339"/>
+      <c r="B57" s="256"/>
+      <c r="C57" s="256"/>
       <c r="D57" s="56"/>
       <c r="E57" s="56"/>
       <c r="F57" s="56"/>
@@ -32574,94 +33009,114 @@
       <c r="O57" s="56"/>
       <c r="P57" s="56"/>
     </row>
-    <row r="58" spans="1:38">
+    <row r="58" spans="1:47">
       <c r="A58" s="58"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="1:38" ht="15" customHeight="1">
+    <row r="59" spans="1:47" ht="15" customHeight="1">
       <c r="A59" s="58"/>
-      <c r="B59" s="333" t="s">
+      <c r="B59" s="268" t="s">
         <v>301</v>
       </c>
-      <c r="C59" s="334"/>
-    </row>
-    <row r="60" spans="1:38" ht="16" customHeight="1" thickBot="1">
+      <c r="C59" s="299"/>
+    </row>
+    <row r="60" spans="1:47" ht="16" customHeight="1" thickBot="1">
       <c r="A60" s="60" t="s">
         <v>293</v>
       </c>
-      <c r="B60" s="334"/>
-      <c r="C60" s="335"/>
-      <c r="L60" s="257"/>
-    </row>
-    <row r="61" spans="1:38" ht="15" customHeight="1">
+      <c r="B60" s="299"/>
+      <c r="C60" s="271"/>
+      <c r="L60" s="250"/>
+    </row>
+    <row r="61" spans="1:47" ht="15" customHeight="1">
       <c r="B61" s="38"/>
       <c r="C61" s="68"/>
-      <c r="N61" s="268" t="s">
+      <c r="N61" s="365" t="s">
         <v>729</v>
       </c>
-      <c r="O61" s="269"/>
-      <c r="P61" s="270"/>
-      <c r="S61" s="71"/>
-      <c r="T61" s="71"/>
+      <c r="O61" s="366"/>
+      <c r="P61" s="367"/>
+      <c r="Q61" s="358"/>
+      <c r="R61" s="358"/>
+      <c r="S61" s="359"/>
+      <c r="T61" s="359"/>
       <c r="U61" s="71"/>
-      <c r="V61" s="268" t="s">
+      <c r="V61" s="334" t="s">
         <v>713</v>
       </c>
-      <c r="W61" s="269"/>
-      <c r="X61" s="270"/>
+      <c r="W61" s="335"/>
+      <c r="X61" s="336"/>
       <c r="AA61" s="71"/>
       <c r="AB61" s="71"/>
-      <c r="AE61" s="268" t="s">
+      <c r="AE61" s="334" t="s">
         <v>730</v>
       </c>
-      <c r="AF61" s="269"/>
-      <c r="AG61" s="270"/>
+      <c r="AF61" s="335"/>
+      <c r="AG61" s="336"/>
       <c r="AJ61" s="71"/>
       <c r="AK61" s="71"/>
-    </row>
-    <row r="62" spans="1:38" ht="15" customHeight="1" thickBot="1">
-      <c r="B62" s="333" t="s">
+      <c r="AO61" s="365" t="s">
+        <v>729</v>
+      </c>
+      <c r="AP61" s="366"/>
+      <c r="AQ61" s="367"/>
+      <c r="AR61" s="358"/>
+      <c r="AS61" s="358"/>
+      <c r="AT61" s="359"/>
+      <c r="AU61" s="359"/>
+    </row>
+    <row r="62" spans="1:47" ht="15" customHeight="1" thickBot="1">
+      <c r="B62" s="268" t="s">
         <v>338</v>
       </c>
-      <c r="C62" s="342"/>
-      <c r="N62" s="271"/>
-      <c r="O62" s="272"/>
-      <c r="P62" s="273"/>
-      <c r="S62" s="71"/>
-      <c r="T62" s="71"/>
+      <c r="C62" s="269"/>
+      <c r="N62" s="368"/>
+      <c r="O62" s="369"/>
+      <c r="P62" s="370"/>
+      <c r="Q62" s="358"/>
+      <c r="R62" s="358"/>
+      <c r="S62" s="359"/>
+      <c r="T62" s="359"/>
       <c r="U62" s="71"/>
-      <c r="V62" s="271"/>
-      <c r="W62" s="272"/>
-      <c r="X62" s="273"/>
+      <c r="V62" s="337"/>
+      <c r="W62" s="338"/>
+      <c r="X62" s="339"/>
       <c r="AA62" s="71"/>
       <c r="AB62" s="71"/>
-      <c r="AE62" s="271"/>
-      <c r="AF62" s="272"/>
-      <c r="AG62" s="273"/>
+      <c r="AE62" s="337"/>
+      <c r="AF62" s="338"/>
+      <c r="AG62" s="339"/>
       <c r="AJ62" s="71"/>
       <c r="AK62" s="71"/>
-    </row>
-    <row r="63" spans="1:38" ht="61" thickBot="1">
-      <c r="B63" s="343"/>
-      <c r="C63" s="335"/>
-      <c r="N63" s="208"/>
-      <c r="O63" s="253" t="s">
+      <c r="AO62" s="368"/>
+      <c r="AP62" s="369"/>
+      <c r="AQ62" s="370"/>
+      <c r="AR62" s="358"/>
+      <c r="AS62" s="358"/>
+      <c r="AT62" s="359"/>
+      <c r="AU62" s="359"/>
+    </row>
+    <row r="63" spans="1:47" ht="61" thickBot="1">
+      <c r="B63" s="270"/>
+      <c r="C63" s="271"/>
+      <c r="N63" s="360"/>
+      <c r="O63" s="361" t="s">
         <v>700</v>
       </c>
-      <c r="P63" s="253" t="s">
+      <c r="P63" s="361" t="s">
         <v>176</v>
       </c>
-      <c r="Q63" s="253" t="s">
+      <c r="Q63" s="362" t="s">
         <v>131</v>
       </c>
-      <c r="R63" s="253" t="s">
+      <c r="R63" s="362" t="s">
         <v>155</v>
       </c>
-      <c r="S63" s="253" t="s">
+      <c r="S63" s="362" t="s">
         <v>152</v>
       </c>
-      <c r="T63" s="253" t="s">
+      <c r="T63" s="362" t="s">
         <v>701</v>
       </c>
       <c r="U63" s="204"/>
@@ -32687,29 +33142,48 @@
         <v>701</v>
       </c>
       <c r="AE63" s="208"/>
-      <c r="AF63" s="253" t="s">
+      <c r="AF63" s="246" t="s">
         <v>731</v>
       </c>
-      <c r="AG63" s="253" t="s">
+      <c r="AG63" s="246" t="s">
         <v>52</v>
       </c>
-      <c r="AH63" s="253" t="s">
+      <c r="AH63" s="246" t="s">
         <v>739</v>
       </c>
-      <c r="AI63" s="253" t="s">
+      <c r="AI63" s="246" t="s">
         <v>155</v>
       </c>
-      <c r="AJ63" s="253" t="s">
+      <c r="AJ63" s="246" t="s">
         <v>732</v>
       </c>
-      <c r="AK63" s="253" t="s">
+      <c r="AK63" s="246" t="s">
         <v>733</v>
       </c>
-      <c r="AL63" s="253" t="s">
+      <c r="AL63" s="246" t="s">
         <v>701</v>
       </c>
-    </row>
-    <row r="64" spans="1:38" ht="55" customHeight="1" thickBot="1">
+      <c r="AO63" s="360"/>
+      <c r="AP63" s="361" t="s">
+        <v>700</v>
+      </c>
+      <c r="AQ63" s="361" t="s">
+        <v>176</v>
+      </c>
+      <c r="AR63" s="362" t="s">
+        <v>741</v>
+      </c>
+      <c r="AS63" s="362" t="s">
+        <v>742</v>
+      </c>
+      <c r="AT63" s="362" t="s">
+        <v>152</v>
+      </c>
+      <c r="AU63" s="398" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="64" spans="1:47" ht="55" customHeight="1" thickBot="1">
       <c r="B64" s="38"/>
       <c r="C64" s="68"/>
       <c r="E64" s="69"/>
@@ -32720,25 +33194,25 @@
       <c r="J64" s="69"/>
       <c r="K64" s="69"/>
       <c r="L64" s="70"/>
-      <c r="N64" s="210" t="s">
+      <c r="N64" s="360" t="s">
         <v>728</v>
       </c>
-      <c r="O64" s="211">
+      <c r="O64" s="363">
         <v>0.21</v>
       </c>
-      <c r="P64" s="211">
+      <c r="P64" s="363">
         <v>0.01</v>
       </c>
-      <c r="Q64" s="211">
+      <c r="Q64" s="363">
         <v>0.49</v>
       </c>
-      <c r="R64" s="211">
+      <c r="R64" s="363">
         <v>0.87</v>
       </c>
-      <c r="S64" s="211">
+      <c r="S64" s="363">
         <v>0.01</v>
       </c>
-      <c r="T64" s="211">
+      <c r="T64" s="363">
         <v>0.4</v>
       </c>
       <c r="U64" s="206"/>
@@ -32787,91 +33261,133 @@
       <c r="AL64" s="211">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="65" spans="2:40" ht="44" customHeight="1" thickBot="1">
-      <c r="B65" s="322" t="s">
+      <c r="AO64" s="360" t="s">
+        <v>728</v>
+      </c>
+      <c r="AP64" s="363">
+        <v>0.21</v>
+      </c>
+      <c r="AQ64" s="363">
+        <v>0.01</v>
+      </c>
+      <c r="AR64" s="363">
+        <v>0.49</v>
+      </c>
+      <c r="AS64" s="363">
+        <v>0.87</v>
+      </c>
+      <c r="AT64" s="363">
+        <v>0.01</v>
+      </c>
+      <c r="AU64" s="399">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="65" spans="2:47" ht="44" customHeight="1" thickBot="1">
+      <c r="B65" s="290" t="s">
         <v>336</v>
       </c>
-      <c r="C65" s="328"/>
+      <c r="C65" s="295"/>
       <c r="D65" s="47"/>
-      <c r="E65" s="329" t="s">
+      <c r="E65" s="264" t="s">
         <v>339</v>
       </c>
-      <c r="F65" s="330"/>
-      <c r="G65" s="330"/>
-      <c r="H65" s="330"/>
-      <c r="I65" s="330"/>
-      <c r="J65" s="330"/>
-      <c r="K65" s="330"/>
-      <c r="L65" s="331"/>
+      <c r="F65" s="296"/>
+      <c r="G65" s="296"/>
+      <c r="H65" s="296"/>
+      <c r="I65" s="296"/>
+      <c r="J65" s="296"/>
+      <c r="K65" s="296"/>
+      <c r="L65" s="265"/>
       <c r="M65" s="47"/>
-      <c r="N65" s="214" t="s">
+      <c r="N65" s="364" t="s">
         <v>726</v>
       </c>
-      <c r="O65" s="246">
+      <c r="O65" s="371">
         <v>0.22370000000000001</v>
       </c>
-      <c r="P65" s="264">
+      <c r="P65" s="372">
         <v>2.7400000000000001E-2</v>
       </c>
-      <c r="Q65" s="212">
+      <c r="Q65" s="371">
         <v>0.43380000000000002</v>
       </c>
-      <c r="R65" s="246">
+      <c r="R65" s="371">
         <v>0.92589999999999995</v>
       </c>
-      <c r="S65" s="264">
+      <c r="S65" s="372">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="T65" s="371">
+        <v>0.376</v>
+      </c>
+      <c r="U65" s="206"/>
+      <c r="V65" s="213" t="s">
+        <v>703</v>
+      </c>
+      <c r="W65" s="240">
+        <v>0.224</v>
+      </c>
+      <c r="X65" s="385">
+        <v>2.7E-2</v>
+      </c>
+      <c r="Y65" s="386">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="Z65" s="240">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="AA65" s="385">
         <v>2.1700000000000001E-3</v>
       </c>
-      <c r="T65" s="246">
-        <v>0.376</v>
-      </c>
-      <c r="U65" s="206"/>
-      <c r="V65" s="214" t="s">
-        <v>703</v>
-      </c>
-      <c r="W65" s="246">
-        <v>0.224</v>
-      </c>
-      <c r="X65" s="264">
-        <v>2.7E-2</v>
-      </c>
-      <c r="Y65" s="212">
-        <v>0.46400000000000002</v>
-      </c>
-      <c r="Z65" s="247">
-        <v>0.82699999999999996</v>
-      </c>
-      <c r="AA65" s="264">
-        <v>2.1700000000000001E-3</v>
-      </c>
-      <c r="AB65" s="246">
+      <c r="AB65" s="240">
         <v>0.34699999999999998</v>
       </c>
-      <c r="AE65" s="214" t="s">
+      <c r="AE65" s="213" t="s">
         <v>726</v>
       </c>
-      <c r="AF65" s="246">
+      <c r="AF65" s="239">
         <v>0.14799999999999999</v>
       </c>
-      <c r="AG65" s="252">
+      <c r="AG65" s="245">
         <v>1</v>
       </c>
       <c r="AH65" s="212">
         <v>0.41399999999999998</v>
       </c>
-      <c r="AI65" s="246">
+      <c r="AI65" s="239">
         <v>0.92589999999999995</v>
       </c>
-      <c r="AJ65" s="264">
+      <c r="AJ65" s="321">
         <v>2.1700000000000001E-3</v>
       </c>
-      <c r="AK65" s="246"/>
-      <c r="AL65" s="246">
+      <c r="AK65" s="239"/>
+      <c r="AL65" s="239">
         <v>0.39419999999999999</v>
       </c>
-    </row>
-    <row r="66" spans="2:40" ht="76" thickBot="1">
+      <c r="AO65" s="397" t="s">
+        <v>743</v>
+      </c>
+      <c r="AP65" s="400">
+        <v>0.22370000000000001</v>
+      </c>
+      <c r="AQ65" s="401">
+        <v>2.7400000000000001E-2</v>
+      </c>
+      <c r="AR65" s="400">
+        <v>0.43380000000000002</v>
+      </c>
+      <c r="AS65" s="400">
+        <v>0.92589999999999995</v>
+      </c>
+      <c r="AT65" s="401">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="AU65" s="402">
+        <v>0.376</v>
+      </c>
+    </row>
+    <row r="66" spans="2:47" ht="76" thickBot="1">
       <c r="B66" s="38"/>
       <c r="C66" s="68"/>
       <c r="E66" s="69"/>
@@ -32885,64 +33401,68 @@
       <c r="N66" s="208" t="s">
         <v>727</v>
       </c>
-      <c r="O66" s="254">
+      <c r="O66" s="373">
         <v>0.41049999999999998</v>
       </c>
-      <c r="P66" s="265"/>
-      <c r="Q66" s="254">
+      <c r="P66" s="374">
+        <v>2.7400000000000001E-2</v>
+      </c>
+      <c r="Q66" s="373">
         <v>0.65439999999999998</v>
       </c>
-      <c r="R66" s="255">
+      <c r="R66" s="373">
         <v>1</v>
       </c>
-      <c r="S66" s="265"/>
-      <c r="T66" s="254">
+      <c r="S66" s="374">
+        <v>2.1700000000000001E-3</v>
+      </c>
+      <c r="T66" s="373">
         <v>0.36919999999999997</v>
       </c>
       <c r="U66" s="207"/>
       <c r="V66" s="210" t="s">
         <v>704</v>
       </c>
-      <c r="W66" s="213">
+      <c r="W66" s="211">
         <v>0.41</v>
       </c>
-      <c r="X66" s="263"/>
-      <c r="Y66" s="213">
+      <c r="X66" s="387"/>
+      <c r="Y66" s="211">
         <v>0.69899999999999995</v>
       </c>
       <c r="Z66" s="211">
         <v>1</v>
       </c>
-      <c r="AA66" s="265"/>
-      <c r="AB66" s="213">
+      <c r="AA66" s="387"/>
+      <c r="AB66" s="211">
         <v>0.36940000000000001</v>
       </c>
       <c r="AE66" s="208" t="s">
         <v>738</v>
       </c>
-      <c r="AF66" s="254">
+      <c r="AF66" s="247">
         <v>0.23</v>
       </c>
-      <c r="AG66" s="256">
+      <c r="AG66" s="249">
         <v>1</v>
       </c>
-      <c r="AH66" s="254">
+      <c r="AH66" s="247">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="AI66" s="255">
+      <c r="AI66" s="248">
         <v>1</v>
       </c>
-      <c r="AJ66" s="265"/>
-      <c r="AK66" s="254"/>
-      <c r="AL66" s="254">
+      <c r="AJ66" s="323"/>
+      <c r="AK66" s="247"/>
+      <c r="AL66" s="247">
         <v>0.36399999999999999</v>
       </c>
     </row>
-    <row r="67" spans="2:40" ht="14" customHeight="1" thickBot="1">
-      <c r="B67" s="322" t="s">
+    <row r="67" spans="2:47" ht="14" customHeight="1" thickBot="1">
+      <c r="B67" s="290" t="s">
         <v>337</v>
       </c>
-      <c r="C67" s="323"/>
+      <c r="C67" s="291"/>
       <c r="E67" s="69"/>
       <c r="F67" s="69"/>
       <c r="G67" s="69"/>
@@ -32966,19 +33486,19 @@
       <c r="Z67" s="17"/>
       <c r="AA67" s="71"/>
       <c r="AB67" s="207"/>
-      <c r="AE67" s="262" t="s">
+      <c r="AE67" s="353" t="s">
         <v>734</v>
       </c>
-      <c r="AH67" s="264">
+      <c r="AH67" s="321">
         <v>0.34</v>
       </c>
-      <c r="AL67" s="266">
+      <c r="AL67" s="354">
         <v>0.39300000000000002</v>
       </c>
     </row>
-    <row r="68" spans="2:40" ht="55" customHeight="1" thickBot="1">
-      <c r="B68" s="324"/>
-      <c r="C68" s="325"/>
+    <row r="68" spans="2:47" ht="55" customHeight="1" thickBot="1">
+      <c r="B68" s="258"/>
+      <c r="C68" s="292"/>
       <c r="E68" s="70"/>
       <c r="F68" s="70"/>
       <c r="G68" s="70"/>
@@ -32987,7 +33507,7 @@
       <c r="J68" s="70"/>
       <c r="K68" s="70"/>
       <c r="L68" s="70"/>
-      <c r="N68" s="220" t="s">
+      <c r="N68" s="218" t="s">
         <v>710</v>
       </c>
       <c r="O68" s="209" t="s">
@@ -33009,7 +33529,7 @@
         <v>701</v>
       </c>
       <c r="U68" s="207"/>
-      <c r="V68" s="220" t="s">
+      <c r="V68" s="218" t="s">
         <v>711</v>
       </c>
       <c r="W68" s="209" t="s">
@@ -33030,13 +33550,13 @@
       <c r="AB68" s="209" t="s">
         <v>701</v>
       </c>
-      <c r="AE68" s="263"/>
-      <c r="AH68" s="265"/>
-      <c r="AL68" s="267"/>
-    </row>
-    <row r="69" spans="2:40" ht="16" thickBot="1">
-      <c r="B69" s="326"/>
-      <c r="C69" s="327"/>
+      <c r="AE68" s="322"/>
+      <c r="AH68" s="323"/>
+      <c r="AL68" s="355"/>
+    </row>
+    <row r="69" spans="2:47" ht="16" thickBot="1">
+      <c r="B69" s="293"/>
+      <c r="C69" s="294"/>
       <c r="N69" s="210" t="s">
         <v>702</v>
       </c>
@@ -33080,108 +33600,108 @@
       <c r="AB69" s="211">
         <v>0.4</v>
       </c>
-      <c r="AE69" s="262" t="s">
+      <c r="AE69" s="353" t="s">
         <v>735</v>
       </c>
-      <c r="AH69" s="264">
+      <c r="AH69" s="321">
         <v>9.8000000000000004E-2</v>
       </c>
-      <c r="AL69" s="266">
+      <c r="AL69" s="354">
         <v>0.378</v>
       </c>
     </row>
-    <row r="70" spans="2:40" ht="31" thickBot="1">
-      <c r="N70" s="215" t="s">
+    <row r="70" spans="2:47" ht="31" thickBot="1">
+      <c r="N70" s="214" t="s">
         <v>703</v>
       </c>
-      <c r="O70" s="239">
+      <c r="O70" s="234">
         <v>0.23769999999999999</v>
       </c>
-      <c r="P70" s="274">
+      <c r="P70" s="375">
         <v>4.5699999999999998E-2</v>
       </c>
-      <c r="Q70" s="234"/>
-      <c r="R70" s="235"/>
-      <c r="S70" s="274">
+      <c r="Q70" s="376"/>
+      <c r="R70" s="377"/>
+      <c r="S70" s="375">
         <v>2.1700000000000001E-3</v>
       </c>
-      <c r="T70" s="239">
+      <c r="T70" s="234">
         <v>0.3478</v>
       </c>
       <c r="U70" s="206"/>
-      <c r="V70" s="242" t="s">
+      <c r="V70" s="235" t="s">
         <v>703</v>
       </c>
-      <c r="W70" s="248"/>
-      <c r="X70" s="279"/>
-      <c r="Y70" s="216">
+      <c r="W70" s="241"/>
+      <c r="X70" s="340"/>
+      <c r="Y70" s="388">
         <v>0.438</v>
       </c>
-      <c r="Z70" s="239">
+      <c r="Z70" s="234">
         <v>0.92589999999999995</v>
       </c>
-      <c r="AA70" s="279"/>
-      <c r="AB70" s="239">
+      <c r="AA70" s="389"/>
+      <c r="AB70" s="234">
         <v>0.376</v>
       </c>
-      <c r="AE70" s="263"/>
-      <c r="AH70" s="265"/>
-      <c r="AL70" s="267"/>
-    </row>
-    <row r="71" spans="2:40" ht="15" customHeight="1" thickBot="1">
-      <c r="N71" s="217"/>
-      <c r="O71" s="217"/>
-      <c r="P71" s="275"/>
-      <c r="Q71" s="236"/>
-      <c r="R71" s="237"/>
-      <c r="S71" s="277"/>
-      <c r="T71" s="217"/>
+      <c r="AE70" s="322"/>
+      <c r="AH70" s="323"/>
+      <c r="AL70" s="355"/>
+    </row>
+    <row r="71" spans="2:47" ht="15" customHeight="1" thickBot="1">
+      <c r="N71" s="215"/>
+      <c r="O71" s="378"/>
+      <c r="P71" s="379"/>
+      <c r="Q71" s="232"/>
+      <c r="R71" s="380"/>
+      <c r="S71" s="379"/>
+      <c r="T71" s="378"/>
       <c r="U71" s="207"/>
-      <c r="V71" s="244"/>
-      <c r="W71" s="244"/>
-      <c r="X71" s="280"/>
-      <c r="Y71" s="218"/>
-      <c r="Z71" s="217"/>
-      <c r="AA71" s="282"/>
-      <c r="AB71" s="217"/>
-    </row>
-    <row r="72" spans="2:40" ht="46" thickBot="1">
-      <c r="N72" s="217" t="s">
+      <c r="V71" s="237"/>
+      <c r="W71" s="237"/>
+      <c r="X71" s="341"/>
+      <c r="Y71" s="217"/>
+      <c r="Z71" s="378"/>
+      <c r="AA71" s="390"/>
+      <c r="AB71" s="378"/>
+    </row>
+    <row r="72" spans="2:47" ht="46" thickBot="1">
+      <c r="N72" s="215" t="s">
         <v>704</v>
       </c>
-      <c r="O72" s="218">
+      <c r="O72" s="217">
         <v>0.43630000000000002</v>
       </c>
-      <c r="P72" s="276"/>
-      <c r="Q72" s="236"/>
-      <c r="R72" s="238"/>
-      <c r="S72" s="278"/>
-      <c r="T72" s="218">
+      <c r="P72" s="381"/>
+      <c r="Q72" s="232"/>
+      <c r="R72" s="232"/>
+      <c r="S72" s="381"/>
+      <c r="T72" s="217">
         <v>0.36980000000000002</v>
       </c>
       <c r="U72" s="205"/>
-      <c r="V72" s="244" t="s">
+      <c r="V72" s="237" t="s">
         <v>704</v>
       </c>
-      <c r="W72" s="243"/>
-      <c r="X72" s="281"/>
-      <c r="Y72" s="218">
+      <c r="W72" s="236"/>
+      <c r="X72" s="342"/>
+      <c r="Y72" s="217">
         <v>0.65400000000000003</v>
       </c>
-      <c r="Z72" s="219">
+      <c r="Z72" s="217">
         <v>1</v>
       </c>
-      <c r="AA72" s="283"/>
-      <c r="AB72" s="218">
+      <c r="AA72" s="391"/>
+      <c r="AB72" s="217">
         <v>0.36899999999999999</v>
       </c>
-      <c r="AF72" s="350" t="s">
+      <c r="AF72" s="347" t="s">
         <v>724</v>
       </c>
-      <c r="AG72" s="351"/>
-      <c r="AH72" s="352"/>
-    </row>
-    <row r="73" spans="2:40" ht="16" customHeight="1" thickBot="1">
+      <c r="AG72" s="348"/>
+      <c r="AH72" s="349"/>
+    </row>
+    <row r="73" spans="2:47" ht="16" customHeight="1" thickBot="1">
       <c r="N73" s="17"/>
       <c r="O73" s="17"/>
       <c r="P73" s="17"/>
@@ -33192,12 +33712,12 @@
       <c r="U73" s="205"/>
       <c r="V73" s="205"/>
       <c r="W73" s="205"/>
-      <c r="AF73" s="353"/>
-      <c r="AG73" s="354"/>
-      <c r="AH73" s="355"/>
-    </row>
-    <row r="74" spans="2:40" ht="46" thickBot="1">
-      <c r="N74" s="220" t="s">
+      <c r="AF73" s="350"/>
+      <c r="AG73" s="351"/>
+      <c r="AH73" s="352"/>
+    </row>
+    <row r="74" spans="2:47" ht="46" thickBot="1">
+      <c r="N74" s="218" t="s">
         <v>706</v>
       </c>
       <c r="O74" s="209" t="s">
@@ -33219,7 +33739,7 @@
         <v>701</v>
       </c>
       <c r="U74" s="205"/>
-      <c r="V74" s="220" t="s">
+      <c r="V74" s="218" t="s">
         <v>714</v>
       </c>
       <c r="W74" s="209" t="s">
@@ -33240,10 +33760,10 @@
       <c r="AB74" s="209" t="s">
         <v>701</v>
       </c>
-      <c r="AC74" s="249" t="s">
+      <c r="AC74" s="242" t="s">
         <v>719</v>
       </c>
-      <c r="AF74" s="220" t="s">
+      <c r="AF74" s="218" t="s">
         <v>720</v>
       </c>
       <c r="AG74" s="209" t="s">
@@ -33265,7 +33785,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="75" spans="2:40" ht="16" thickBot="1">
+    <row r="75" spans="2:47" ht="16" thickBot="1">
       <c r="N75" s="210" t="s">
         <v>702</v>
       </c>
@@ -33309,9 +33829,9 @@
       <c r="AB75" s="211">
         <v>0.4</v>
       </c>
-      <c r="AC75" s="250"/>
-      <c r="AD75" s="250"/>
-      <c r="AE75" s="250"/>
+      <c r="AC75" s="243"/>
+      <c r="AD75" s="243"/>
+      <c r="AE75" s="243"/>
       <c r="AF75" s="210" t="s">
         <v>702</v>
       </c>
@@ -33333,146 +33853,146 @@
       <c r="AL75" s="211">
         <v>0.4</v>
       </c>
-      <c r="AM75" s="250"/>
-      <c r="AN75" s="251" t="s">
+      <c r="AM75" s="243"/>
+      <c r="AN75" s="244" t="s">
         <v>722</v>
       </c>
     </row>
-    <row r="76" spans="2:40" ht="30">
-      <c r="N76" s="215" t="s">
+    <row r="76" spans="2:47" ht="30">
+      <c r="N76" s="214" t="s">
         <v>703</v>
       </c>
-      <c r="O76" s="240">
+      <c r="O76" s="234">
         <v>0.22</v>
       </c>
-      <c r="P76" s="274">
+      <c r="P76" s="375">
         <v>3.3399999999999999E-2</v>
       </c>
-      <c r="Q76" s="234"/>
-      <c r="R76" s="235"/>
-      <c r="S76" s="274">
+      <c r="Q76" s="376"/>
+      <c r="R76" s="377"/>
+      <c r="S76" s="375">
         <v>2.1700000000000001E-3</v>
       </c>
-      <c r="T76" s="239">
+      <c r="T76" s="234">
         <v>0.34599999999999997</v>
       </c>
       <c r="U76" s="17"/>
-      <c r="V76" s="242" t="s">
+      <c r="V76" s="235" t="s">
         <v>703</v>
       </c>
-      <c r="W76" s="248"/>
-      <c r="X76" s="279"/>
-      <c r="Y76" s="216">
+      <c r="W76" s="241"/>
+      <c r="X76" s="340"/>
+      <c r="Y76" s="388">
         <v>0.46700000000000003</v>
       </c>
-      <c r="Z76" s="239">
+      <c r="Z76" s="234">
         <v>0.59699999999999998</v>
       </c>
-      <c r="AA76" s="279"/>
-      <c r="AB76" s="367">
+      <c r="AA76" s="389"/>
+      <c r="AB76" s="392">
         <v>0.28289999999999998</v>
       </c>
-      <c r="AF76" s="242" t="s">
+      <c r="AF76" s="235" t="s">
         <v>703</v>
       </c>
-      <c r="AG76" s="239">
+      <c r="AG76" s="233">
         <v>0.22339999999999999</v>
       </c>
-      <c r="AH76" s="274">
+      <c r="AH76" s="313">
         <v>3.3399999999999999E-2</v>
       </c>
-      <c r="AI76" s="216">
+      <c r="AI76" s="395">
         <v>0.46700000000000003</v>
       </c>
-      <c r="AJ76" s="239">
+      <c r="AJ76" s="233">
         <v>0.59699999999999998</v>
       </c>
-      <c r="AK76" s="274">
+      <c r="AK76" s="313">
         <v>2.1700000000000001E-3</v>
       </c>
-      <c r="AL76" s="239">
+      <c r="AL76" s="233">
         <v>0.28100000000000003</v>
       </c>
-      <c r="AN76" s="239">
+      <c r="AN76" s="233">
         <v>0.28100000000000003</v>
       </c>
     </row>
-    <row r="77" spans="2:40" ht="16" thickBot="1">
-      <c r="N77" s="217"/>
-      <c r="O77" s="217"/>
-      <c r="P77" s="277"/>
-      <c r="Q77" s="236"/>
-      <c r="R77" s="237"/>
-      <c r="S77" s="277"/>
-      <c r="T77" s="217"/>
+    <row r="77" spans="2:47" ht="16" thickBot="1">
+      <c r="N77" s="215"/>
+      <c r="O77" s="378"/>
+      <c r="P77" s="379"/>
+      <c r="Q77" s="232"/>
+      <c r="R77" s="380"/>
+      <c r="S77" s="379"/>
+      <c r="T77" s="378"/>
       <c r="U77" s="17"/>
-      <c r="V77" s="244"/>
-      <c r="W77" s="244"/>
-      <c r="X77" s="280"/>
-      <c r="Y77" s="218"/>
-      <c r="Z77" s="217"/>
-      <c r="AA77" s="282"/>
-      <c r="AB77" s="217"/>
-      <c r="AF77" s="244"/>
-      <c r="AG77" s="217"/>
-      <c r="AH77" s="275"/>
-      <c r="AI77" s="218"/>
-      <c r="AJ77" s="217"/>
-      <c r="AK77" s="277"/>
-      <c r="AL77" s="217"/>
-      <c r="AN77" s="217"/>
-    </row>
-    <row r="78" spans="2:40" ht="46" thickBot="1">
-      <c r="N78" s="217" t="s">
+      <c r="V77" s="237"/>
+      <c r="W77" s="237"/>
+      <c r="X77" s="341"/>
+      <c r="Y77" s="217"/>
+      <c r="Z77" s="378"/>
+      <c r="AA77" s="390"/>
+      <c r="AB77" s="378"/>
+      <c r="AF77" s="237"/>
+      <c r="AG77" s="215"/>
+      <c r="AH77" s="316"/>
+      <c r="AI77" s="396"/>
+      <c r="AJ77" s="215"/>
+      <c r="AK77" s="314"/>
+      <c r="AL77" s="215"/>
+      <c r="AN77" s="215"/>
+    </row>
+    <row r="78" spans="2:47" ht="46" thickBot="1">
+      <c r="N78" s="215" t="s">
         <v>704</v>
       </c>
-      <c r="O78" s="218">
+      <c r="O78" s="217">
         <v>0.41</v>
       </c>
-      <c r="P78" s="278"/>
-      <c r="Q78" s="236"/>
-      <c r="R78" s="238"/>
-      <c r="S78" s="278"/>
-      <c r="T78" s="218">
+      <c r="P78" s="381"/>
+      <c r="Q78" s="232"/>
+      <c r="R78" s="232"/>
+      <c r="S78" s="381"/>
+      <c r="T78" s="217">
         <v>0.36799999999999999</v>
       </c>
       <c r="U78" s="17"/>
-      <c r="V78" s="244" t="s">
+      <c r="V78" s="237" t="s">
         <v>704</v>
       </c>
-      <c r="W78" s="243"/>
-      <c r="X78" s="281"/>
-      <c r="Y78" s="218">
+      <c r="W78" s="236"/>
+      <c r="X78" s="342"/>
+      <c r="Y78" s="217">
         <v>0.70399999999999996</v>
       </c>
-      <c r="Z78" s="219">
+      <c r="Z78" s="217">
         <v>1</v>
       </c>
-      <c r="AA78" s="283"/>
-      <c r="AB78" s="218">
+      <c r="AA78" s="391"/>
+      <c r="AB78" s="217">
         <v>0.37</v>
       </c>
-      <c r="AF78" s="244" t="s">
+      <c r="AF78" s="237" t="s">
         <v>704</v>
       </c>
-      <c r="AG78" s="218">
+      <c r="AG78" s="216">
         <v>0.41</v>
       </c>
-      <c r="AH78" s="276"/>
-      <c r="AI78" s="218">
+      <c r="AH78" s="317"/>
+      <c r="AI78" s="216">
         <v>0.70469999999999999</v>
       </c>
-      <c r="AJ78" s="219">
+      <c r="AJ78" s="217">
         <v>1</v>
       </c>
-      <c r="AK78" s="278"/>
-      <c r="AL78" s="218">
+      <c r="AK78" s="315"/>
+      <c r="AL78" s="216">
         <v>0.36799999999999999</v>
       </c>
     </row>
-    <row r="79" spans="2:40" ht="16" thickBot="1"/>
-    <row r="80" spans="2:40" ht="46" thickBot="1">
-      <c r="N80" s="220" t="s">
+    <row r="79" spans="2:47" ht="16" thickBot="1"/>
+    <row r="80" spans="2:47" ht="46" thickBot="1">
+      <c r="N80" s="218" t="s">
         <v>705</v>
       </c>
       <c r="O80" s="209" t="s">
@@ -33493,7 +34013,7 @@
       <c r="T80" s="209" t="s">
         <v>701</v>
       </c>
-      <c r="V80" s="220" t="s">
+      <c r="V80" s="218" t="s">
         <v>717</v>
       </c>
       <c r="W80" s="209" t="s">
@@ -33514,10 +34034,10 @@
       <c r="AB80" s="209" t="s">
         <v>701</v>
       </c>
-      <c r="AC80" s="249" t="s">
+      <c r="AC80" s="242" t="s">
         <v>718</v>
       </c>
-      <c r="AF80" s="220" t="s">
+      <c r="AF80" s="218" t="s">
         <v>721</v>
       </c>
       <c r="AG80" s="209" t="s">
@@ -33561,7 +34081,7 @@
       <c r="T81" s="211">
         <v>0.4</v>
       </c>
-      <c r="U81" s="250"/>
+      <c r="U81" s="243"/>
       <c r="V81" s="210" t="s">
         <v>702</v>
       </c>
@@ -33583,9 +34103,9 @@
       <c r="AB81" s="211">
         <v>0.4</v>
       </c>
-      <c r="AC81" s="250"/>
-      <c r="AD81" s="250"/>
-      <c r="AE81" s="250"/>
+      <c r="AC81" s="243"/>
+      <c r="AD81" s="243"/>
+      <c r="AE81" s="243"/>
       <c r="AF81" s="210" t="s">
         <v>702</v>
       </c>
@@ -33607,143 +34127,143 @@
       <c r="AL81" s="211">
         <v>0.4</v>
       </c>
-      <c r="AM81" s="250"/>
-      <c r="AN81" s="251" t="s">
+      <c r="AM81" s="243"/>
+      <c r="AN81" s="244" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="82" spans="14:40" ht="30">
-      <c r="N82" s="215" t="s">
+      <c r="N82" s="214" t="s">
         <v>703</v>
       </c>
-      <c r="O82" s="240">
+      <c r="O82" s="234">
         <v>0.25</v>
       </c>
-      <c r="P82" s="274">
+      <c r="P82" s="375">
         <v>5.79E-2</v>
       </c>
-      <c r="Q82" s="241"/>
-      <c r="R82" s="242"/>
-      <c r="S82" s="274">
+      <c r="Q82" s="382"/>
+      <c r="R82" s="383"/>
+      <c r="S82" s="375">
         <v>2.1700000000000001E-3</v>
       </c>
-      <c r="T82" s="239">
+      <c r="T82" s="234">
         <v>0.34899999999999998</v>
       </c>
-      <c r="V82" s="242" t="s">
+      <c r="V82" s="235" t="s">
         <v>703</v>
       </c>
-      <c r="W82" s="248"/>
-      <c r="X82" s="279"/>
-      <c r="Y82" s="216">
+      <c r="W82" s="241"/>
+      <c r="X82" s="340"/>
+      <c r="Y82" s="388">
         <v>0.4</v>
       </c>
-      <c r="Z82" s="239">
+      <c r="Z82" s="234">
         <v>1</v>
       </c>
-      <c r="AA82" s="279"/>
-      <c r="AB82" s="367">
+      <c r="AA82" s="389"/>
+      <c r="AB82" s="392">
         <v>0.39300000000000002</v>
       </c>
-      <c r="AF82" s="242" t="s">
+      <c r="AF82" s="235" t="s">
         <v>703</v>
       </c>
-      <c r="AG82" s="239">
+      <c r="AG82" s="233">
         <v>0.251</v>
       </c>
-      <c r="AH82" s="274">
+      <c r="AH82" s="313">
         <v>5.79E-2</v>
       </c>
-      <c r="AI82" s="216">
+      <c r="AI82" s="395">
         <v>0.40400000000000003</v>
       </c>
-      <c r="AJ82" s="239">
+      <c r="AJ82" s="233">
         <v>1</v>
       </c>
-      <c r="AK82" s="274">
+      <c r="AK82" s="313">
         <v>2.1700000000000001E-3</v>
       </c>
-      <c r="AL82" s="239">
+      <c r="AL82" s="233">
         <v>0.39489999999999997</v>
       </c>
-      <c r="AN82" s="239">
+      <c r="AN82" s="233">
         <v>0.39489999999999997</v>
       </c>
     </row>
     <row r="83" spans="14:40" ht="16" thickBot="1">
-      <c r="N83" s="217"/>
-      <c r="O83" s="217"/>
-      <c r="P83" s="275"/>
-      <c r="Q83" s="243"/>
-      <c r="R83" s="244"/>
-      <c r="S83" s="277"/>
-      <c r="T83" s="217"/>
-      <c r="V83" s="244"/>
-      <c r="W83" s="244"/>
-      <c r="X83" s="280"/>
-      <c r="Y83" s="218"/>
-      <c r="Z83" s="217"/>
-      <c r="AA83" s="282"/>
-      <c r="AB83" s="217"/>
-      <c r="AF83" s="244"/>
-      <c r="AG83" s="217"/>
-      <c r="AH83" s="275"/>
-      <c r="AI83" s="218"/>
-      <c r="AJ83" s="217"/>
-      <c r="AK83" s="277"/>
-      <c r="AL83" s="217"/>
-      <c r="AN83" s="217"/>
+      <c r="N83" s="215"/>
+      <c r="O83" s="378"/>
+      <c r="P83" s="379"/>
+      <c r="Q83" s="238"/>
+      <c r="R83" s="384"/>
+      <c r="S83" s="379"/>
+      <c r="T83" s="378"/>
+      <c r="V83" s="237"/>
+      <c r="W83" s="237"/>
+      <c r="X83" s="341"/>
+      <c r="Y83" s="217"/>
+      <c r="Z83" s="378"/>
+      <c r="AA83" s="390"/>
+      <c r="AB83" s="378"/>
+      <c r="AF83" s="237"/>
+      <c r="AG83" s="215"/>
+      <c r="AH83" s="316"/>
+      <c r="AI83" s="396"/>
+      <c r="AJ83" s="215"/>
+      <c r="AK83" s="314"/>
+      <c r="AL83" s="215"/>
+      <c r="AN83" s="215"/>
     </row>
     <row r="84" spans="14:40" ht="46" thickBot="1">
-      <c r="N84" s="217" t="s">
+      <c r="N84" s="215" t="s">
         <v>704</v>
       </c>
-      <c r="O84" s="218">
+      <c r="O84" s="217">
         <v>0.46</v>
       </c>
-      <c r="P84" s="276"/>
-      <c r="Q84" s="243"/>
-      <c r="R84" s="245"/>
-      <c r="S84" s="278"/>
-      <c r="T84" s="218">
+      <c r="P84" s="381"/>
+      <c r="Q84" s="238"/>
+      <c r="R84" s="238"/>
+      <c r="S84" s="381"/>
+      <c r="T84" s="217">
         <v>0.371</v>
       </c>
-      <c r="V84" s="244" t="s">
+      <c r="V84" s="237" t="s">
         <v>704</v>
       </c>
-      <c r="W84" s="243"/>
-      <c r="X84" s="281"/>
-      <c r="Y84" s="218">
+      <c r="W84" s="236"/>
+      <c r="X84" s="342"/>
+      <c r="Y84" s="217">
         <v>0.60399999999999998</v>
       </c>
-      <c r="Z84" s="219">
+      <c r="Z84" s="217">
         <v>1</v>
       </c>
-      <c r="AA84" s="283"/>
-      <c r="AB84" s="218">
+      <c r="AA84" s="391"/>
+      <c r="AB84" s="217">
         <v>0.36199999999999999</v>
       </c>
-      <c r="AF84" s="244" t="s">
+      <c r="AF84" s="237" t="s">
         <v>704</v>
       </c>
-      <c r="AG84" s="218">
+      <c r="AG84" s="216">
         <v>0.46200000000000002</v>
       </c>
-      <c r="AH84" s="276"/>
-      <c r="AI84" s="218">
+      <c r="AH84" s="317"/>
+      <c r="AI84" s="216">
         <v>0.60399999999999998</v>
       </c>
-      <c r="AJ84" s="219">
+      <c r="AJ84" s="217">
         <v>1</v>
       </c>
-      <c r="AK84" s="278"/>
-      <c r="AL84" s="218">
+      <c r="AK84" s="315"/>
+      <c r="AL84" s="216">
         <v>0.36399999999999999</v>
       </c>
     </row>
     <row r="85" spans="14:40" ht="16" thickBot="1"/>
     <row r="86" spans="14:40" ht="46" thickBot="1">
-      <c r="V86" s="220" t="s">
+      <c r="V86" s="218" t="s">
         <v>716</v>
       </c>
       <c r="W86" s="209" t="s">
@@ -33789,51 +34309,51 @@
       </c>
     </row>
     <row r="88" spans="14:40" ht="30">
-      <c r="V88" s="242" t="s">
+      <c r="V88" s="235" t="s">
         <v>703</v>
       </c>
-      <c r="W88" s="248"/>
-      <c r="X88" s="279"/>
-      <c r="Y88" s="365">
+      <c r="W88" s="241"/>
+      <c r="X88" s="340"/>
+      <c r="Y88" s="393">
         <v>0.45879999999999999</v>
       </c>
-      <c r="Z88" s="239">
+      <c r="Z88" s="234">
         <v>0.92589999999999995</v>
       </c>
-      <c r="AA88" s="279"/>
-      <c r="AB88" s="239">
+      <c r="AA88" s="389"/>
+      <c r="AB88" s="234">
         <v>0.37569999999999998</v>
       </c>
     </row>
     <row r="89" spans="14:40" ht="16" thickBot="1">
-      <c r="V89" s="244"/>
-      <c r="W89" s="244"/>
-      <c r="X89" s="282"/>
-      <c r="Y89" s="366"/>
-      <c r="Z89" s="217"/>
-      <c r="AA89" s="282"/>
-      <c r="AB89" s="217"/>
+      <c r="V89" s="237"/>
+      <c r="W89" s="237"/>
+      <c r="X89" s="343"/>
+      <c r="Y89" s="394"/>
+      <c r="Z89" s="378"/>
+      <c r="AA89" s="390"/>
+      <c r="AB89" s="378"/>
     </row>
     <row r="90" spans="14:40" ht="46" thickBot="1">
-      <c r="V90" s="244" t="s">
+      <c r="V90" s="237" t="s">
         <v>704</v>
       </c>
-      <c r="W90" s="243"/>
-      <c r="X90" s="283"/>
-      <c r="Y90" s="218">
+      <c r="W90" s="236"/>
+      <c r="X90" s="344"/>
+      <c r="Y90" s="217">
         <v>0.69210000000000005</v>
       </c>
-      <c r="Z90" s="219">
+      <c r="Z90" s="217">
         <v>1</v>
       </c>
-      <c r="AA90" s="283"/>
-      <c r="AB90" s="218">
+      <c r="AA90" s="391"/>
+      <c r="AB90" s="217">
         <v>0.36890000000000001</v>
       </c>
     </row>
     <row r="91" spans="14:40" ht="16" thickBot="1"/>
     <row r="92" spans="14:40" ht="46" thickBot="1">
-      <c r="V92" s="220" t="s">
+      <c r="V92" s="218" t="s">
         <v>715</v>
       </c>
       <c r="W92" s="209" t="s">
@@ -33879,77 +34399,98 @@
       </c>
     </row>
     <row r="94" spans="14:40" ht="30">
-      <c r="V94" s="242" t="s">
+      <c r="V94" s="235" t="s">
         <v>703</v>
       </c>
-      <c r="W94" s="248"/>
-      <c r="X94" s="279"/>
-      <c r="Y94" s="365">
+      <c r="W94" s="241"/>
+      <c r="X94" s="340"/>
+      <c r="Y94" s="393">
         <v>0.40799999999999997</v>
       </c>
-      <c r="Z94" s="239">
+      <c r="Z94" s="234">
         <v>0.92589999999999995</v>
       </c>
-      <c r="AA94" s="279"/>
-      <c r="AB94" s="239">
+      <c r="AA94" s="389"/>
+      <c r="AB94" s="234">
         <v>0.37589</v>
       </c>
     </row>
     <row r="95" spans="14:40" ht="16" thickBot="1">
-      <c r="V95" s="244"/>
-      <c r="W95" s="244"/>
-      <c r="X95" s="282"/>
-      <c r="Y95" s="366"/>
-      <c r="Z95" s="217"/>
-      <c r="AA95" s="282"/>
-      <c r="AB95" s="217"/>
+      <c r="V95" s="237"/>
+      <c r="W95" s="237"/>
+      <c r="X95" s="343"/>
+      <c r="Y95" s="394"/>
+      <c r="Z95" s="378"/>
+      <c r="AA95" s="390"/>
+      <c r="AB95" s="378"/>
     </row>
     <row r="96" spans="14:40" ht="46" thickBot="1">
-      <c r="V96" s="244" t="s">
+      <c r="V96" s="237" t="s">
         <v>704</v>
       </c>
-      <c r="W96" s="243"/>
-      <c r="X96" s="283"/>
-      <c r="Y96" s="218">
+      <c r="W96" s="236"/>
+      <c r="X96" s="344"/>
+      <c r="Y96" s="217">
         <v>0.61660000000000004</v>
       </c>
-      <c r="Z96" s="219">
+      <c r="Z96" s="217">
         <v>1</v>
       </c>
-      <c r="AA96" s="283"/>
-      <c r="AB96" s="218">
+      <c r="AA96" s="391"/>
+      <c r="AB96" s="217">
         <v>0.37</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="108">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="T6:V17"/>
-    <mergeCell ref="T3:V4"/>
-    <mergeCell ref="AA3:AB4"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="H3:I4"/>
-    <mergeCell ref="K3:L4"/>
-    <mergeCell ref="N3:O4"/>
-    <mergeCell ref="Q3:R4"/>
-    <mergeCell ref="X3:Y4"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="E3:F4"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="T21:V22"/>
-    <mergeCell ref="Q21:R22"/>
-    <mergeCell ref="K21:L22"/>
-    <mergeCell ref="E21:F22"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B21:C22"/>
-    <mergeCell ref="H21:I22"/>
-    <mergeCell ref="N21:O22"/>
+  <mergeCells count="107">
+    <mergeCell ref="AL69:AL70"/>
+    <mergeCell ref="AE61:AG62"/>
+    <mergeCell ref="AJ65:AJ66"/>
+    <mergeCell ref="AH67:AH68"/>
+    <mergeCell ref="AL67:AL68"/>
+    <mergeCell ref="AE67:AE68"/>
+    <mergeCell ref="AH76:AH78"/>
+    <mergeCell ref="AK76:AK78"/>
+    <mergeCell ref="AO61:AQ62"/>
+    <mergeCell ref="AH82:AH84"/>
+    <mergeCell ref="AK82:AK84"/>
+    <mergeCell ref="X82:X84"/>
+    <mergeCell ref="AA82:AA84"/>
+    <mergeCell ref="X88:X90"/>
+    <mergeCell ref="AA88:AA90"/>
+    <mergeCell ref="X94:X96"/>
+    <mergeCell ref="AA94:AA96"/>
+    <mergeCell ref="X70:X72"/>
+    <mergeCell ref="AA70:AA72"/>
+    <mergeCell ref="AF72:AH73"/>
+    <mergeCell ref="AE69:AE70"/>
+    <mergeCell ref="AH69:AH70"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="H24:I24"/>
+    <mergeCell ref="V61:X62"/>
+    <mergeCell ref="X76:X78"/>
+    <mergeCell ref="AA76:AA78"/>
+    <mergeCell ref="Q6:R17"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="P70:P72"/>
+    <mergeCell ref="S70:S72"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="N61:P62"/>
+    <mergeCell ref="S76:S78"/>
+    <mergeCell ref="P82:P84"/>
+    <mergeCell ref="S82:S84"/>
+    <mergeCell ref="P76:P78"/>
+    <mergeCell ref="Q49:AA55"/>
+    <mergeCell ref="O26:Q37"/>
+    <mergeCell ref="X65:X66"/>
+    <mergeCell ref="AA65:AA66"/>
+    <mergeCell ref="W41:X43"/>
+    <mergeCell ref="Q41:R42"/>
+    <mergeCell ref="N41:O43"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="E36:F38"/>
     <mergeCell ref="H36:I38"/>
@@ -33971,19 +34512,22 @@
     <mergeCell ref="E41:F42"/>
     <mergeCell ref="H41:I42"/>
     <mergeCell ref="B62:C63"/>
-    <mergeCell ref="E6:F18"/>
-    <mergeCell ref="S76:S78"/>
-    <mergeCell ref="P82:P84"/>
-    <mergeCell ref="S82:S84"/>
-    <mergeCell ref="P76:P78"/>
-    <mergeCell ref="Q49:AA55"/>
-    <mergeCell ref="O26:Q37"/>
-    <mergeCell ref="X65:X66"/>
-    <mergeCell ref="AA65:AA66"/>
-    <mergeCell ref="W41:X43"/>
-    <mergeCell ref="Q41:R42"/>
-    <mergeCell ref="N41:O43"/>
     <mergeCell ref="E46:F46"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="T21:V22"/>
+    <mergeCell ref="Q21:R22"/>
+    <mergeCell ref="K21:L22"/>
+    <mergeCell ref="E21:F22"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="H21:I22"/>
+    <mergeCell ref="N21:O22"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="K24:L24"/>
@@ -33993,47 +34537,23 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="V61:X62"/>
-    <mergeCell ref="X76:X78"/>
-    <mergeCell ref="AA76:AA78"/>
-    <mergeCell ref="Q6:R17"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="P70:P72"/>
-    <mergeCell ref="S70:S72"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="N61:P62"/>
-    <mergeCell ref="P65:P66"/>
-    <mergeCell ref="S65:S66"/>
-    <mergeCell ref="AH82:AH84"/>
-    <mergeCell ref="AK82:AK84"/>
-    <mergeCell ref="X82:X84"/>
-    <mergeCell ref="AA82:AA84"/>
-    <mergeCell ref="X88:X90"/>
-    <mergeCell ref="AA88:AA90"/>
-    <mergeCell ref="X94:X96"/>
-    <mergeCell ref="AA94:AA96"/>
-    <mergeCell ref="X70:X72"/>
-    <mergeCell ref="AA70:AA72"/>
-    <mergeCell ref="AF72:AH73"/>
-    <mergeCell ref="AE69:AE70"/>
-    <mergeCell ref="AH69:AH70"/>
-    <mergeCell ref="AL69:AL70"/>
-    <mergeCell ref="AE61:AG62"/>
-    <mergeCell ref="AJ65:AJ66"/>
-    <mergeCell ref="AH67:AH68"/>
-    <mergeCell ref="AL67:AL68"/>
-    <mergeCell ref="AE67:AE68"/>
-    <mergeCell ref="AH76:AH78"/>
-    <mergeCell ref="AK76:AK78"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="T6:V17"/>
+    <mergeCell ref="T3:V4"/>
+    <mergeCell ref="AA3:AB4"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="H3:I4"/>
+    <mergeCell ref="K3:L4"/>
+    <mergeCell ref="N3:O4"/>
+    <mergeCell ref="Q3:R4"/>
+    <mergeCell ref="X3:Y4"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="E3:F4"/>
+    <mergeCell ref="E6:F18"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -34274,10 +34794,10 @@
       <c r="E1" s="51"/>
       <c r="F1" s="87"/>
       <c r="I1" s="76"/>
-      <c r="J1" s="363" t="s">
+      <c r="J1" s="356" t="s">
         <v>410</v>
       </c>
-      <c r="K1" s="363"/>
+      <c r="K1" s="356"/>
     </row>
     <row r="2" spans="2:14" ht="28">
       <c r="B2" s="51" t="s">

</xml_diff>